<commit_message>
fix: product size + filegroups update
</commit_message>
<xml_diff>
--- a/filegroup_support/Filegroups_support.xlsx
+++ b/filegroup_support/Filegroups_support.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\wwi\filegroup_support\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B296AB84-4220-4BDD-8B21-6856CAFC5C37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C78B429-EF9F-4573-91F0-158CAB642619}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{060E0144-75C7-4C12-B4D9-C7F9369402C2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{060E0144-75C7-4C12-B4D9-C7F9369402C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="166">
   <si>
     <t>Data types</t>
   </si>
@@ -473,9 +473,6 @@
     <t>FK (Logistic PK)</t>
   </si>
   <si>
-    <t>Logs</t>
-  </si>
-  <si>
     <t>Error</t>
   </si>
   <si>
@@ -540,6 +537,12 @@
   </si>
   <si>
     <t>varchar - Could be a char(3)</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Monitoring</t>
   </si>
 </sst>
 </file>
@@ -751,7 +754,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -770,25 +773,24 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1106,10 +1108,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61C2F128-56C4-4A17-AFB6-7B93C606ECA2}">
-  <dimension ref="A1:Y71"/>
+  <dimension ref="A1:AA71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F37" workbookViewId="0">
-      <selection activeCell="R24" sqref="R24"/>
+    <sheetView tabSelected="1" topLeftCell="B46" workbookViewId="0">
+      <selection activeCell="E56" sqref="E56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1122,22 +1124,24 @@
     <col min="8" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.28515625" customWidth="1"/>
     <col min="10" max="10" width="12.85546875" customWidth="1"/>
-    <col min="11" max="12" width="4" customWidth="1"/>
-    <col min="13" max="13" width="17.85546875" customWidth="1"/>
-    <col min="14" max="14" width="23.7109375" customWidth="1"/>
-    <col min="15" max="15" width="12.85546875" customWidth="1"/>
-    <col min="16" max="16" width="17" customWidth="1"/>
-    <col min="17" max="17" width="10.7109375" customWidth="1"/>
-    <col min="18" max="18" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="18.140625" customWidth="1"/>
-    <col min="24" max="24" width="10.5703125" customWidth="1"/>
-    <col min="25" max="25" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.85546875" customWidth="1"/>
+    <col min="12" max="13" width="4" customWidth="1"/>
+    <col min="14" max="14" width="19.7109375" customWidth="1"/>
+    <col min="15" max="15" width="23.7109375" customWidth="1"/>
+    <col min="16" max="16" width="12.85546875" customWidth="1"/>
+    <col min="17" max="17" width="17" customWidth="1"/>
+    <col min="18" max="18" width="10.7109375" customWidth="1"/>
+    <col min="19" max="19" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.140625" customWidth="1"/>
+    <col min="22" max="22" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="18.140625" customWidth="1"/>
+    <col min="26" max="26" width="10.5703125" customWidth="1"/>
+    <col min="27" max="27" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1162,44 +1166,46 @@
       <c r="J1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="K1" s="29"/>
+      <c r="N1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="N1" s="12" t="s">
+      <c r="O1" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="O1" s="12" t="s">
+      <c r="P1" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="P1" s="12" t="s">
+      <c r="Q1" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="Q1" s="12" t="s">
+      <c r="R1" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="T1" s="29"/>
+      <c r="V1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="U1" s="12" t="s">
+      <c r="W1" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="V1" s="12" t="s">
+      <c r="X1" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="W1" s="12" t="s">
+      <c r="Y1" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="X1" s="12" t="s">
+      <c r="Z1" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -1215,36 +1221,38 @@
       <c r="I2" s="10">
         <v>19</v>
       </c>
-      <c r="J2" s="30">
+      <c r="J2" s="23">
         <f>SUM(J3:J7)</f>
         <v>418</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="N2" s="10"/>
       <c r="O2" s="10"/>
       <c r="P2" s="10"/>
-      <c r="Q2" s="10">
+      <c r="Q2" s="10"/>
+      <c r="R2" s="10">
         <v>5</v>
       </c>
-      <c r="R2" s="30">
-        <f>SUM(R3:R4)</f>
+      <c r="S2" s="23">
+        <f>SUM(S3:S4)</f>
         <v>70</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="V2" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="U2" s="10"/>
-      <c r="V2" s="10"/>
       <c r="W2" s="10"/>
       <c r="X2" s="10"/>
-      <c r="Y2" s="3">
-        <f>SUM(Y3:Y7)</f>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y2" s="10"/>
+      <c r="Z2" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="AA2" s="3">
+        <f>SUM(AA3:AA7)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -1268,40 +1276,45 @@
         <f>PRODUCT(I3,H3)</f>
         <v>76</v>
       </c>
-      <c r="L3" s="1"/>
-      <c r="M3" s="4"/>
-      <c r="N3" t="s">
+      <c r="K3" s="27"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="4"/>
+      <c r="O3" t="s">
         <v>21</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>5</v>
       </c>
-      <c r="P3">
-        <v>4</v>
-      </c>
       <c r="Q3">
+        <v>4</v>
+      </c>
+      <c r="R3">
         <v>5</v>
       </c>
-      <c r="R3" s="5">
-        <f>PRODUCT(P3,Q3)</f>
+      <c r="S3" s="5">
+        <f>PRODUCT(Q3,R3)</f>
         <v>20</v>
       </c>
-      <c r="T3" s="4"/>
-      <c r="U3" t="s">
+      <c r="T3" s="27"/>
+      <c r="V3" s="4"/>
+      <c r="W3" t="s">
         <v>21</v>
       </c>
-      <c r="V3" t="s">
+      <c r="X3" t="s">
         <v>25</v>
       </c>
-      <c r="W3">
-        <v>4</v>
-      </c>
-      <c r="Y3" s="5">
-        <f>PRODUCT(X3,W3)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y3">
+        <v>4</v>
+      </c>
+      <c r="Z3">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="5">
+        <f>PRODUCT(Z3,Y3)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
@@ -1326,40 +1339,45 @@
         <f>PRODUCT(I4,H4)</f>
         <v>133</v>
       </c>
-      <c r="M4" s="4"/>
-      <c r="N4" t="s">
+      <c r="K4" s="27"/>
+      <c r="N4" s="4"/>
+      <c r="O4" t="s">
         <v>17</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>26</v>
       </c>
-      <c r="P4">
+      <c r="Q4">
         <f>(12+16+9+8+5)/5</f>
         <v>10</v>
       </c>
-      <c r="Q4">
+      <c r="R4">
         <v>5</v>
       </c>
-      <c r="R4" s="5">
-        <f>PRODUCT(P4,Q4)</f>
+      <c r="S4" s="5">
+        <f>PRODUCT(Q4,R4)</f>
         <v>50</v>
       </c>
-      <c r="T4" s="4"/>
-      <c r="U4" t="s">
+      <c r="T4" s="27"/>
+      <c r="V4" s="4"/>
+      <c r="W4" t="s">
         <v>89</v>
       </c>
-      <c r="V4" t="s">
+      <c r="X4" t="s">
         <v>11</v>
       </c>
-      <c r="W4">
+      <c r="Y4">
         <v>3</v>
       </c>
-      <c r="Y4" s="5">
-        <f>PRODUCT(X4,W4)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z4">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="5">
+        <f>PRODUCT(Z4,Y4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
@@ -1384,28 +1402,33 @@
         <f>PRODUCT(I5,H5)</f>
         <v>152</v>
       </c>
-      <c r="M5" s="6"/>
-      <c r="N5" s="17"/>
-      <c r="O5" s="17"/>
-      <c r="P5" s="17"/>
-      <c r="Q5" s="17"/>
-      <c r="R5" s="7"/>
-      <c r="T5" s="4"/>
-      <c r="U5" t="s">
+      <c r="K5" s="27"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="16"/>
+      <c r="P5" s="16"/>
+      <c r="Q5" s="16"/>
+      <c r="R5" s="16"/>
+      <c r="S5" s="7"/>
+      <c r="T5" s="27"/>
+      <c r="V5" s="4"/>
+      <c r="W5" t="s">
         <v>90</v>
       </c>
-      <c r="V5" t="s">
+      <c r="X5" t="s">
         <v>11</v>
       </c>
-      <c r="W5">
+      <c r="Y5">
         <v>3</v>
       </c>
-      <c r="Y5" s="5">
-        <f>PRODUCT(X5,W5)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z5">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="5">
+        <f>PRODUCT(Z5,Y5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
@@ -1429,35 +1452,39 @@
         <f>PRODUCT(I6,H6)</f>
         <v>19</v>
       </c>
-      <c r="M6" s="2" t="s">
+      <c r="K6" s="27"/>
+      <c r="N6" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="N6" s="10"/>
       <c r="O6" s="10"/>
       <c r="P6" s="10"/>
-      <c r="Q6">
+      <c r="Q6" s="10"/>
+      <c r="R6">
         <v>2</v>
       </c>
-      <c r="R6" s="29">
-        <f>SUM(R7:R8)</f>
+      <c r="S6" s="22">
+        <f>SUM(S7:S8)</f>
         <v>36</v>
       </c>
-      <c r="T6" s="4"/>
-      <c r="U6" t="s">
+      <c r="V6" s="4"/>
+      <c r="W6" t="s">
         <v>91</v>
       </c>
-      <c r="V6" t="s">
+      <c r="X6" t="s">
         <v>25</v>
       </c>
-      <c r="W6">
-        <v>4</v>
-      </c>
-      <c r="Y6" s="5">
-        <f>PRODUCT(X6,W6)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y6">
+        <v>4</v>
+      </c>
+      <c r="Z6">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="5">
+        <f>PRODUCT(Z6,Y6)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
@@ -1481,30 +1508,32 @@
         <f>PRODUCT(I7,H7)</f>
         <v>38</v>
       </c>
-      <c r="M7" s="4"/>
-      <c r="N7" t="s">
+      <c r="K7" s="27"/>
+      <c r="N7" s="4"/>
+      <c r="O7" t="s">
         <v>21</v>
       </c>
-      <c r="O7" t="s">
+      <c r="P7" t="s">
         <v>58</v>
       </c>
-      <c r="P7">
-        <v>4</v>
-      </c>
       <c r="Q7">
+        <v>4</v>
+      </c>
+      <c r="R7">
         <v>2</v>
       </c>
-      <c r="R7" s="5">
-        <f>PRODUCT(Q7,P7)</f>
+      <c r="S7" s="5">
+        <f>PRODUCT(R7,Q7)</f>
         <v>8</v>
       </c>
-      <c r="T7" s="4"/>
-      <c r="Y7" s="7">
-        <f>PRODUCT(X7,W7)</f>
+      <c r="T7" s="27"/>
+      <c r="V7" s="4"/>
+      <c r="AA7" s="7">
+        <f>PRODUCT(Z7,Y7)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
@@ -1521,37 +1550,41 @@
         <v>10</v>
       </c>
       <c r="J8" s="3"/>
-      <c r="M8" s="4"/>
-      <c r="N8" t="s">
+      <c r="K8" s="29"/>
+      <c r="N8" s="4"/>
+      <c r="O8" t="s">
         <v>17</v>
       </c>
-      <c r="O8" t="s">
+      <c r="P8" t="s">
         <v>26</v>
       </c>
-      <c r="P8">
+      <c r="Q8">
         <f>12+2</f>
         <v>14</v>
       </c>
-      <c r="Q8">
+      <c r="R8">
         <v>2</v>
       </c>
-      <c r="R8" s="5">
-        <f>PRODUCT(Q8,P8)</f>
+      <c r="S8" s="5">
+        <f>PRODUCT(R8,Q8)</f>
         <v>28</v>
       </c>
-      <c r="T8" s="2" t="s">
+      <c r="T8" s="27"/>
+      <c r="V8" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="U8" s="10"/>
-      <c r="V8" s="10"/>
       <c r="W8" s="10"/>
       <c r="X8" s="10"/>
-      <c r="Y8" s="15">
-        <f>SUM(Y9:Y15)</f>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y8" s="10"/>
+      <c r="Z8" s="10">
+        <v>402</v>
+      </c>
+      <c r="AA8" s="22">
+        <f>SUM(AA9:AA15)</f>
+        <v>7638</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>10</v>
       </c>
@@ -1575,29 +1608,33 @@
         <f>PRODUCT(I9,H9)</f>
         <v>40</v>
       </c>
-      <c r="M9" s="6"/>
-      <c r="N9" s="17"/>
-      <c r="O9" s="17"/>
-      <c r="P9" s="17"/>
-      <c r="Q9" s="17"/>
-      <c r="R9" s="7"/>
-      <c r="T9" s="4"/>
-      <c r="U9" s="18" t="s">
+      <c r="K9" s="27"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="16"/>
+      <c r="P9" s="16"/>
+      <c r="Q9" s="16"/>
+      <c r="R9" s="16"/>
+      <c r="S9" s="7"/>
+      <c r="T9" s="27"/>
+      <c r="V9" s="4"/>
+      <c r="W9" t="s">
         <v>21</v>
       </c>
-      <c r="V9" s="18" t="s">
+      <c r="X9" t="s">
         <v>58</v>
       </c>
-      <c r="W9" s="21">
-        <v>4</v>
-      </c>
-      <c r="X9" s="18"/>
-      <c r="Y9" s="5">
-        <f>PRODUCT(W9,X9)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y9">
+        <v>4</v>
+      </c>
+      <c r="Z9" s="28">
+        <v>402</v>
+      </c>
+      <c r="AA9" s="5">
+        <f>PRODUCT(Y9,Z9)</f>
+        <v>1608</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>11</v>
       </c>
@@ -1621,31 +1658,33 @@
         <f>PRODUCT(I10,H10)</f>
         <v>10</v>
       </c>
-      <c r="M10" s="13" t="s">
+      <c r="K10" s="27"/>
+      <c r="N10" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="Q10">
+      <c r="R10">
         <v>3</v>
       </c>
-      <c r="R10" s="29">
-        <f>SUM(R11:R12)</f>
+      <c r="S10" s="22">
+        <f>SUM(S11:S12)</f>
         <v>18</v>
       </c>
-      <c r="T10" s="4"/>
-      <c r="U10" s="18" t="s">
+      <c r="V10" s="4"/>
+      <c r="W10" t="s">
         <v>17</v>
       </c>
-      <c r="V10" s="18" t="s">
+      <c r="X10" t="s">
         <v>26</v>
       </c>
-      <c r="W10" s="18"/>
-      <c r="X10" s="18"/>
-      <c r="Y10" s="5">
-        <f>PRODUCT(W10,X10)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z10" s="28">
+        <v>402</v>
+      </c>
+      <c r="AA10" s="5">
+        <f>PRODUCT(Y10,Z10)</f>
+        <v>402</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>12</v>
       </c>
@@ -1666,38 +1705,41 @@
         <f>PRODUCT(I11,H11)</f>
         <v>90</v>
       </c>
-      <c r="M11" s="4"/>
-      <c r="N11" t="s">
+      <c r="K11" s="27"/>
+      <c r="N11" s="4"/>
+      <c r="O11" t="s">
         <v>21</v>
       </c>
-      <c r="O11" t="s">
+      <c r="P11" t="s">
         <v>7</v>
       </c>
-      <c r="P11">
+      <c r="Q11">
         <v>1</v>
       </c>
-      <c r="Q11">
+      <c r="R11">
         <v>3</v>
       </c>
-      <c r="R11" s="5">
-        <f>PRODUCT(Q11,P11)</f>
+      <c r="S11" s="5">
+        <f>PRODUCT(R11,Q11)</f>
         <v>3</v>
       </c>
-      <c r="T11" s="4"/>
-      <c r="U11" s="18" t="s">
+      <c r="T11" s="27"/>
+      <c r="V11" s="4"/>
+      <c r="W11" t="s">
         <v>103</v>
       </c>
-      <c r="V11" s="18" t="s">
+      <c r="X11" t="s">
         <v>26</v>
       </c>
-      <c r="W11" s="18"/>
-      <c r="X11" s="18"/>
-      <c r="Y11" s="5">
-        <f>PRODUCT(W11,X11)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z11" s="28">
+        <v>402</v>
+      </c>
+      <c r="AA11" s="5">
+        <f>PRODUCT(Y11,Z11)</f>
+        <v>402</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>14</v>
       </c>
@@ -1705,45 +1747,48 @@
         <v>4</v>
       </c>
       <c r="E12" s="4"/>
-      <c r="J12" s="29">
+      <c r="J12" s="22">
         <f>SUM(J9:J11)</f>
         <v>140</v>
       </c>
-      <c r="M12" s="4"/>
-      <c r="N12" s="18" t="s">
+      <c r="N12" s="4"/>
+      <c r="O12" t="s">
         <v>17</v>
       </c>
-      <c r="O12" s="32" t="s">
-        <v>164</v>
-      </c>
-      <c r="P12" s="18">
+      <c r="P12" s="25" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q12">
         <f>3+2</f>
         <v>5</v>
       </c>
-      <c r="Q12">
+      <c r="R12">
         <v>3</v>
       </c>
-      <c r="R12" s="5">
-        <f>PRODUCT(Q12,P12)</f>
+      <c r="S12" s="5">
+        <f>PRODUCT(R12,Q12)</f>
         <v>15</v>
       </c>
-      <c r="T12" s="4"/>
-      <c r="U12" s="18" t="s">
+      <c r="T12" s="27"/>
+      <c r="V12" s="4"/>
+      <c r="W12" t="s">
         <v>104</v>
       </c>
-      <c r="V12" s="18" t="s">
+      <c r="X12" t="s">
         <v>10</v>
       </c>
-      <c r="W12" s="18">
+      <c r="Y12">
         <v>1</v>
       </c>
-      <c r="X12" s="18"/>
-      <c r="Y12" s="5">
-        <f>PRODUCT(W12,X12)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z12" s="28">
+        <v>402</v>
+      </c>
+      <c r="AA12" s="5">
+        <f>PRODUCT(Y12,Z12)</f>
+        <v>402</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>13</v>
       </c>
@@ -1759,37 +1804,40 @@
       <c r="I13" s="10">
         <v>9</v>
       </c>
-      <c r="J13" s="30">
+      <c r="J13" s="23">
         <f xml:space="preserve"> SUM(J14:J15)</f>
         <v>135</v>
       </c>
-      <c r="M13" s="19"/>
       <c r="N13" s="17"/>
-      <c r="O13" s="17"/>
-      <c r="P13" s="17"/>
-      <c r="Q13" s="17"/>
-      <c r="R13" s="20"/>
-      <c r="T13" s="4"/>
-      <c r="U13" s="18" t="s">
+      <c r="O13" s="16"/>
+      <c r="P13" s="16"/>
+      <c r="Q13" s="16"/>
+      <c r="R13" s="16"/>
+      <c r="S13" s="18"/>
+      <c r="T13" s="29"/>
+      <c r="V13" s="4"/>
+      <c r="W13" t="s">
         <v>105</v>
       </c>
-      <c r="V13" s="18" t="s">
+      <c r="X13" t="s">
         <v>58</v>
       </c>
-      <c r="W13" s="18">
-        <v>4</v>
-      </c>
-      <c r="X13" s="18"/>
-      <c r="Y13" s="5">
-        <f>PRODUCT(W13,X13)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A14" s="25" t="s">
-        <v>163</v>
-      </c>
-      <c r="B14" s="26">
+      <c r="Y13">
+        <v>4</v>
+      </c>
+      <c r="Z13" s="28">
+        <v>402</v>
+      </c>
+      <c r="AA13" s="5">
+        <f>PRODUCT(Y13,Z13)</f>
+        <v>1608</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="B14" s="5">
         <v>4</v>
       </c>
       <c r="E14" s="4"/>
@@ -1809,40 +1857,43 @@
         <f>PRODUCT(I13,H14)</f>
         <v>36</v>
       </c>
-      <c r="M14" s="2" t="s">
+      <c r="K14" s="27"/>
+      <c r="N14" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="N14" s="10"/>
       <c r="O14" s="10"/>
       <c r="P14" s="10"/>
-      <c r="Q14">
+      <c r="Q14" s="10"/>
+      <c r="R14">
         <v>2</v>
       </c>
-      <c r="R14" s="30">
-        <f>SUM(R15:R16)</f>
+      <c r="S14" s="23">
+        <f>SUM(S15:S16)</f>
         <v>16</v>
       </c>
-      <c r="T14" s="4"/>
-      <c r="U14" s="18" t="s">
+      <c r="V14" s="4"/>
+      <c r="W14" t="s">
         <v>106</v>
       </c>
-      <c r="V14" s="18" t="s">
+      <c r="X14" t="s">
         <v>58</v>
       </c>
-      <c r="W14" s="18">
-        <v>4</v>
-      </c>
-      <c r="X14" s="18"/>
-      <c r="Y14" s="5">
-        <f t="shared" ref="Y14:Y15" si="0">PRODUCT(W14,X14)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A15" s="27" t="s">
-        <v>161</v>
-      </c>
-      <c r="B15" s="28">
+      <c r="Y14">
+        <v>4</v>
+      </c>
+      <c r="Z14" s="28">
+        <v>402</v>
+      </c>
+      <c r="AA14" s="5">
+        <f t="shared" ref="AA14:AA15" si="0">PRODUCT(Y14,Z14)</f>
+        <v>1608</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="B15" s="7">
         <v>8</v>
       </c>
       <c r="E15" s="4"/>
@@ -1863,67 +1914,73 @@
         <f>PRODUCT(I15,H15)</f>
         <v>99</v>
       </c>
-      <c r="M15" s="4"/>
-      <c r="N15" s="18" t="s">
+      <c r="K15" s="27"/>
+      <c r="N15" s="4"/>
+      <c r="O15" t="s">
         <v>21</v>
       </c>
-      <c r="O15" s="18" t="s">
+      <c r="P15" t="s">
         <v>61</v>
       </c>
-      <c r="P15" s="18">
+      <c r="Q15">
         <v>3</v>
       </c>
-      <c r="Q15">
+      <c r="R15">
         <v>2</v>
       </c>
-      <c r="R15" s="5">
-        <f>PRODUCT(P15,Q15)</f>
+      <c r="S15" s="5">
+        <f>PRODUCT(Q15,R15)</f>
         <v>6</v>
       </c>
-      <c r="T15" s="4"/>
-      <c r="U15" s="18" t="s">
+      <c r="T15" s="27"/>
+      <c r="V15" s="4"/>
+      <c r="W15" t="s">
         <v>107</v>
       </c>
-      <c r="V15" s="18" t="s">
+      <c r="X15" t="s">
         <v>58</v>
       </c>
-      <c r="W15" s="18">
-        <v>4</v>
-      </c>
-      <c r="X15" s="18"/>
-      <c r="Y15" s="5">
+      <c r="Y15">
+        <v>4</v>
+      </c>
+      <c r="Z15" s="28">
+        <v>402</v>
+      </c>
+      <c r="AA15" s="5">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+        <v>1608</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="E16" s="4"/>
       <c r="J16" s="5"/>
-      <c r="M16" s="4"/>
-      <c r="N16" s="21" t="s">
+      <c r="K16" s="27"/>
+      <c r="N16" s="4"/>
+      <c r="O16" t="s">
         <v>17</v>
       </c>
-      <c r="O16" s="21" t="s">
+      <c r="P16" t="s">
         <v>26</v>
       </c>
-      <c r="P16" s="18">
+      <c r="Q16">
         <v>5</v>
       </c>
-      <c r="Q16">
+      <c r="R16">
         <v>2</v>
       </c>
-      <c r="R16" s="5">
-        <f>PRODUCT(P16,Q16)</f>
+      <c r="S16" s="5">
+        <f>PRODUCT(Q16,R16)</f>
         <v>10</v>
       </c>
-      <c r="T16" s="6"/>
-      <c r="U16" s="17"/>
-      <c r="V16" s="17"/>
-      <c r="W16" s="17"/>
-      <c r="X16" s="17"/>
-      <c r="Y16" s="7"/>
-    </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="T16" s="27"/>
+      <c r="V16" s="6"/>
+      <c r="W16" s="16"/>
+      <c r="X16" s="16"/>
+      <c r="Y16" s="16"/>
+      <c r="Z16" s="16"/>
+      <c r="AA16" s="7"/>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>46</v>
       </c>
@@ -1936,29 +1993,32 @@
       <c r="I17" s="10">
         <v>23272</v>
       </c>
-      <c r="J17" s="30">
+      <c r="J17" s="23">
         <f>SUM(J18:J19)</f>
         <v>349080</v>
       </c>
-      <c r="M17" s="6"/>
-      <c r="N17" s="17"/>
-      <c r="O17" s="17"/>
-      <c r="P17" s="17"/>
-      <c r="Q17" s="17"/>
-      <c r="R17" s="7"/>
-      <c r="T17" s="2" t="s">
+      <c r="N17" s="6"/>
+      <c r="O17" s="16"/>
+      <c r="P17" s="16"/>
+      <c r="Q17" s="16"/>
+      <c r="R17" s="16"/>
+      <c r="S17" s="7"/>
+      <c r="T17" s="27"/>
+      <c r="V17" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="U17" s="10"/>
-      <c r="V17" s="10"/>
       <c r="W17" s="10"/>
       <c r="X17" s="10"/>
-      <c r="Y17" s="15">
-        <f>SUM(Y18:Y20)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Y17" s="10"/>
+      <c r="Z17" s="10">
+        <v>402</v>
+      </c>
+      <c r="AA17" s="22">
+        <f>SUM(AA18:AA20)</f>
+        <v>17286</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>27</v>
       </c>
@@ -1979,35 +2039,36 @@
         <f>(H18*I18)</f>
         <v>93088</v>
       </c>
-      <c r="M18" s="13" t="s">
+      <c r="K18" s="27"/>
+      <c r="N18" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="N18" s="18"/>
-      <c r="O18" s="18"/>
-      <c r="P18" s="18"/>
-      <c r="Q18">
+      <c r="R18">
         <v>2</v>
       </c>
-      <c r="R18" s="29">
-        <f>SUM(R19:R22)</f>
+      <c r="S18" s="22">
+        <f>SUM(S19:S22)</f>
         <v>38</v>
       </c>
-      <c r="T18" s="4"/>
-      <c r="U18" s="21" t="s">
+      <c r="V18" s="4"/>
+      <c r="W18" t="s">
         <v>109</v>
       </c>
-      <c r="V18" s="21" t="s">
+      <c r="X18" t="s">
         <v>58</v>
       </c>
-      <c r="W18" s="21">
-        <v>4</v>
-      </c>
-      <c r="Y18" s="5">
-        <f>PRODUCT(W18,X18)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y18">
+        <v>4</v>
+      </c>
+      <c r="Z18" s="28">
+        <v>402</v>
+      </c>
+      <c r="AA18" s="5">
+        <f>PRODUCT(Y18,Z18)</f>
+        <v>1608</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>35</v>
       </c>
@@ -2032,36 +2093,44 @@
         <f>(H19*I19)</f>
         <v>255992</v>
       </c>
-      <c r="M19" s="4"/>
-      <c r="N19" s="18" t="s">
+      <c r="K19" s="27"/>
+      <c r="N19" s="4"/>
+      <c r="O19" t="s">
         <v>63</v>
       </c>
-      <c r="O19" s="18" t="s">
+      <c r="P19" t="s">
         <v>61</v>
       </c>
-      <c r="P19" s="18">
+      <c r="Q19">
         <v>3</v>
       </c>
-      <c r="Q19">
+      <c r="R19">
         <v>2</v>
       </c>
-      <c r="R19" s="5">
-        <f>PRODUCT(P19*Q19)</f>
+      <c r="S19" s="5">
+        <f>PRODUCT(Q19*R19)</f>
         <v>6</v>
       </c>
-      <c r="T19" s="4"/>
-      <c r="U19" s="21" t="s">
+      <c r="T19" s="27"/>
+      <c r="V19" s="4"/>
+      <c r="W19" t="s">
         <v>110</v>
       </c>
-      <c r="V19" t="s">
+      <c r="X19" t="s">
         <v>26</v>
       </c>
-      <c r="Y19" s="5">
-        <f>PRODUCT(W19,X19)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y19">
+        <v>22</v>
+      </c>
+      <c r="Z19" s="28">
+        <v>402</v>
+      </c>
+      <c r="AA19" s="5">
+        <f>PRODUCT(Y19,Z19)</f>
+        <v>8844</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
         <v>31</v>
       </c>
@@ -2070,33 +2139,44 @@
       </c>
       <c r="E20" s="4"/>
       <c r="J20" s="5"/>
-      <c r="M20" s="4"/>
-      <c r="N20" s="21" t="s">
+      <c r="K20" s="27"/>
+      <c r="N20" s="4"/>
+      <c r="O20" t="s">
         <v>64</v>
       </c>
-      <c r="O20" s="21" t="s">
+      <c r="P20" t="s">
         <v>61</v>
       </c>
-      <c r="P20" s="18">
+      <c r="Q20">
         <v>3</v>
       </c>
-      <c r="Q20">
+      <c r="R20">
         <v>2</v>
       </c>
-      <c r="R20" s="5">
-        <f>PRODUCT(P20*Q20)</f>
+      <c r="S20" s="5">
+        <f>PRODUCT(Q20*R20)</f>
         <v>6</v>
       </c>
-      <c r="T20" s="4"/>
-      <c r="U20" s="21" t="s">
+      <c r="T20" s="27"/>
+      <c r="V20" s="4"/>
+      <c r="W20" t="s">
         <v>111</v>
       </c>
-      <c r="V20" t="s">
+      <c r="X20" t="s">
         <v>26</v>
       </c>
-      <c r="Y20" s="5"/>
-    </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y20">
+        <v>17</v>
+      </c>
+      <c r="Z20" s="28">
+        <v>402</v>
+      </c>
+      <c r="AA20" s="5">
+        <f>PRODUCT(Y20,Z20)</f>
+        <v>6834</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>32</v>
       </c>
@@ -2112,35 +2192,36 @@
       <c r="I21" s="10">
         <v>1</v>
       </c>
-      <c r="J21" s="30">
+      <c r="J21" s="23">
         <f>SUM(J22:J23)</f>
         <v>16</v>
       </c>
-      <c r="M21" s="4"/>
-      <c r="N21" s="21" t="s">
+      <c r="N21" s="4"/>
+      <c r="O21" t="s">
         <v>65</v>
       </c>
-      <c r="O21" s="21" t="s">
+      <c r="P21" t="s">
         <v>67</v>
       </c>
-      <c r="P21" s="18">
+      <c r="Q21">
         <v>5</v>
       </c>
-      <c r="Q21">
+      <c r="R21">
         <v>2</v>
       </c>
-      <c r="R21" s="5">
-        <f>PRODUCT(P21*Q21)</f>
+      <c r="S21" s="5">
+        <f>PRODUCT(Q21*R21)</f>
         <v>10</v>
       </c>
-      <c r="T21" s="6"/>
-      <c r="U21" s="17"/>
-      <c r="V21" s="17"/>
-      <c r="W21" s="17"/>
-      <c r="X21" s="17"/>
-      <c r="Y21" s="7"/>
-    </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="T21" s="27"/>
+      <c r="V21" s="6"/>
+      <c r="W21" s="16"/>
+      <c r="X21" s="16"/>
+      <c r="Y21" s="16"/>
+      <c r="Z21" s="16"/>
+      <c r="AA21" s="7"/>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>33</v>
       </c>
@@ -2164,36 +2245,40 @@
         <f>PRODUCT(H22*I22)</f>
         <v>1</v>
       </c>
-      <c r="M22" s="4"/>
-      <c r="N22" s="21" t="s">
+      <c r="K22" s="27"/>
+      <c r="N22" s="4"/>
+      <c r="O22" t="s">
         <v>66</v>
       </c>
-      <c r="O22" s="21" t="s">
+      <c r="P22" t="s">
         <v>12</v>
       </c>
-      <c r="P22" s="21">
+      <c r="Q22">
         <v>8</v>
       </c>
-      <c r="Q22">
+      <c r="R22">
         <v>2</v>
       </c>
-      <c r="R22" s="5">
-        <f>PRODUCT(P22*Q22)</f>
+      <c r="S22" s="5">
+        <f>PRODUCT(Q22*R22)</f>
         <v>16</v>
       </c>
-      <c r="T22" s="2" t="s">
+      <c r="T22" s="27"/>
+      <c r="V22" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="U22" s="10"/>
-      <c r="V22" s="10"/>
       <c r="W22" s="10"/>
       <c r="X22" s="10"/>
-      <c r="Y22" s="3">
-        <f>SUM(Y23:Y25)</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y22" s="10"/>
+      <c r="Z22" s="10">
+        <v>0</v>
+      </c>
+      <c r="AA22" s="3">
+        <f>SUM(AA23:AA25)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>34</v>
       </c>
@@ -2218,53 +2303,65 @@
         <f>PRODUCT(H23*I23)</f>
         <v>15</v>
       </c>
-      <c r="M23" s="6"/>
-      <c r="N23" s="17"/>
-      <c r="O23" s="17"/>
-      <c r="P23" s="17"/>
-      <c r="Q23" s="17"/>
-      <c r="R23" s="7"/>
-      <c r="T23" s="4"/>
-      <c r="U23" s="21" t="s">
+      <c r="K23" s="27"/>
+      <c r="N23" s="6"/>
+      <c r="O23" s="16"/>
+      <c r="P23" s="16"/>
+      <c r="Q23" s="16"/>
+      <c r="R23" s="16"/>
+      <c r="S23" s="7"/>
+      <c r="T23" s="27"/>
+      <c r="V23" s="4"/>
+      <c r="W23" t="s">
         <v>21</v>
       </c>
-      <c r="V23" s="21" t="s">
+      <c r="X23" t="s">
         <v>26</v>
       </c>
-      <c r="Y23" s="5">
-        <f>PRODUCT(W23,X23)</f>
+      <c r="Y23" t="s">
+        <v>113</v>
+      </c>
+      <c r="Z23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA23" s="5">
+        <f>PRODUCT(Y23,Z23)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E24" s="4"/>
       <c r="J24" s="7"/>
-      <c r="M24" s="13" t="s">
+      <c r="K24" s="27"/>
+      <c r="N24" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="Q24">
+      <c r="R24">
         <v>11</v>
       </c>
-      <c r="R24" s="29">
-        <f>SUM(R25:R26)</f>
+      <c r="S24" s="22">
+        <f>SUM(S25:S26)</f>
         <v>99</v>
       </c>
-      <c r="T24" s="4"/>
-      <c r="U24" s="21" t="s">
+      <c r="V24" s="4"/>
+      <c r="W24" t="s">
         <v>115</v>
       </c>
-      <c r="V24" s="21" t="s">
+      <c r="X24" t="s">
         <v>12</v>
       </c>
-      <c r="W24">
+      <c r="Y24">
         <v>8</v>
       </c>
-      <c r="Y24" s="5">
-        <f>PRODUCT(W24,X24)</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z24">
+        <v>0</v>
+      </c>
+      <c r="AA24" s="5">
+        <f>PRODUCT(Y24,Z24)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>45</v>
       </c>
@@ -2277,47 +2374,51 @@
       <c r="I25" s="10">
         <v>1</v>
       </c>
-      <c r="J25" s="29">
+      <c r="J25" s="22">
         <f>SUM(J26:J28)</f>
         <v>17</v>
       </c>
-      <c r="M25" s="4"/>
-      <c r="N25" t="s">
+      <c r="N25" s="4"/>
+      <c r="O25" t="s">
         <v>21</v>
       </c>
-      <c r="O25" t="s">
+      <c r="P25" t="s">
         <v>7</v>
       </c>
-      <c r="P25">
+      <c r="Q25">
         <v>1</v>
       </c>
-      <c r="Q25">
+      <c r="R25">
         <v>11</v>
       </c>
-      <c r="R25" s="5">
-        <f>PRODUCT(Q25,P25)</f>
+      <c r="S25" s="5">
+        <f>PRODUCT(R25,Q25)</f>
         <v>11</v>
       </c>
-      <c r="T25" s="4" t="s">
+      <c r="T25" s="27"/>
+      <c r="V25" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="U25" t="s">
+      <c r="W25" t="s">
         <v>114</v>
       </c>
-      <c r="V25" s="21" t="s">
+      <c r="X25" t="s">
         <v>58</v>
       </c>
-      <c r="W25">
-        <v>4</v>
-      </c>
-      <c r="Y25" s="5"/>
-    </row>
-    <row r="26" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="16" t="s">
+      <c r="Y25">
+        <v>4</v>
+      </c>
+      <c r="Z25">
+        <v>0</v>
+      </c>
+      <c r="AA25" s="5"/>
+    </row>
+    <row r="26" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="B26" s="16"/>
-      <c r="C26" s="16"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="26"/>
       <c r="E26" s="4"/>
       <c r="F26" t="s">
         <v>21</v>
@@ -2335,35 +2436,37 @@
         <f>PRODUCT(H26*I26)</f>
         <v>1</v>
       </c>
-      <c r="M26" s="4"/>
-      <c r="N26" t="s">
+      <c r="K26" s="27"/>
+      <c r="N26" s="4"/>
+      <c r="O26" t="s">
         <v>57</v>
       </c>
-      <c r="O26" t="s">
+      <c r="P26" t="s">
         <v>26</v>
       </c>
-      <c r="P26">
+      <c r="Q26">
         <f>6+2</f>
         <v>8</v>
       </c>
-      <c r="Q26">
+      <c r="R26">
         <v>11</v>
       </c>
-      <c r="R26" s="5">
-        <f>PRODUCT(P26,Q26)</f>
+      <c r="S26" s="5">
+        <f>PRODUCT(Q26,R26)</f>
         <v>88</v>
       </c>
-      <c r="T26" s="19"/>
-      <c r="U26" s="17"/>
+      <c r="T26" s="27"/>
       <c r="V26" s="17"/>
-      <c r="W26" s="17"/>
-      <c r="X26" s="17"/>
-      <c r="Y26" s="20"/>
-    </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A27" s="16"/>
-      <c r="B27" s="16"/>
-      <c r="C27" s="16"/>
+      <c r="W26" s="16"/>
+      <c r="X26" s="16"/>
+      <c r="Y26" s="16"/>
+      <c r="Z26" s="16"/>
+      <c r="AA26" s="18"/>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A27" s="26"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="26"/>
       <c r="E27" s="4"/>
       <c r="F27" t="s">
         <v>17</v>
@@ -2382,24 +2485,29 @@
         <f>PRODUCT(H27*I27)</f>
         <v>15</v>
       </c>
-      <c r="M27" s="19"/>
+      <c r="K27" s="27"/>
       <c r="N27" s="17"/>
-      <c r="O27" s="17"/>
-      <c r="P27" s="17"/>
-      <c r="Q27" s="17"/>
-      <c r="R27" s="20"/>
-      <c r="T27" s="13" t="s">
+      <c r="O27" s="16"/>
+      <c r="P27" s="16"/>
+      <c r="Q27" s="16"/>
+      <c r="R27" s="16"/>
+      <c r="S27" s="18"/>
+      <c r="T27" s="29"/>
+      <c r="V27" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="Y27" s="15">
-        <f>SUM(Y28:Y34)</f>
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A28" s="16"/>
-      <c r="B28" s="16"/>
-      <c r="C28" s="16"/>
+      <c r="Z27" s="28">
+        <v>70510</v>
+      </c>
+      <c r="AA27" s="22">
+        <f>SUM(AA28:AA34)</f>
+        <v>1833260</v>
+      </c>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A28" s="26"/>
+      <c r="B28" s="26"/>
+      <c r="C28" s="26"/>
       <c r="E28" s="4"/>
       <c r="F28" t="s">
         <v>44</v>
@@ -2417,66 +2525,76 @@
         <f>PRODUCT(H28*I28)</f>
         <v>1</v>
       </c>
-      <c r="M28" s="13" t="s">
+      <c r="K28" s="27"/>
+      <c r="N28" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="Q28" s="22"/>
-      <c r="R28" s="5">
-        <f>(R29+R30)</f>
+      <c r="R28" s="19"/>
+      <c r="S28" s="5">
+        <f>(S29+S30)</f>
         <v>0</v>
       </c>
-      <c r="T28" s="4"/>
-      <c r="U28" t="s">
+      <c r="T28" s="27"/>
+      <c r="V28" s="4"/>
+      <c r="W28" t="s">
         <v>120</v>
       </c>
-      <c r="V28" t="s">
+      <c r="X28" t="s">
         <v>58</v>
       </c>
-      <c r="W28">
-        <v>4</v>
-      </c>
-      <c r="Y28" s="5">
-        <f>PRODUCT(W28,X28)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y28">
+        <v>4</v>
+      </c>
+      <c r="Z28" s="28">
+        <v>70510</v>
+      </c>
+      <c r="AA28" s="5">
+        <f>PRODUCT(Y28,Z28)</f>
+        <v>282040</v>
+      </c>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E29" s="6"/>
       <c r="J29" s="7"/>
-      <c r="M29" s="4"/>
-      <c r="N29" t="s">
+      <c r="K29" s="27"/>
+      <c r="N29" s="4"/>
+      <c r="O29" t="s">
         <v>21</v>
       </c>
-      <c r="O29" t="s">
+      <c r="P29" t="s">
         <v>58</v>
       </c>
-      <c r="P29">
-        <v>4</v>
-      </c>
-      <c r="Q29" s="22"/>
-      <c r="R29" s="5">
-        <f>(P29*Q29)</f>
+      <c r="Q29">
+        <v>4</v>
+      </c>
+      <c r="R29" s="19"/>
+      <c r="S29" s="5">
+        <f>(Q29*R29)</f>
         <v>0</v>
       </c>
-      <c r="T29" s="4"/>
-      <c r="U29" t="s">
+      <c r="T29" s="27"/>
+      <c r="V29" s="4"/>
+      <c r="W29" t="s">
         <v>121</v>
       </c>
-      <c r="V29" t="s">
+      <c r="X29" t="s">
         <v>58</v>
       </c>
-      <c r="W29">
-        <v>4</v>
-      </c>
-      <c r="Y29" s="5">
-        <f>PRODUCT(W29,X29)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y29">
+        <v>4</v>
+      </c>
+      <c r="Z29" s="28">
+        <v>70510</v>
+      </c>
+      <c r="AA29" s="5">
+        <f>PRODUCT(Y29,Z29)</f>
+        <v>282040</v>
+      </c>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
       <c r="E30" s="13" t="s">
         <v>39</v>
       </c>
@@ -2486,39 +2604,41 @@
       <c r="I30" s="10">
         <v>53</v>
       </c>
-      <c r="J30" s="29">
+      <c r="J30" s="22">
         <f>SUM(J31:J33)</f>
         <v>848</v>
       </c>
-      <c r="M30" s="4"/>
-      <c r="N30" s="18" t="s">
+      <c r="N30" s="4"/>
+      <c r="O30" t="s">
         <v>17</v>
       </c>
-      <c r="O30" s="18" t="s">
+      <c r="P30" t="s">
         <v>26</v>
       </c>
-      <c r="P30" s="18"/>
-      <c r="Q30" s="24"/>
-      <c r="R30" s="5">
+      <c r="R30" s="21"/>
+      <c r="S30" s="5">
         <v>0</v>
       </c>
-      <c r="T30" s="4"/>
-      <c r="U30" s="18" t="s">
+      <c r="T30" s="27"/>
+      <c r="V30" s="4"/>
+      <c r="W30" t="s">
         <v>122</v>
       </c>
-      <c r="V30" s="18" t="s">
+      <c r="X30" t="s">
         <v>58</v>
       </c>
-      <c r="W30" s="18">
-        <v>4</v>
-      </c>
-      <c r="X30" s="18"/>
-      <c r="Y30" s="5">
-        <f>PRODUCT(W30,X30)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y30">
+        <v>4</v>
+      </c>
+      <c r="Z30" s="28">
+        <v>70510</v>
+      </c>
+      <c r="AA30" s="5">
+        <f>PRODUCT(Y30,Z30)</f>
+        <v>282040</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
       <c r="E31" s="4"/>
       <c r="F31" t="s">
         <v>21</v>
@@ -2536,29 +2656,33 @@
         <f>PRODUCT(H31,I31)</f>
         <v>106</v>
       </c>
-      <c r="M31" s="19"/>
+      <c r="K31" s="27"/>
       <c r="N31" s="17"/>
-      <c r="O31" s="17"/>
-      <c r="P31" s="17"/>
-      <c r="Q31" s="17"/>
-      <c r="R31" s="20"/>
-      <c r="T31" s="13"/>
-      <c r="U31" s="18" t="s">
+      <c r="O31" s="16"/>
+      <c r="P31" s="16"/>
+      <c r="Q31" s="16"/>
+      <c r="R31" s="16"/>
+      <c r="S31" s="18"/>
+      <c r="T31" s="29"/>
+      <c r="V31" s="13"/>
+      <c r="W31" t="s">
         <v>123</v>
       </c>
-      <c r="V31" s="18" t="s">
+      <c r="X31" t="s">
         <v>58</v>
       </c>
-      <c r="W31" s="21">
-        <v>4</v>
-      </c>
-      <c r="X31" s="18"/>
-      <c r="Y31" s="5">
-        <f>PRODUCT(W31,X31)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y31">
+        <v>4</v>
+      </c>
+      <c r="Z31" s="28">
+        <v>70510</v>
+      </c>
+      <c r="AA31" s="5">
+        <f>PRODUCT(Y31,Z31)</f>
+        <v>282040</v>
+      </c>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="E32" s="4"/>
       <c r="F32" t="s">
         <v>17</v>
@@ -2577,33 +2701,38 @@
         <f>PRODUCT(H32,I32)</f>
         <v>530</v>
       </c>
-      <c r="M32" s="2" t="s">
+      <c r="K32" s="27"/>
+      <c r="N32" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="N32" s="10"/>
       <c r="O32" s="10"/>
       <c r="P32" s="10"/>
-      <c r="Q32" s="23"/>
-      <c r="R32" s="15">
-        <f>SUM(R33:R47)</f>
+      <c r="Q32" s="10"/>
+      <c r="R32" s="20"/>
+      <c r="S32" s="15">
+        <f>SUM(S33:S47)</f>
         <v>32</v>
       </c>
-      <c r="T32" s="4"/>
-      <c r="U32" s="21" t="s">
+      <c r="T32" s="29"/>
+      <c r="V32" s="4"/>
+      <c r="W32" t="s">
         <v>124</v>
       </c>
-      <c r="V32" s="21" t="s">
+      <c r="X32" t="s">
         <v>11</v>
       </c>
-      <c r="W32" s="21">
+      <c r="Y32">
         <v>3</v>
       </c>
-      <c r="Y32" s="5">
-        <f>PRODUCT(W32,X32)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="5:25" x14ac:dyDescent="0.25">
+      <c r="Z32" s="28">
+        <v>70510</v>
+      </c>
+      <c r="AA32" s="5">
+        <f>PRODUCT(Y32,Z32)</f>
+        <v>211530</v>
+      </c>
+    </row>
+    <row r="33" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E33" s="4"/>
       <c r="F33" t="s">
         <v>43</v>
@@ -2622,74 +2751,84 @@
         <f>PRODUCT(H33,I33)</f>
         <v>212</v>
       </c>
-      <c r="M33" s="4"/>
-      <c r="N33" t="s">
+      <c r="K33" s="27"/>
+      <c r="N33" s="4"/>
+      <c r="O33" t="s">
         <v>21</v>
       </c>
-      <c r="O33" t="s">
+      <c r="P33" t="s">
         <v>58</v>
       </c>
-      <c r="P33">
-        <v>4</v>
-      </c>
-      <c r="Q33" s="22"/>
-      <c r="R33" s="5">
-        <f>PRODUCT(P33*Q33)</f>
+      <c r="Q33">
+        <v>4</v>
+      </c>
+      <c r="R33" s="19"/>
+      <c r="S33" s="5">
+        <f>PRODUCT(Q33*R33)</f>
         <v>0</v>
       </c>
-      <c r="T33" s="4"/>
-      <c r="U33" s="21" t="s">
+      <c r="T33" s="27"/>
+      <c r="V33" s="4"/>
+      <c r="W33" t="s">
         <v>125</v>
       </c>
-      <c r="V33" s="21" t="s">
+      <c r="X33" t="s">
         <v>11</v>
       </c>
-      <c r="W33" s="21">
+      <c r="Y33">
         <v>3</v>
       </c>
-      <c r="Y33" s="5">
-        <f t="shared" ref="Y33:Y38" si="1">PRODUCT(W33,X33)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="5:25" x14ac:dyDescent="0.25">
+      <c r="Z33" s="28">
+        <v>70510</v>
+      </c>
+      <c r="AA33" s="5">
+        <f t="shared" ref="AA33:AA38" si="1">PRODUCT(Y33,Z33)</f>
+        <v>211530</v>
+      </c>
+    </row>
+    <row r="34" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E34" s="6"/>
-      <c r="F34" s="17"/>
-      <c r="G34" s="17"/>
-      <c r="H34" s="17"/>
-      <c r="I34" s="17"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="16"/>
+      <c r="H34" s="16"/>
+      <c r="I34" s="16"/>
       <c r="J34" s="7"/>
-      <c r="M34" s="4"/>
-      <c r="N34" t="s">
+      <c r="K34" s="27"/>
+      <c r="N34" s="4"/>
+      <c r="O34" t="s">
         <v>87</v>
       </c>
-      <c r="O34" t="s">
+      <c r="P34" t="s">
         <v>58</v>
       </c>
-      <c r="P34">
-        <v>4</v>
-      </c>
-      <c r="Q34" s="22"/>
-      <c r="R34" s="5">
-        <f>PRODUCT(P34*Q34)</f>
+      <c r="Q34">
+        <v>4</v>
+      </c>
+      <c r="R34" s="19"/>
+      <c r="S34" s="5">
+        <f>PRODUCT(Q34*R34)</f>
         <v>0</v>
       </c>
-      <c r="T34" s="4"/>
-      <c r="U34" s="21" t="s">
+      <c r="T34" s="27"/>
+      <c r="V34" s="4"/>
+      <c r="W34" t="s">
         <v>101</v>
       </c>
-      <c r="V34" s="21" t="s">
+      <c r="X34" t="s">
         <v>58</v>
       </c>
-      <c r="W34" s="21">
-        <v>4</v>
-      </c>
-      <c r="Y34" s="5">
+      <c r="Y34">
+        <v>4</v>
+      </c>
+      <c r="Z34" s="28">
+        <v>70510</v>
+      </c>
+      <c r="AA34" s="5">
         <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35" spans="5:25" x14ac:dyDescent="0.25">
+        <v>282040</v>
+      </c>
+    </row>
+    <row r="35" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E35" s="2" t="s">
         <v>96</v>
       </c>
@@ -2699,39 +2838,42 @@
       <c r="I35" s="10">
         <v>53</v>
       </c>
-      <c r="J35" s="29">
+      <c r="J35" s="22">
         <f>SUM(J36:J37)</f>
         <v>159</v>
       </c>
-      <c r="M35" s="4"/>
-      <c r="N35" s="18" t="s">
+      <c r="N35" s="4"/>
+      <c r="O35" t="s">
         <v>74</v>
       </c>
-      <c r="O35" s="18" t="s">
+      <c r="P35" t="s">
         <v>26</v>
       </c>
-      <c r="P35" s="18"/>
-      <c r="Q35" s="24"/>
-      <c r="R35" s="5">
-        <f>PRODUCT(P35*Q35)</f>
+      <c r="R35" s="21"/>
+      <c r="S35" s="5">
+        <f>PRODUCT(Q35*R35)</f>
         <v>0</v>
       </c>
-      <c r="T35" s="4"/>
-      <c r="U35" s="21" t="s">
+      <c r="T35" s="27"/>
+      <c r="V35" s="4"/>
+      <c r="W35" t="s">
         <v>126</v>
       </c>
-      <c r="V35" s="21" t="s">
+      <c r="X35" t="s">
         <v>61</v>
       </c>
-      <c r="W35" s="21">
+      <c r="Y35">
         <v>3</v>
       </c>
-      <c r="Y35" s="5">
+      <c r="Z35" s="28">
+        <v>70510</v>
+      </c>
+      <c r="AA35" s="5">
         <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="36" spans="5:25" x14ac:dyDescent="0.25">
+        <v>211530</v>
+      </c>
+    </row>
+    <row r="36" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E36" s="4"/>
       <c r="F36" t="s">
         <v>97</v>
@@ -2742,42 +2884,46 @@
       <c r="H36">
         <v>2</v>
       </c>
-      <c r="I36" s="21">
+      <c r="I36">
         <v>53</v>
       </c>
       <c r="J36" s="5">
         <f>PRODUCT(H36,I36)</f>
         <v>106</v>
       </c>
-      <c r="M36" s="13"/>
-      <c r="N36" s="21" t="s">
+      <c r="K36" s="27"/>
+      <c r="N36" s="13"/>
+      <c r="O36" t="s">
         <v>75</v>
       </c>
-      <c r="O36" s="21" t="s">
+      <c r="P36" t="s">
         <v>26</v>
       </c>
-      <c r="Q36" s="22"/>
-      <c r="R36" s="5">
-        <f>PRODUCT(P36*Q36)</f>
+      <c r="R36" s="19"/>
+      <c r="S36" s="5">
+        <f>PRODUCT(Q36*R36)</f>
         <v>0</v>
       </c>
-      <c r="T36" s="4"/>
-      <c r="U36" s="18" t="s">
+      <c r="T36" s="27"/>
+      <c r="V36" s="4"/>
+      <c r="W36" t="s">
         <v>82</v>
       </c>
-      <c r="V36" s="18" t="s">
+      <c r="X36" t="s">
         <v>10</v>
       </c>
-      <c r="W36" s="21">
+      <c r="Y36">
         <v>1</v>
       </c>
-      <c r="X36" s="18"/>
-      <c r="Y36" s="5">
+      <c r="Z36" s="28">
+        <v>70510</v>
+      </c>
+      <c r="AA36" s="5">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="5:25" x14ac:dyDescent="0.25">
+        <v>70510</v>
+      </c>
+    </row>
+    <row r="37" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E37" s="4"/>
       <c r="F37" t="s">
         <v>98</v>
@@ -2788,78 +2934,85 @@
       <c r="H37">
         <v>1</v>
       </c>
-      <c r="I37" s="21">
+      <c r="I37">
         <v>53</v>
       </c>
       <c r="J37" s="5">
         <f>PRODUCT(H37,I37)</f>
         <v>53</v>
       </c>
-      <c r="M37" s="4"/>
-      <c r="N37" s="21" t="s">
+      <c r="K37" s="27"/>
+      <c r="N37" s="4"/>
+      <c r="O37" t="s">
         <v>76</v>
       </c>
-      <c r="O37" s="21" t="s">
+      <c r="P37" t="s">
         <v>26</v>
       </c>
-      <c r="Q37" s="22"/>
-      <c r="R37" s="5">
-        <f>PRODUCT(P37,Q37)</f>
+      <c r="R37" s="19"/>
+      <c r="S37" s="5">
+        <f>PRODUCT(Q37,R37)</f>
         <v>0</v>
       </c>
-      <c r="T37" s="4"/>
-      <c r="U37" s="21" t="s">
+      <c r="T37" s="27"/>
+      <c r="V37" s="4"/>
+      <c r="W37" t="s">
         <v>127</v>
       </c>
-      <c r="V37" s="21" t="s">
+      <c r="X37" t="s">
         <v>58</v>
       </c>
-      <c r="W37" s="21">
-        <v>4</v>
-      </c>
-      <c r="X37" s="18"/>
-      <c r="Y37" s="5">
+      <c r="Y37">
+        <v>4</v>
+      </c>
+      <c r="Z37" s="28">
+        <v>70510</v>
+      </c>
+      <c r="AA37" s="5">
         <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="38" spans="5:25" x14ac:dyDescent="0.25">
+        <v>282040</v>
+      </c>
+    </row>
+    <row r="38" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E38" s="6"/>
-      <c r="F38" s="17"/>
-      <c r="G38" s="17"/>
-      <c r="H38" s="17"/>
-      <c r="I38" s="17"/>
+      <c r="F38" s="16"/>
+      <c r="G38" s="16"/>
+      <c r="H38" s="16"/>
+      <c r="I38" s="16"/>
       <c r="J38" s="7"/>
-      <c r="M38" s="4"/>
-      <c r="N38" s="21" t="s">
+      <c r="K38" s="27"/>
+      <c r="N38" s="4"/>
+      <c r="O38" t="s">
         <v>77</v>
       </c>
-      <c r="O38" s="21" t="s">
+      <c r="P38" t="s">
         <v>26</v>
       </c>
-      <c r="P38" s="18"/>
-      <c r="Q38" s="24"/>
-      <c r="R38" s="5">
-        <f>PRODUCT(P38,Q38)</f>
+      <c r="R38" s="21"/>
+      <c r="S38" s="5">
+        <f>PRODUCT(Q38,R38)</f>
         <v>0</v>
       </c>
-      <c r="T38" s="4"/>
-      <c r="U38" s="21" t="s">
+      <c r="T38" s="27"/>
+      <c r="V38" s="4"/>
+      <c r="W38" t="s">
         <v>128</v>
       </c>
-      <c r="V38" s="21" t="s">
-        <v>161</v>
-      </c>
-      <c r="W38" s="18">
+      <c r="X38" t="s">
+        <v>160</v>
+      </c>
+      <c r="Y38">
         <v>8</v>
       </c>
-      <c r="X38" s="18"/>
-      <c r="Y38" s="5">
+      <c r="Z38" s="28">
+        <v>70510</v>
+      </c>
+      <c r="AA38" s="5">
         <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="39" spans="5:25" x14ac:dyDescent="0.25">
+        <v>564080</v>
+      </c>
+    </row>
+    <row r="39" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E39" s="13" t="s">
         <v>47</v>
       </c>
@@ -2870,33 +3023,35 @@
         <f>I17</f>
         <v>23272</v>
       </c>
-      <c r="J39" s="29">
+      <c r="J39" s="22">
         <f>SUM(J40:J44)</f>
         <v>349080</v>
       </c>
-      <c r="M39" s="4"/>
-      <c r="N39" s="21" t="s">
+      <c r="K39" s="30"/>
+      <c r="N39" s="4"/>
+      <c r="O39" t="s">
         <v>78</v>
       </c>
-      <c r="O39" s="21" t="s">
-        <v>161</v>
-      </c>
-      <c r="P39" s="18">
+      <c r="P39" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q39">
         <v>8</v>
       </c>
-      <c r="Q39" s="24"/>
-      <c r="R39" s="5">
-        <f>PRODUCT(P39,Q39)</f>
+      <c r="R39" s="21"/>
+      <c r="S39" s="5">
+        <f>PRODUCT(Q39,R39)</f>
         <v>8</v>
       </c>
-      <c r="T39" s="6"/>
-      <c r="U39" s="17"/>
-      <c r="V39" s="17"/>
-      <c r="W39" s="17"/>
-      <c r="X39" s="17"/>
-      <c r="Y39" s="7"/>
-    </row>
-    <row r="40" spans="5:25" x14ac:dyDescent="0.25">
+      <c r="T39" s="27"/>
+      <c r="V39" s="6"/>
+      <c r="W39" s="16"/>
+      <c r="X39" s="16"/>
+      <c r="Y39" s="16"/>
+      <c r="Z39" s="16"/>
+      <c r="AA39" s="7"/>
+    </row>
+    <row r="40" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E40" s="4"/>
       <c r="F40" t="s">
         <v>21</v>
@@ -2915,31 +3070,38 @@
         <f>PRODUCT(H40,I40)</f>
         <v>93088</v>
       </c>
-      <c r="M40" s="4"/>
-      <c r="N40" s="21" t="s">
+      <c r="K40" s="27"/>
+      <c r="N40" s="4"/>
+      <c r="O40" t="s">
         <v>79</v>
       </c>
-      <c r="O40" s="21" t="s">
-        <v>161</v>
-      </c>
-      <c r="P40" s="18">
+      <c r="P40" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q40">
         <v>8</v>
       </c>
-      <c r="Q40" s="24"/>
-      <c r="R40" s="5">
-        <f t="shared" ref="R40:R46" si="2">PRODUCT(P40,Q40)</f>
+      <c r="R40" s="21"/>
+      <c r="S40" s="5">
+        <f t="shared" ref="S40:S46" si="2">PRODUCT(Q40,R40)</f>
         <v>8</v>
       </c>
-      <c r="T40" s="2" t="s">
+      <c r="T40" s="27"/>
+      <c r="V40" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="U40" s="10"/>
-      <c r="V40" s="10"/>
       <c r="W40" s="10"/>
       <c r="X40" s="10"/>
-      <c r="Y40" s="11"/>
-    </row>
-    <row r="41" spans="5:25" x14ac:dyDescent="0.25">
+      <c r="Y40" s="10"/>
+      <c r="Z40">
+        <v>228265</v>
+      </c>
+      <c r="AA40" s="22">
+        <f>SUM(AA41:AA49)</f>
+        <v>11641515</v>
+      </c>
+    </row>
+    <row r="41" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E41" s="4"/>
       <c r="F41" t="s">
         <v>48</v>
@@ -2958,35 +3120,42 @@
         <f>PRODUCT(H41,I41)</f>
         <v>93088</v>
       </c>
-      <c r="M41" s="4"/>
-      <c r="N41" s="21" t="s">
+      <c r="K41" s="27"/>
+      <c r="N41" s="4"/>
+      <c r="O41" t="s">
         <v>80</v>
       </c>
-      <c r="O41" s="21" t="s">
+      <c r="P41" t="s">
         <v>67</v>
       </c>
-      <c r="P41" s="18">
+      <c r="Q41">
         <v>5</v>
       </c>
-      <c r="Q41" s="24"/>
-      <c r="R41" s="5">
+      <c r="R41" s="21"/>
+      <c r="S41" s="5">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="T41" s="4"/>
-      <c r="U41" s="18" t="s">
+      <c r="T41" s="27"/>
+      <c r="V41" s="4"/>
+      <c r="W41" t="s">
         <v>130</v>
       </c>
-      <c r="V41" s="18" t="s">
+      <c r="X41" t="s">
         <v>58</v>
       </c>
-      <c r="W41" s="18">
-        <v>4</v>
-      </c>
-      <c r="X41" s="18"/>
-      <c r="Y41" s="5"/>
-    </row>
-    <row r="42" spans="5:25" x14ac:dyDescent="0.25">
+      <c r="Y41">
+        <v>4</v>
+      </c>
+      <c r="Z41">
+        <v>228265</v>
+      </c>
+      <c r="AA41" s="5">
+        <f>PRODUCT(Y41,Z41)</f>
+        <v>913060</v>
+      </c>
+    </row>
+    <row r="42" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E42" s="4"/>
       <c r="F42" t="s">
         <v>49</v>
@@ -3005,35 +3174,42 @@
         <f>PRODUCT(H42,I42)</f>
         <v>93088</v>
       </c>
-      <c r="M42" s="4"/>
-      <c r="N42" s="21" t="s">
+      <c r="K42" s="27"/>
+      <c r="N42" s="4"/>
+      <c r="O42" t="s">
         <v>81</v>
       </c>
-      <c r="O42" s="21" t="s">
+      <c r="P42" t="s">
         <v>88</v>
       </c>
-      <c r="P42" s="21">
+      <c r="Q42">
         <v>5</v>
       </c>
-      <c r="Q42" s="24"/>
-      <c r="R42" s="5">
+      <c r="R42" s="21"/>
+      <c r="S42" s="5">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="T42" s="4"/>
-      <c r="U42" s="18" t="s">
+      <c r="T42" s="27"/>
+      <c r="V42" s="4"/>
+      <c r="W42" t="s">
         <v>131</v>
       </c>
-      <c r="V42" s="18" t="s">
+      <c r="X42" t="s">
         <v>58</v>
       </c>
-      <c r="W42" s="18">
-        <v>4</v>
-      </c>
-      <c r="X42" s="18"/>
-      <c r="Y42" s="5"/>
-    </row>
-    <row r="43" spans="5:25" x14ac:dyDescent="0.25">
+      <c r="Y42">
+        <v>4</v>
+      </c>
+      <c r="Z42">
+        <v>228265</v>
+      </c>
+      <c r="AA42" s="5">
+        <f>PRODUCT(Y42,Z42)</f>
+        <v>913060</v>
+      </c>
+    </row>
+    <row r="43" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E43" s="4"/>
       <c r="F43" t="s">
         <v>50</v>
@@ -3052,35 +3228,42 @@
         <f>PRODUCT(H43,I43)</f>
         <v>46544</v>
       </c>
-      <c r="M43" s="4"/>
-      <c r="N43" s="21" t="s">
+      <c r="K43" s="27"/>
+      <c r="N43" s="4"/>
+      <c r="O43" t="s">
         <v>82</v>
       </c>
-      <c r="O43" s="21" t="s">
+      <c r="P43" t="s">
         <v>10</v>
       </c>
-      <c r="P43" s="21">
+      <c r="Q43">
         <v>1</v>
       </c>
-      <c r="Q43" s="24"/>
-      <c r="R43" s="5">
+      <c r="R43" s="21"/>
+      <c r="S43" s="5">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="T43" s="4"/>
-      <c r="U43" s="18" t="s">
+      <c r="T43" s="27"/>
+      <c r="V43" s="4"/>
+      <c r="W43" t="s">
         <v>132</v>
       </c>
-      <c r="V43" s="18" t="s">
+      <c r="X43" t="s">
         <v>6</v>
       </c>
-      <c r="W43" s="18">
+      <c r="Y43">
         <v>2</v>
       </c>
-      <c r="X43" s="18"/>
-      <c r="Y43" s="5"/>
-    </row>
-    <row r="44" spans="5:25" x14ac:dyDescent="0.25">
+      <c r="Z43">
+        <v>228265</v>
+      </c>
+      <c r="AA43" s="5">
+        <f>PRODUCT(Y43,Z43)</f>
+        <v>456530</v>
+      </c>
+    </row>
+    <row r="44" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E44" s="4"/>
       <c r="F44" t="s">
         <v>51</v>
@@ -3099,66 +3282,80 @@
         <f>PRODUCT(H44,I44)</f>
         <v>23272</v>
       </c>
-      <c r="M44" s="4"/>
-      <c r="N44" s="21" t="s">
+      <c r="K44" s="27"/>
+      <c r="N44" s="4"/>
+      <c r="O44" t="s">
         <v>83</v>
       </c>
-      <c r="O44" s="21" t="s">
+      <c r="P44" t="s">
         <v>7</v>
       </c>
-      <c r="P44" s="21">
+      <c r="Q44">
         <v>1</v>
       </c>
-      <c r="Q44" s="24"/>
-      <c r="R44" s="5">
+      <c r="R44" s="21"/>
+      <c r="S44" s="5">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="T44" s="4"/>
-      <c r="U44" s="18" t="s">
+      <c r="T44" s="27"/>
+      <c r="V44" s="4"/>
+      <c r="W44" t="s">
         <v>133</v>
       </c>
-      <c r="V44" s="18" t="s">
-        <v>161</v>
-      </c>
-      <c r="W44" s="18">
+      <c r="X44" t="s">
+        <v>160</v>
+      </c>
+      <c r="Y44">
         <v>8</v>
       </c>
-      <c r="X44" s="18"/>
-      <c r="Y44" s="5"/>
-    </row>
-    <row r="45" spans="5:25" x14ac:dyDescent="0.25">
+      <c r="Z44">
+        <v>228265</v>
+      </c>
+      <c r="AA44" s="5">
+        <f>PRODUCT(Y44,Z44)</f>
+        <v>1826120</v>
+      </c>
+    </row>
+    <row r="45" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E45" s="6"/>
       <c r="J45" s="5"/>
-      <c r="M45" s="4"/>
-      <c r="N45" s="21" t="s">
+      <c r="K45" s="27"/>
+      <c r="N45" s="4"/>
+      <c r="O45" t="s">
         <v>84</v>
       </c>
-      <c r="O45" s="21" t="s">
+      <c r="P45" t="s">
         <v>58</v>
       </c>
-      <c r="P45" s="21">
-        <v>4</v>
-      </c>
-      <c r="Q45" s="24"/>
-      <c r="R45" s="5">
+      <c r="Q45">
+        <v>4</v>
+      </c>
+      <c r="R45" s="21"/>
+      <c r="S45" s="5">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="T45" s="4"/>
-      <c r="U45" s="18" t="s">
+      <c r="T45" s="27"/>
+      <c r="V45" s="4"/>
+      <c r="W45" t="s">
         <v>134</v>
       </c>
-      <c r="V45" s="18" t="s">
-        <v>161</v>
-      </c>
-      <c r="W45" s="18">
+      <c r="X45" t="s">
+        <v>160</v>
+      </c>
+      <c r="Y45">
         <v>8</v>
       </c>
-      <c r="X45" s="18"/>
-      <c r="Y45" s="5"/>
-    </row>
-    <row r="46" spans="5:25" x14ac:dyDescent="0.25">
+      <c r="Z45">
+        <v>228265</v>
+      </c>
+      <c r="AA45" s="5">
+        <f>PRODUCT(Y45,Z45)</f>
+        <v>1826120</v>
+      </c>
+    </row>
+    <row r="46" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E46" s="13" t="s">
         <v>52</v>
       </c>
@@ -3168,36 +3365,42 @@
       <c r="I46" s="10">
         <v>317</v>
       </c>
-      <c r="J46" s="31">
+      <c r="J46" s="24">
         <v>1268</v>
       </c>
-      <c r="M46" s="4"/>
-      <c r="N46" s="21" t="s">
+      <c r="K46" s="31"/>
+      <c r="N46" s="4"/>
+      <c r="O46" t="s">
         <v>85</v>
       </c>
-      <c r="O46" s="21" t="s">
+      <c r="P46" t="s">
         <v>26</v>
       </c>
-      <c r="P46" s="18"/>
-      <c r="Q46" s="24"/>
-      <c r="R46" s="5">
+      <c r="R46" s="21"/>
+      <c r="S46" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="T46" s="4"/>
-      <c r="U46" s="18" t="s">
+      <c r="T46" s="27"/>
+      <c r="V46" s="4"/>
+      <c r="W46" t="s">
         <v>80</v>
       </c>
-      <c r="V46" s="18" t="s">
+      <c r="X46" t="s">
         <v>67</v>
       </c>
-      <c r="W46" s="18">
+      <c r="Y46">
         <v>5</v>
       </c>
-      <c r="X46" s="18"/>
-      <c r="Y46" s="5"/>
-    </row>
-    <row r="47" spans="5:25" x14ac:dyDescent="0.25">
+      <c r="Z46">
+        <v>228265</v>
+      </c>
+      <c r="AA46" s="5">
+        <f t="shared" ref="AA46:AA49" si="4">PRODUCT(Y46,Z46)</f>
+        <v>1141325</v>
+      </c>
+    </row>
+    <row r="47" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E47" s="4"/>
       <c r="F47" t="s">
         <v>21</v>
@@ -3215,61 +3418,74 @@
         <f>PRODUCT(H47,I47)</f>
         <v>1268</v>
       </c>
-      <c r="M47" s="4"/>
-      <c r="N47" s="21" t="s">
+      <c r="K47" s="27"/>
+      <c r="N47" s="4"/>
+      <c r="O47" t="s">
         <v>86</v>
       </c>
-      <c r="O47" s="21" t="s">
+      <c r="P47" t="s">
         <v>26</v>
       </c>
-      <c r="P47" s="18"/>
-      <c r="Q47" s="24"/>
-      <c r="R47" s="5">
-        <f>PRODUCT(P47,Q47)</f>
+      <c r="R47" s="21"/>
+      <c r="S47" s="5">
+        <f>PRODUCT(Q47,R47)</f>
         <v>0</v>
       </c>
-      <c r="T47" s="4"/>
-      <c r="U47" s="18" t="s">
+      <c r="T47" s="27"/>
+      <c r="V47" s="4"/>
+      <c r="W47" t="s">
         <v>135</v>
       </c>
-      <c r="V47" s="18" t="s">
-        <v>161</v>
-      </c>
-      <c r="W47" s="18">
+      <c r="X47" t="s">
+        <v>160</v>
+      </c>
+      <c r="Y47">
         <v>8</v>
       </c>
-      <c r="X47" s="18"/>
-      <c r="Y47" s="5"/>
-    </row>
-    <row r="48" spans="5:25" x14ac:dyDescent="0.25">
+      <c r="Z47">
+        <v>228265</v>
+      </c>
+      <c r="AA47" s="5">
+        <f t="shared" si="4"/>
+        <v>1826120</v>
+      </c>
+    </row>
+    <row r="48" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E48" s="6"/>
-      <c r="F48" s="17"/>
-      <c r="G48" s="17"/>
-      <c r="H48" s="17"/>
-      <c r="I48" s="17"/>
+      <c r="F48" s="16"/>
+      <c r="G48" s="16"/>
+      <c r="H48" s="16"/>
+      <c r="I48" s="16"/>
       <c r="J48" s="7"/>
-      <c r="M48" s="6"/>
-      <c r="N48" s="17" t="s">
+      <c r="K48" s="27"/>
+      <c r="N48" s="6"/>
+      <c r="O48" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="O48" s="17"/>
-      <c r="P48" s="17"/>
-      <c r="Q48" s="17"/>
-      <c r="R48" s="7"/>
-      <c r="T48" s="4"/>
-      <c r="U48" s="18" t="s">
+      <c r="P48" s="16"/>
+      <c r="Q48" s="16"/>
+      <c r="R48" s="16"/>
+      <c r="S48" s="7"/>
+      <c r="T48" s="27"/>
+      <c r="V48" s="4"/>
+      <c r="W48" t="s">
         <v>136</v>
       </c>
-      <c r="V48" s="18" t="s">
+      <c r="X48" t="s">
         <v>58</v>
       </c>
-      <c r="W48" s="18">
-        <v>4</v>
-      </c>
-      <c r="X48" s="18"/>
-      <c r="Y48" s="5"/>
-    </row>
-    <row r="49" spans="5:25" x14ac:dyDescent="0.25">
+      <c r="Y48">
+        <v>4</v>
+      </c>
+      <c r="Z48">
+        <v>228265</v>
+      </c>
+      <c r="AA48" s="5">
+        <f t="shared" si="4"/>
+        <v>913060</v>
+      </c>
+    </row>
+    <row r="49" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E49" s="2" t="s">
         <v>99</v>
       </c>
@@ -3277,555 +3493,600 @@
       <c r="G49" s="10"/>
       <c r="H49" s="10"/>
       <c r="I49" s="10"/>
-      <c r="J49" s="29">
+      <c r="J49" s="22">
         <f>SUM(J50:J54)</f>
         <v>14</v>
       </c>
-      <c r="M49" s="2" t="s">
+      <c r="K49" s="30"/>
+      <c r="N49" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="N49" s="10"/>
       <c r="O49" s="10"/>
       <c r="P49" s="10"/>
       <c r="Q49" s="10"/>
-      <c r="R49" s="15">
-        <f>SUM(R50:R51)</f>
-        <v>0</v>
-      </c>
-      <c r="T49" s="4"/>
-      <c r="U49" s="18" t="s">
+      <c r="R49">
+        <v>508</v>
+      </c>
+      <c r="S49" s="22">
+        <f>SUM(S50:S51)</f>
+        <v>2540</v>
+      </c>
+      <c r="T49" s="29"/>
+      <c r="V49" s="4"/>
+      <c r="W49" t="s">
         <v>137</v>
       </c>
-      <c r="V49" s="18" t="s">
-        <v>161</v>
-      </c>
-      <c r="W49" s="18">
+      <c r="X49" t="s">
+        <v>160</v>
+      </c>
+      <c r="Y49">
         <v>8</v>
       </c>
-      <c r="X49" s="18"/>
-      <c r="Y49" s="5"/>
-    </row>
-    <row r="50" spans="5:25" x14ac:dyDescent="0.25">
+      <c r="Z49">
+        <v>228265</v>
+      </c>
+      <c r="AA49" s="5">
+        <f t="shared" si="4"/>
+        <v>1826120</v>
+      </c>
+    </row>
+    <row r="50" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E50" s="4"/>
-      <c r="F50" s="18" t="s">
+      <c r="F50" t="s">
         <v>21</v>
       </c>
-      <c r="G50" s="18" t="s">
+      <c r="G50" t="s">
         <v>58</v>
       </c>
-      <c r="H50" s="18">
-        <v>4</v>
-      </c>
-      <c r="I50" s="18"/>
+      <c r="H50">
+        <v>4</v>
+      </c>
       <c r="J50" s="5">
         <f>PRODUCT(H50,I50)</f>
         <v>4</v>
       </c>
-      <c r="M50" s="4"/>
-      <c r="N50" s="21" t="s">
+      <c r="K50" s="27"/>
+      <c r="N50" s="4"/>
+      <c r="O50" t="s">
         <v>117</v>
       </c>
-      <c r="O50" s="21" t="s">
+      <c r="P50" t="s">
         <v>7</v>
       </c>
-      <c r="P50" s="18">
+      <c r="Q50">
         <v>1</v>
       </c>
-      <c r="Q50" s="18"/>
-      <c r="R50" s="5">
-        <f>PRODUCT(P50*Q50)</f>
-        <v>0</v>
-      </c>
-      <c r="T50" s="6"/>
-      <c r="U50" s="17"/>
-      <c r="V50" s="17"/>
-      <c r="W50" s="17"/>
-      <c r="X50" s="17"/>
-      <c r="Y50" s="7"/>
-    </row>
-    <row r="51" spans="5:25" x14ac:dyDescent="0.25">
+      <c r="R50">
+        <v>508</v>
+      </c>
+      <c r="S50" s="5">
+        <f>PRODUCT(Q50*R50)</f>
+        <v>508</v>
+      </c>
+      <c r="T50" s="27"/>
+      <c r="V50" s="6"/>
+      <c r="W50" s="16"/>
+      <c r="X50" s="16"/>
+      <c r="Y50" s="16"/>
+      <c r="Z50" s="16"/>
+      <c r="AA50" s="7"/>
+    </row>
+    <row r="51" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E51" s="4"/>
-      <c r="F51" s="18" t="s">
+      <c r="F51" t="s">
         <v>99</v>
       </c>
-      <c r="G51" s="18" t="s">
+      <c r="G51" t="s">
         <v>26</v>
       </c>
-      <c r="H51" s="18">
+      <c r="H51">
         <v>2</v>
       </c>
-      <c r="I51" s="18"/>
       <c r="J51" s="5">
         <f>PRODUCT(H51,I51)</f>
         <v>2</v>
       </c>
-      <c r="M51" s="4"/>
-      <c r="N51" s="21" t="s">
+      <c r="K51" s="27"/>
+      <c r="N51" s="4"/>
+      <c r="O51" t="s">
         <v>118</v>
       </c>
-      <c r="O51" s="21" t="s">
+      <c r="P51" t="s">
         <v>58</v>
       </c>
-      <c r="P51" s="18">
-        <v>4</v>
-      </c>
-      <c r="Q51" s="18"/>
-      <c r="R51" s="5">
-        <f>PRODUCT(P51*Q51)</f>
-        <v>0</v>
-      </c>
-      <c r="T51" s="2" t="s">
+      <c r="Q51">
+        <v>4</v>
+      </c>
+      <c r="R51">
+        <v>508</v>
+      </c>
+      <c r="S51" s="5">
+        <f>PRODUCT(Q51*R51)</f>
+        <v>2032</v>
+      </c>
+      <c r="T51" s="27"/>
+      <c r="V51" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="U51" s="10"/>
-      <c r="V51" s="10"/>
       <c r="W51" s="10"/>
       <c r="X51" s="10"/>
-      <c r="Y51" s="11"/>
-    </row>
-    <row r="52" spans="5:25" x14ac:dyDescent="0.25">
+      <c r="Z51" s="10">
+        <v>70510</v>
+      </c>
+      <c r="AA51" s="23">
+        <f>SUM(AA52:AA53)</f>
+        <v>846120</v>
+      </c>
+    </row>
+    <row r="52" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E52" s="4"/>
-      <c r="F52" s="18" t="s">
+      <c r="F52" t="s">
         <v>100</v>
       </c>
-      <c r="G52" s="18" t="s">
+      <c r="G52" t="s">
         <v>58</v>
       </c>
-      <c r="H52" s="18">
-        <v>4</v>
-      </c>
-      <c r="I52" s="18"/>
+      <c r="H52">
+        <v>4</v>
+      </c>
       <c r="J52" s="5">
         <f>PRODUCT(H52,I52)</f>
         <v>4</v>
       </c>
-      <c r="M52" s="6"/>
-      <c r="N52" s="17"/>
-      <c r="O52" s="17"/>
-      <c r="P52" s="17"/>
-      <c r="Q52" s="17"/>
-      <c r="R52" s="7"/>
-      <c r="T52" s="4"/>
-      <c r="U52" s="18" t="s">
+      <c r="K52" s="27"/>
+      <c r="N52" s="6"/>
+      <c r="O52" s="16"/>
+      <c r="P52" s="16"/>
+      <c r="Q52" s="16"/>
+      <c r="R52" s="16"/>
+      <c r="S52" s="7"/>
+      <c r="T52" s="27"/>
+      <c r="V52" s="4"/>
+      <c r="W52" t="s">
         <v>131</v>
       </c>
-      <c r="V52" s="18" t="s">
+      <c r="X52" t="s">
         <v>58</v>
       </c>
-      <c r="W52" s="21">
-        <v>4</v>
-      </c>
-      <c r="X52" s="18"/>
-      <c r="Y52" s="5"/>
-    </row>
-    <row r="53" spans="5:25" x14ac:dyDescent="0.25">
+      <c r="Y52">
+        <v>4</v>
+      </c>
+      <c r="Z52" s="27">
+        <v>70510</v>
+      </c>
+      <c r="AA52" s="5">
+        <f>PRODUCT(Y52,Z52)</f>
+        <v>282040</v>
+      </c>
+    </row>
+    <row r="53" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E53" s="4"/>
-      <c r="F53" s="18" t="s">
+      <c r="F53" t="s">
         <v>101</v>
       </c>
-      <c r="G53" s="18" t="s">
+      <c r="G53" t="s">
         <v>58</v>
       </c>
-      <c r="H53" s="18">
-        <v>4</v>
-      </c>
-      <c r="I53" s="18"/>
+      <c r="H53">
+        <v>4</v>
+      </c>
       <c r="J53" s="5">
         <f>PRODUCT(H53,I53)</f>
         <v>4</v>
       </c>
-      <c r="M53" s="10"/>
+      <c r="K53" s="27"/>
       <c r="N53" s="10"/>
       <c r="O53" s="10"/>
       <c r="P53" s="10"/>
       <c r="Q53" s="10"/>
       <c r="R53" s="10"/>
-      <c r="T53" s="4"/>
-      <c r="U53" s="18" t="s">
+      <c r="S53" s="10"/>
+      <c r="T53" s="27"/>
+      <c r="V53" s="4"/>
+      <c r="W53" t="s">
         <v>138</v>
       </c>
-      <c r="V53" s="18" t="s">
-        <v>163</v>
-      </c>
-      <c r="W53" s="21">
+      <c r="X53" t="s">
+        <v>162</v>
+      </c>
+      <c r="Y53">
         <v>8</v>
       </c>
-      <c r="X53" s="18"/>
-      <c r="Y53" s="5"/>
-    </row>
-    <row r="54" spans="5:25" x14ac:dyDescent="0.25">
+      <c r="Z53" s="27">
+        <v>70510</v>
+      </c>
+      <c r="AA53" s="5">
+        <f>PRODUCT(Y53,Z53)</f>
+        <v>564080</v>
+      </c>
+    </row>
+    <row r="54" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E54" s="6"/>
-      <c r="F54" s="17"/>
-      <c r="G54" s="17"/>
-      <c r="H54" s="17"/>
-      <c r="I54" s="17"/>
+      <c r="F54" s="16"/>
+      <c r="G54" s="16"/>
+      <c r="H54" s="16"/>
+      <c r="I54" s="16"/>
       <c r="J54" s="7"/>
-      <c r="M54" s="18"/>
-      <c r="N54" s="18"/>
-      <c r="O54" s="18"/>
-      <c r="P54" s="18"/>
-      <c r="Q54" s="18"/>
-      <c r="R54" s="18"/>
-      <c r="T54" s="6"/>
-      <c r="U54" s="17"/>
-      <c r="V54" s="17"/>
-      <c r="W54" s="17"/>
-      <c r="X54" s="17"/>
-      <c r="Y54" s="7"/>
-    </row>
-    <row r="55" spans="5:25" x14ac:dyDescent="0.25">
-      <c r="M55" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="N55" s="10"/>
+      <c r="K54" s="27"/>
+      <c r="V54" s="6"/>
+      <c r="W54" s="16"/>
+      <c r="X54" s="16"/>
+      <c r="Y54" s="16"/>
+      <c r="Z54" s="16"/>
+      <c r="AA54" s="7"/>
+    </row>
+    <row r="55" spans="5:27" x14ac:dyDescent="0.25">
+      <c r="N55" s="2" t="s">
+        <v>142</v>
+      </c>
       <c r="O55" s="10"/>
       <c r="P55" s="10"/>
       <c r="Q55" s="10"/>
-      <c r="R55" s="11"/>
-      <c r="T55" s="13" t="s">
+      <c r="R55" s="10"/>
+      <c r="S55" s="11"/>
+      <c r="T55" s="27"/>
+      <c r="V55" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="U55" s="18"/>
-      <c r="V55" s="18"/>
-      <c r="W55" s="18"/>
-      <c r="X55" s="18"/>
-      <c r="Y55" s="5"/>
-    </row>
-    <row r="56" spans="5:25" x14ac:dyDescent="0.25">
+      <c r="Z55" s="28">
+        <v>272</v>
+      </c>
+      <c r="AA55" s="22">
+        <f>SUM(AA56:AA59)</f>
+        <v>1102</v>
+      </c>
+    </row>
+    <row r="56" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E56" s="2" t="s">
-        <v>142</v>
+        <v>165</v>
       </c>
       <c r="F56" s="10"/>
       <c r="G56" s="10"/>
       <c r="H56" s="10"/>
       <c r="I56" s="10"/>
       <c r="J56" s="11"/>
-      <c r="M56" s="4"/>
-      <c r="N56" s="18" t="s">
+      <c r="K56" s="27"/>
+      <c r="N56" s="4"/>
+      <c r="O56" t="s">
+        <v>143</v>
+      </c>
+      <c r="P56" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q56">
+        <v>4</v>
+      </c>
+      <c r="S56" s="5"/>
+      <c r="T56" s="27"/>
+      <c r="V56" s="4"/>
+      <c r="W56" t="s">
+        <v>131</v>
+      </c>
+      <c r="X56" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y56">
+        <v>4</v>
+      </c>
+      <c r="Z56" s="28">
+        <v>272</v>
+      </c>
+      <c r="AA56" s="5">
+        <f>SUM(Y56,Z56)</f>
+        <v>276</v>
+      </c>
+    </row>
+    <row r="57" spans="5:27" x14ac:dyDescent="0.25">
+      <c r="E57" s="4"/>
+      <c r="F57" t="s">
+        <v>150</v>
+      </c>
+      <c r="G57" t="s">
+        <v>26</v>
+      </c>
+      <c r="J57" s="5"/>
+      <c r="K57" s="27"/>
+      <c r="N57" s="4"/>
+      <c r="O57" t="s">
         <v>144</v>
       </c>
-      <c r="O56" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="P56" s="18">
-        <v>4</v>
-      </c>
-      <c r="Q56" s="18"/>
-      <c r="R56" s="5"/>
-      <c r="T56" s="4"/>
-      <c r="U56" s="18" t="s">
-        <v>131</v>
-      </c>
-      <c r="V56" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="W56" s="18">
-        <v>4</v>
-      </c>
-      <c r="X56" s="18"/>
-      <c r="Y56" s="5"/>
-    </row>
-    <row r="57" spans="5:25" x14ac:dyDescent="0.25">
-      <c r="E57" s="4"/>
-      <c r="F57" s="18" t="s">
+      <c r="P57" t="s">
+        <v>26</v>
+      </c>
+      <c r="S57" s="5"/>
+      <c r="T57" s="27"/>
+      <c r="V57" s="4"/>
+      <c r="W57" t="s">
+        <v>140</v>
+      </c>
+      <c r="X57" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y57">
+        <v>3</v>
+      </c>
+      <c r="Z57" s="28">
+        <v>272</v>
+      </c>
+      <c r="AA57" s="5">
+        <f t="shared" ref="AA57:AA58" si="5">SUM(Y57,Z57)</f>
+        <v>275</v>
+      </c>
+    </row>
+    <row r="58" spans="5:27" x14ac:dyDescent="0.25">
+      <c r="E58" s="4"/>
+      <c r="F58" t="s">
         <v>151</v>
       </c>
-      <c r="G57" s="18" t="s">
+      <c r="G58" t="s">
         <v>26</v>
       </c>
-      <c r="H57" s="18"/>
-      <c r="I57" s="18"/>
-      <c r="J57" s="5"/>
-      <c r="M57" s="4"/>
-      <c r="N57" s="18" t="s">
+      <c r="J58" s="5"/>
+      <c r="K58" s="27"/>
+      <c r="N58" s="6"/>
+      <c r="O58" s="16"/>
+      <c r="P58" s="16"/>
+      <c r="Q58" s="16"/>
+      <c r="R58" s="16"/>
+      <c r="S58" s="7"/>
+      <c r="T58" s="27"/>
+      <c r="V58" s="4"/>
+      <c r="W58" t="s">
+        <v>125</v>
+      </c>
+      <c r="X58" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y58">
+        <v>3</v>
+      </c>
+      <c r="Z58" s="28">
+        <v>272</v>
+      </c>
+      <c r="AA58" s="5">
+        <f t="shared" si="5"/>
+        <v>275</v>
+      </c>
+    </row>
+    <row r="59" spans="5:27" x14ac:dyDescent="0.25">
+      <c r="E59" s="4"/>
+      <c r="F59" t="s">
+        <v>152</v>
+      </c>
+      <c r="G59" t="s">
+        <v>26</v>
+      </c>
+      <c r="J59" s="5"/>
+      <c r="K59" s="27"/>
+      <c r="N59" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="O57" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="P57" s="18"/>
-      <c r="Q57" s="18"/>
-      <c r="R57" s="5"/>
-      <c r="T57" s="4"/>
-      <c r="U57" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="V57" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="W57" s="18">
-        <v>3</v>
-      </c>
-      <c r="X57" s="18"/>
-      <c r="Y57" s="5"/>
-    </row>
-    <row r="58" spans="5:25" x14ac:dyDescent="0.25">
-      <c r="E58" s="4"/>
-      <c r="F58" s="18" t="s">
-        <v>152</v>
-      </c>
-      <c r="G58" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="H58" s="18"/>
-      <c r="I58" s="18"/>
-      <c r="J58" s="5"/>
-      <c r="M58" s="6"/>
-      <c r="N58" s="17"/>
-      <c r="O58" s="17"/>
-      <c r="P58" s="17"/>
-      <c r="Q58" s="17"/>
-      <c r="R58" s="7"/>
-      <c r="T58" s="4"/>
-      <c r="U58" s="18" t="s">
-        <v>125</v>
-      </c>
-      <c r="V58" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="W58" s="18">
-        <v>3</v>
-      </c>
-      <c r="X58" s="18"/>
-      <c r="Y58" s="5"/>
-    </row>
-    <row r="59" spans="5:25" x14ac:dyDescent="0.25">
-      <c r="E59" s="4"/>
-      <c r="F59" s="18" t="s">
-        <v>153</v>
-      </c>
-      <c r="G59" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="H59" s="18"/>
-      <c r="I59" s="18"/>
-      <c r="J59" s="5"/>
-      <c r="M59" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="N59" s="10"/>
       <c r="O59" s="10"/>
       <c r="P59" s="10"/>
       <c r="Q59" s="10"/>
-      <c r="R59" s="11"/>
-      <c r="T59" s="4"/>
-      <c r="U59" s="18" t="s">
+      <c r="R59" s="10"/>
+      <c r="S59" s="11"/>
+      <c r="T59" s="27"/>
+      <c r="V59" s="4"/>
+      <c r="W59" t="s">
         <v>141</v>
       </c>
-      <c r="V59" s="21" t="s">
+      <c r="X59" t="s">
         <v>58</v>
       </c>
-      <c r="W59" s="21">
-        <v>4</v>
-      </c>
-      <c r="X59" s="18"/>
-      <c r="Y59" s="5"/>
-    </row>
-    <row r="60" spans="5:25" x14ac:dyDescent="0.25">
+      <c r="Y59">
+        <v>4</v>
+      </c>
+      <c r="Z59" s="28">
+        <v>272</v>
+      </c>
+      <c r="AA59" s="5">
+        <f>SUM(Y59,Z59)</f>
+        <v>276</v>
+      </c>
+    </row>
+    <row r="60" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E60" s="4"/>
-      <c r="F60" s="18" t="s">
+      <c r="F60" t="s">
+        <v>153</v>
+      </c>
+      <c r="G60" t="s">
+        <v>26</v>
+      </c>
+      <c r="J60" s="5"/>
+      <c r="K60" s="27"/>
+      <c r="N60" s="4"/>
+      <c r="O60" t="s">
+        <v>146</v>
+      </c>
+      <c r="P60" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q60">
+        <v>4</v>
+      </c>
+      <c r="S60" s="5"/>
+      <c r="T60" s="27"/>
+      <c r="V60" s="6"/>
+      <c r="W60" s="16"/>
+      <c r="X60" s="16"/>
+      <c r="Y60" s="16"/>
+      <c r="Z60" s="16"/>
+      <c r="AA60" s="7"/>
+    </row>
+    <row r="61" spans="5:27" x14ac:dyDescent="0.25">
+      <c r="E61" s="4"/>
+      <c r="F61" t="s">
         <v>154</v>
       </c>
-      <c r="G60" s="18" t="s">
+      <c r="G61" t="s">
+        <v>8</v>
+      </c>
+      <c r="H61">
+        <v>8</v>
+      </c>
+      <c r="J61" s="5"/>
+      <c r="K61" s="27"/>
+      <c r="N61" s="4"/>
+      <c r="O61" t="s">
+        <v>147</v>
+      </c>
+      <c r="P61" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q61">
+        <v>4</v>
+      </c>
+      <c r="S61" s="5"/>
+      <c r="T61" s="27"/>
+    </row>
+    <row r="62" spans="5:27" x14ac:dyDescent="0.25">
+      <c r="E62" s="4"/>
+      <c r="F62" t="s">
+        <v>155</v>
+      </c>
+      <c r="G62" t="s">
+        <v>10</v>
+      </c>
+      <c r="H62">
+        <v>1</v>
+      </c>
+      <c r="J62" s="5"/>
+      <c r="K62" s="27"/>
+      <c r="N62" s="4"/>
+      <c r="O62" t="s">
+        <v>148</v>
+      </c>
+      <c r="P62" t="s">
         <v>26</v>
       </c>
-      <c r="H60" s="18"/>
-      <c r="I60" s="18"/>
-      <c r="J60" s="5"/>
-      <c r="M60" s="4"/>
-      <c r="N60" s="18" t="s">
-        <v>147</v>
-      </c>
-      <c r="O60" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="P60" s="18">
-        <v>4</v>
-      </c>
-      <c r="Q60" s="18"/>
-      <c r="R60" s="5"/>
-      <c r="T60" s="6"/>
-      <c r="U60" s="17"/>
-      <c r="V60" s="17"/>
-      <c r="W60" s="17"/>
-      <c r="X60" s="17"/>
-      <c r="Y60" s="7"/>
-    </row>
-    <row r="61" spans="5:25" x14ac:dyDescent="0.25">
-      <c r="E61" s="4"/>
-      <c r="F61" s="18" t="s">
-        <v>155</v>
-      </c>
-      <c r="G61" s="18" t="s">
+      <c r="S62" s="5"/>
+      <c r="T62" s="27"/>
+    </row>
+    <row r="63" spans="5:27" x14ac:dyDescent="0.25">
+      <c r="E63" s="4"/>
+      <c r="F63" t="s">
+        <v>156</v>
+      </c>
+      <c r="G63" t="s">
+        <v>10</v>
+      </c>
+      <c r="H63">
+        <v>1</v>
+      </c>
+      <c r="J63" s="5"/>
+      <c r="K63" s="27"/>
+      <c r="N63" s="4"/>
+      <c r="O63" t="s">
+        <v>149</v>
+      </c>
+      <c r="P63" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q63">
         <v>8</v>
       </c>
-      <c r="H61" s="18">
+      <c r="S63" s="5"/>
+      <c r="T63" s="27"/>
+    </row>
+    <row r="64" spans="5:27" x14ac:dyDescent="0.25">
+      <c r="E64" s="4"/>
+      <c r="F64" t="s">
+        <v>66</v>
+      </c>
+      <c r="G64" t="s">
+        <v>12</v>
+      </c>
+      <c r="H64">
         <v>8</v>
       </c>
-      <c r="I61" s="18"/>
-      <c r="J61" s="5"/>
-      <c r="M61" s="4"/>
-      <c r="N61" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="O61" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="P61" s="18">
-        <v>4</v>
-      </c>
-      <c r="Q61" s="18"/>
-      <c r="R61" s="5"/>
-    </row>
-    <row r="62" spans="5:25" x14ac:dyDescent="0.25">
-      <c r="E62" s="4"/>
-      <c r="F62" s="18" t="s">
-        <v>156</v>
-      </c>
-      <c r="G62" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="H62" s="18">
-        <v>1</v>
-      </c>
-      <c r="I62" s="18"/>
-      <c r="J62" s="5"/>
-      <c r="M62" s="4"/>
-      <c r="N62" s="18" t="s">
-        <v>149</v>
-      </c>
-      <c r="O62" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="P62" s="18"/>
-      <c r="Q62" s="18"/>
-      <c r="R62" s="5"/>
-    </row>
-    <row r="63" spans="5:25" x14ac:dyDescent="0.25">
-      <c r="E63" s="4"/>
-      <c r="F63" s="18" t="s">
+      <c r="J64" s="5"/>
+      <c r="K64" s="27"/>
+      <c r="N64" s="6"/>
+      <c r="O64" s="16"/>
+      <c r="P64" s="16"/>
+      <c r="Q64" s="16"/>
+      <c r="R64" s="16"/>
+      <c r="S64" s="7"/>
+      <c r="T64" s="27"/>
+    </row>
+    <row r="65" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E65" s="4"/>
+      <c r="J65" s="5"/>
+      <c r="K65" s="27"/>
+    </row>
+    <row r="66" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E66" s="2" t="s">
         <v>157</v>
-      </c>
-      <c r="G63" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="H63" s="18">
-        <v>1</v>
-      </c>
-      <c r="I63" s="18"/>
-      <c r="J63" s="5"/>
-      <c r="M63" s="4"/>
-      <c r="N63" s="18" t="s">
-        <v>150</v>
-      </c>
-      <c r="O63" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="P63" s="18">
-        <v>8</v>
-      </c>
-      <c r="Q63" s="18"/>
-      <c r="R63" s="5"/>
-    </row>
-    <row r="64" spans="5:25" x14ac:dyDescent="0.25">
-      <c r="E64" s="4"/>
-      <c r="F64" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="G64" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="H64" s="21">
-        <v>8</v>
-      </c>
-      <c r="I64" s="18"/>
-      <c r="J64" s="5"/>
-      <c r="M64" s="6"/>
-      <c r="N64" s="17"/>
-      <c r="O64" s="17"/>
-      <c r="P64" s="17"/>
-      <c r="Q64" s="17"/>
-      <c r="R64" s="7"/>
-    </row>
-    <row r="65" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E65" s="4"/>
-      <c r="F65" s="18"/>
-      <c r="G65" s="18"/>
-      <c r="H65" s="18"/>
-      <c r="I65" s="18"/>
-      <c r="J65" s="5"/>
-    </row>
-    <row r="66" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E66" s="2" t="s">
-        <v>158</v>
       </c>
       <c r="F66" s="10"/>
       <c r="G66" s="10"/>
       <c r="H66" s="10"/>
       <c r="I66" s="10"/>
       <c r="J66" s="11"/>
-    </row>
-    <row r="67" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K66" s="27"/>
+    </row>
+    <row r="67" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E67" s="4"/>
-      <c r="F67" s="18" t="s">
-        <v>152</v>
-      </c>
-      <c r="G67" s="18" t="s">
+      <c r="F67" t="s">
+        <v>151</v>
+      </c>
+      <c r="G67" t="s">
         <v>26</v>
       </c>
-      <c r="H67" s="18"/>
-      <c r="I67" s="18"/>
       <c r="J67" s="5"/>
-    </row>
-    <row r="68" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K67" s="27"/>
+    </row>
+    <row r="68" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E68" s="4"/>
-      <c r="F68" s="18" t="s">
+      <c r="F68" t="s">
+        <v>158</v>
+      </c>
+      <c r="G68" t="s">
+        <v>8</v>
+      </c>
+      <c r="H68">
+        <v>8</v>
+      </c>
+      <c r="J68" s="5"/>
+      <c r="K68" s="27"/>
+    </row>
+    <row r="69" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E69" s="4"/>
+      <c r="F69" t="s">
         <v>159</v>
       </c>
-      <c r="G68" s="18" t="s">
+      <c r="G69" t="s">
         <v>8</v>
       </c>
-      <c r="H68" s="18">
+      <c r="H69">
         <v>8</v>
       </c>
-      <c r="I68" s="18"/>
-      <c r="J68" s="5"/>
-    </row>
-    <row r="69" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E69" s="4"/>
-      <c r="F69" s="18" t="s">
-        <v>160</v>
-      </c>
-      <c r="G69" s="18" t="s">
+      <c r="J69" s="5"/>
+      <c r="K69" s="27"/>
+    </row>
+    <row r="70" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E70" s="4"/>
+      <c r="F70" t="s">
+        <v>66</v>
+      </c>
+      <c r="G70" t="s">
+        <v>12</v>
+      </c>
+      <c r="H70">
         <v>8</v>
       </c>
-      <c r="H69" s="18">
-        <v>8</v>
-      </c>
-      <c r="I69" s="18"/>
-      <c r="J69" s="5"/>
-    </row>
-    <row r="70" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E70" s="4"/>
-      <c r="F70" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="G70" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="H70" s="18">
-        <v>8</v>
-      </c>
-      <c r="I70" s="18"/>
       <c r="J70" s="5"/>
-    </row>
-    <row r="71" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K70" s="27"/>
+    </row>
+    <row r="71" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E71" s="6"/>
-      <c r="F71" s="17"/>
-      <c r="G71" s="17"/>
-      <c r="H71" s="17"/>
-      <c r="I71" s="17"/>
+      <c r="F71" s="16"/>
+      <c r="G71" s="16"/>
+      <c r="H71" s="16"/>
+      <c r="I71" s="16"/>
       <c r="J71" s="7"/>
+      <c r="K71" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
fix: mr + filegroups
</commit_message>
<xml_diff>
--- a/filegroup_support/Filegroups_support.xlsx
+++ b/filegroup_support/Filegroups_support.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\wwi\filegroup_support\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC9E18ED-66B4-4460-B2B7-531CFFC0E054}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE4327CD-18EE-4D1C-ABE2-1F40193B387C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{060E0144-75C7-4C12-B4D9-C7F9369402C2}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="178">
   <si>
     <t>Data types</t>
   </si>
@@ -238,9 +238,6 @@
   </si>
   <si>
     <t>PreferredName</t>
-  </si>
-  <si>
-    <t>Bills</t>
   </si>
   <si>
     <t>Discount</t>
@@ -452,9 +449,6 @@
     <t>LineTotal</t>
   </si>
   <si>
-    <t>Profit</t>
-  </si>
-  <si>
     <t>Transport</t>
   </si>
   <si>
@@ -518,18 +512,6 @@
     <t>Total Init(Bytes)</t>
   </si>
   <si>
-    <t>Sum</t>
-  </si>
-  <si>
-    <t>Average</t>
-  </si>
-  <si>
-    <t>Running Total</t>
-  </si>
-  <si>
-    <t>Count</t>
-  </si>
-  <si>
     <t>DEFINE THE ERROR MSGs</t>
   </si>
   <si>
@@ -542,24 +524,12 @@
     <t>SystemControl Schema</t>
   </si>
   <si>
-    <t>FK(Table PK)</t>
-  </si>
-  <si>
     <t>ColumnInfo</t>
   </si>
   <si>
-    <t>FK (Column PK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FK (Column PK </t>
-  </si>
-  <si>
     <t>Estimation</t>
   </si>
   <si>
-    <t>FK (Table PK)</t>
-  </si>
-  <si>
     <t>Contacts</t>
   </si>
   <si>
@@ -591,6 +561,24 @@
   </si>
   <si>
     <t>FK (SellingPackage)</t>
+  </si>
+  <si>
+    <t>SchemaName</t>
+  </si>
+  <si>
+    <t>TableName</t>
+  </si>
+  <si>
+    <t>ColumnName</t>
+  </si>
+  <si>
+    <t>varhcar</t>
+  </si>
+  <si>
+    <t>Para view</t>
+  </si>
+  <si>
+    <t>Para Transport</t>
   </si>
 </sst>
 </file>
@@ -813,7 +801,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -839,25 +827,19 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="3" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1167,7 +1149,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1175,10 +1157,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61C2F128-56C4-4A17-AFB6-7B93C606ECA2}">
-  <dimension ref="A1:AA81"/>
+  <dimension ref="A1:AA80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E16" workbookViewId="0">
-      <selection activeCell="Q30" sqref="Q30"/>
+    <sheetView tabSelected="1" topLeftCell="J34" workbookViewId="0">
+      <selection activeCell="U63" sqref="U63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1218,35 +1200,35 @@
       <c r="E1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="24" t="s">
+      <c r="G1" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="24" t="s">
-        <v>90</v>
+      <c r="H1" s="23" t="s">
+        <v>89</v>
       </c>
       <c r="I1" s="12" t="s">
         <v>37</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="K1" s="1"/>
       <c r="N1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="O1" s="24" t="s">
+      <c r="O1" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="P1" s="24" t="s">
+      <c r="P1" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="Q1" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="R1" s="24" t="s">
+      <c r="Q1" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="R1" s="23" t="s">
         <v>37</v>
       </c>
       <c r="S1" s="9" t="s">
@@ -1256,14 +1238,14 @@
       <c r="V1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="W1" s="24" t="s">
+      <c r="W1" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="X1" s="24" t="s">
+      <c r="X1" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="Y1" s="24" t="s">
-        <v>90</v>
+      <c r="Y1" s="23" t="s">
+        <v>89</v>
       </c>
       <c r="Z1" s="12" t="s">
         <v>37</v>
@@ -1280,7 +1262,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F2" t="s">
         <v>21</v>
@@ -1305,9 +1287,8 @@
       <c r="Q2">
         <v>4</v>
       </c>
-      <c r="R2" s="27"/>
       <c r="V2" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="W2" t="s">
         <v>21</v>
@@ -1354,7 +1335,7 @@
       </c>
       <c r="V3" s="4"/>
       <c r="W3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="X3" t="s">
         <v>11</v>
@@ -1397,7 +1378,7 @@
       </c>
       <c r="V4" s="4"/>
       <c r="W4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="X4" t="s">
         <v>11</v>
@@ -1433,7 +1414,7 @@
       <c r="S5" s="7"/>
       <c r="V5" s="4"/>
       <c r="W5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="X5" t="s">
         <v>25</v>
@@ -1482,7 +1463,7 @@
       <c r="Z6" s="19">
         <v>0</v>
       </c>
-      <c r="AA6" s="28">
+      <c r="AA6" s="26">
         <f>PRODUCT(Y6:Z6)</f>
         <v>0</v>
       </c>
@@ -1497,7 +1478,7 @@
       <c r="E7" s="4"/>
       <c r="F7" s="16"/>
       <c r="G7" s="16"/>
-      <c r="H7" s="26">
+      <c r="H7" s="25">
         <f>SUM(H2:H6)</f>
         <v>22</v>
       </c>
@@ -1569,7 +1550,7 @@
         <v>28</v>
       </c>
       <c r="V8" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="W8" t="s">
         <v>21</v>
@@ -1621,7 +1602,7 @@
         <v>23</v>
       </c>
       <c r="G10" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="H10">
         <v>8</v>
@@ -1666,7 +1647,7 @@
         <v>17</v>
       </c>
       <c r="P11" s="22" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="Q11">
         <f>3+2</f>
@@ -1675,7 +1656,7 @@
       <c r="S11" s="5"/>
       <c r="V11" s="4"/>
       <c r="W11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="X11" t="s">
         <v>10</v>
@@ -1706,13 +1687,13 @@
       <c r="R12">
         <v>3</v>
       </c>
-      <c r="S12" s="25">
+      <c r="S12" s="24">
         <f>PRODUCT(R12,Q12)</f>
         <v>18</v>
       </c>
       <c r="V12" s="4"/>
       <c r="W12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="X12" t="s">
         <v>58</v>
@@ -1741,7 +1722,6 @@
       <c r="H13">
         <v>4</v>
       </c>
-      <c r="I13" s="27"/>
       <c r="N13" s="17"/>
       <c r="O13" s="16"/>
       <c r="P13" s="16"/>
@@ -1751,7 +1731,7 @@
       <c r="T13" s="1"/>
       <c r="V13" s="4"/>
       <c r="W13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="X13" t="s">
         <v>58</v>
@@ -1763,7 +1743,7 @@
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B14" s="5">
         <v>4</v>
@@ -1794,7 +1774,7 @@
       </c>
       <c r="V14" s="4"/>
       <c r="W14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="X14" t="s">
         <v>58</v>
@@ -1806,7 +1786,7 @@
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B15" s="5">
         <v>8</v>
@@ -1848,10 +1828,10 @@
       </c>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A16" s="29" t="s">
-        <v>163</v>
-      </c>
-      <c r="B16" s="30">
+      <c r="A16" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="B16" s="7">
         <v>16</v>
       </c>
       <c r="E16" s="4"/>
@@ -1898,13 +1878,13 @@
       <c r="Q17" s="16"/>
       <c r="R17" s="16"/>
       <c r="S17" s="7"/>
-      <c r="V17" s="32" t="s">
-        <v>171</v>
-      </c>
-      <c r="W17" s="35" t="s">
+      <c r="V17" s="28" t="s">
+        <v>161</v>
+      </c>
+      <c r="W17" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="X17" s="35" t="s">
+      <c r="X17" s="10" t="s">
         <v>26</v>
       </c>
       <c r="Y17" s="10">
@@ -1943,16 +1923,15 @@
         <v>3</v>
       </c>
       <c r="V18" s="4"/>
-      <c r="W18" s="33" t="s">
-        <v>172</v>
-      </c>
-      <c r="X18" s="33" t="s">
+      <c r="W18" t="s">
+        <v>162</v>
+      </c>
+      <c r="X18" t="s">
         <v>10</v>
       </c>
-      <c r="Y18" s="27">
+      <c r="Y18">
         <v>1</v>
       </c>
-      <c r="Z18" s="27"/>
       <c r="AA18" s="5"/>
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.25">
@@ -1983,16 +1962,15 @@
       </c>
       <c r="S19" s="5"/>
       <c r="V19" s="4"/>
-      <c r="W19" s="33" t="s">
-        <v>173</v>
-      </c>
-      <c r="X19" s="27" t="s">
+      <c r="W19" t="s">
+        <v>163</v>
+      </c>
+      <c r="X19" t="s">
         <v>58</v>
       </c>
-      <c r="Y19" s="27">
-        <v>4</v>
-      </c>
-      <c r="Z19" s="27"/>
+      <c r="Y19">
+        <v>4</v>
+      </c>
       <c r="AA19" s="5"/>
     </row>
     <row r="20" spans="1:27" x14ac:dyDescent="0.25">
@@ -2022,14 +2000,14 @@
       <c r="V20" s="6"/>
       <c r="W20" s="16"/>
       <c r="X20" s="16"/>
-      <c r="Y20" s="26">
+      <c r="Y20" s="25">
         <f>SUM(Y17:Y19)</f>
         <v>20</v>
       </c>
       <c r="Z20" s="16">
         <v>402</v>
       </c>
-      <c r="AA20" s="37">
+      <c r="AA20" s="30">
         <f>PRODUCT(Y20:Z20)</f>
         <v>8040</v>
       </c>
@@ -2053,7 +2031,6 @@
       <c r="H21">
         <v>1</v>
       </c>
-      <c r="I21" s="27"/>
       <c r="N21" s="4"/>
       <c r="O21" t="s">
         <v>66</v>
@@ -2066,10 +2043,10 @@
       </c>
       <c r="S21" s="5"/>
       <c r="V21" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="W21" t="s">
         <v>105</v>
-      </c>
-      <c r="W21" t="s">
-        <v>106</v>
       </c>
       <c r="X21" t="s">
         <v>58</v>
@@ -2077,7 +2054,6 @@
       <c r="Y21">
         <v>4</v>
       </c>
-      <c r="Z21" s="27"/>
       <c r="AA21" s="11"/>
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.25">
@@ -2113,7 +2089,7 @@
       </c>
       <c r="V22" s="4"/>
       <c r="W22" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="X22" t="s">
         <v>26</v>
@@ -2150,7 +2126,7 @@
       <c r="S23" s="7"/>
       <c r="V23" s="4"/>
       <c r="W23" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="X23" t="s">
         <v>26</v>
@@ -2259,13 +2235,13 @@
         <v>99</v>
       </c>
       <c r="V26" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="W26" t="s">
         <v>21</v>
       </c>
       <c r="X26" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="Y26">
         <v>16</v>
@@ -2274,11 +2250,11 @@
       <c r="AA26" s="3"/>
     </row>
     <row r="27" spans="1:27" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="23" t="s">
-        <v>91</v>
-      </c>
-      <c r="B27" s="23"/>
-      <c r="C27" s="23"/>
+      <c r="A27" s="31" t="s">
+        <v>90</v>
+      </c>
+      <c r="B27" s="31"/>
+      <c r="C27" s="31"/>
       <c r="E27" s="4"/>
       <c r="F27" t="s">
         <v>44</v>
@@ -2299,7 +2275,7 @@
       <c r="T27" s="1"/>
       <c r="V27" s="4"/>
       <c r="W27" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="X27" t="s">
         <v>12</v>
@@ -2311,7 +2287,7 @@
     </row>
     <row r="28" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E28" s="4"/>
       <c r="H28" s="1">
@@ -2340,7 +2316,7 @@
       <c r="S28" s="5"/>
       <c r="V28" s="4"/>
       <c r="W28" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="X28" t="s">
         <v>58</v>
@@ -2351,9 +2327,9 @@
       <c r="AA28" s="5"/>
     </row>
     <row r="29" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A29" s="31"/>
-      <c r="B29" s="31"/>
-      <c r="C29" s="31"/>
+      <c r="A29" s="27"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
       <c r="E29" s="6"/>
       <c r="F29" s="16"/>
       <c r="G29" s="16"/>
@@ -2369,7 +2345,7 @@
       <c r="Q29" s="19"/>
       <c r="S29" s="5"/>
       <c r="V29" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Y29" s="1">
         <f>SUM(Y26:Y28)</f>
@@ -2378,7 +2354,7 @@
       <c r="Z29" s="19">
         <v>0</v>
       </c>
-      <c r="AA29" s="28">
+      <c r="AA29" s="26">
         <f>PRODUCT(Y29:Z29)</f>
         <v>0</v>
       </c>
@@ -2391,7 +2367,7 @@
         <v>21</v>
       </c>
       <c r="G30" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H30">
         <v>2</v>
@@ -2431,10 +2407,10 @@
       <c r="S31" s="18"/>
       <c r="T31" s="1"/>
       <c r="V31" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="W31" t="s">
         <v>116</v>
-      </c>
-      <c r="W31" t="s">
-        <v>117</v>
       </c>
       <c r="X31" t="s">
         <v>58</v>
@@ -2457,7 +2433,7 @@
       </c>
       <c r="J32" s="5"/>
       <c r="N32" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="O32" t="s">
         <v>21</v>
@@ -2472,7 +2448,7 @@
       <c r="T32" s="1"/>
       <c r="V32" s="4"/>
       <c r="W32" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="X32" t="s">
         <v>58</v>
@@ -2497,7 +2473,7 @@
       </c>
       <c r="N33" s="4"/>
       <c r="O33" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="P33" t="s">
         <v>58</v>
@@ -2508,7 +2484,7 @@
       <c r="S33" s="5"/>
       <c r="V33" s="4"/>
       <c r="W33" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="X33" t="s">
         <v>58</v>
@@ -2527,7 +2503,7 @@
       <c r="J34" s="7"/>
       <c r="N34" s="4"/>
       <c r="O34" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="P34" t="s">
         <v>26</v>
@@ -2536,7 +2512,7 @@
       <c r="S34" s="5"/>
       <c r="V34" s="4"/>
       <c r="W34" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="X34" t="s">
         <v>58</v>
@@ -2548,13 +2524,13 @@
     </row>
     <row r="35" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E35" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F35" t="s">
         <v>94</v>
       </c>
-      <c r="F35" t="s">
-        <v>95</v>
-      </c>
       <c r="G35" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H35">
         <v>2</v>
@@ -2562,7 +2538,7 @@
       <c r="I35" s="10"/>
       <c r="N35" s="4"/>
       <c r="O35" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="P35" t="s">
         <v>58</v>
@@ -2573,7 +2549,7 @@
       <c r="S35" s="5"/>
       <c r="V35" s="13"/>
       <c r="W35" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="X35" t="s">
         <v>11</v>
@@ -2586,7 +2562,7 @@
     <row r="36" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E36" s="4"/>
       <c r="F36" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G36" t="s">
         <v>7</v>
@@ -2597,7 +2573,7 @@
       <c r="J36" s="5"/>
       <c r="N36" s="13"/>
       <c r="O36" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="P36" t="s">
         <v>58</v>
@@ -2606,15 +2582,17 @@
         <v>4</v>
       </c>
       <c r="S36" s="5"/>
-      <c r="V36" s="4"/>
-      <c r="W36" t="s">
-        <v>122</v>
-      </c>
-      <c r="X36" t="s">
+      <c r="V36" s="22" t="s">
+        <v>177</v>
+      </c>
+      <c r="W36" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="X36" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="Y36">
-        <v>3</v>
+      <c r="Y36" s="22">
+        <v>0</v>
       </c>
       <c r="AA36" s="5"/>
     </row>
@@ -2633,7 +2611,7 @@
       </c>
       <c r="N37" s="4"/>
       <c r="O37" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="P37" t="s">
         <v>58</v>
@@ -2644,7 +2622,7 @@
       <c r="S37" s="5"/>
       <c r="V37" s="4"/>
       <c r="W37" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="X37" t="s">
         <v>58</v>
@@ -2663,10 +2641,10 @@
       <c r="J38" s="7"/>
       <c r="N38" s="4"/>
       <c r="O38" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="P38" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="Q38">
         <v>8</v>
@@ -2674,7 +2652,7 @@
       <c r="S38" s="5"/>
       <c r="V38" s="4"/>
       <c r="W38" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="X38" t="s">
         <v>61</v>
@@ -2700,24 +2678,26 @@
       <c r="I39" s="10"/>
       <c r="N39" s="4"/>
       <c r="O39" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="P39" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="Q39">
         <v>8</v>
       </c>
       <c r="S39" s="5"/>
-      <c r="V39" s="4"/>
-      <c r="W39" t="s">
-        <v>82</v>
-      </c>
-      <c r="X39" t="s">
+      <c r="V39" s="22" t="s">
+        <v>176</v>
+      </c>
+      <c r="W39" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="X39" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="Y39">
-        <v>1</v>
+      <c r="Y39" s="22">
+        <v>0</v>
       </c>
       <c r="AA39" s="5"/>
     </row>
@@ -2735,7 +2715,7 @@
       <c r="J40" s="5"/>
       <c r="N40" s="4"/>
       <c r="O40" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="P40" t="s">
         <v>67</v>
@@ -2744,15 +2724,17 @@
         <v>5</v>
       </c>
       <c r="S40" s="5"/>
-      <c r="V40" s="4"/>
-      <c r="W40" t="s">
-        <v>124</v>
-      </c>
-      <c r="X40" t="s">
+      <c r="V40" s="22" t="s">
+        <v>176</v>
+      </c>
+      <c r="W40" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="X40" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="Y40">
-        <v>4</v>
+      <c r="Y40" s="22">
+        <v>0</v>
       </c>
       <c r="AA40" s="5"/>
     </row>
@@ -2770,24 +2752,26 @@
       <c r="J41" s="5"/>
       <c r="N41" s="4"/>
       <c r="O41" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="P41" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Q41">
         <v>5</v>
       </c>
       <c r="S41" s="5"/>
-      <c r="V41" s="4"/>
-      <c r="W41" t="s">
-        <v>125</v>
-      </c>
-      <c r="X41" t="s">
-        <v>152</v>
-      </c>
-      <c r="Y41">
-        <v>8</v>
+      <c r="V41" s="22" t="s">
+        <v>176</v>
+      </c>
+      <c r="W41" s="22" t="s">
+        <v>124</v>
+      </c>
+      <c r="X41" s="22" t="s">
+        <v>150</v>
+      </c>
+      <c r="Y41" s="22">
+        <v>0</v>
       </c>
       <c r="AA41" s="5"/>
     </row>
@@ -2797,7 +2781,7 @@
         <v>50</v>
       </c>
       <c r="G42" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H42">
         <v>2</v>
@@ -2805,7 +2789,7 @@
       <c r="J42" s="5"/>
       <c r="N42" s="4"/>
       <c r="O42" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="P42" t="s">
         <v>10</v>
@@ -2817,14 +2801,14 @@
       <c r="V42" s="4"/>
       <c r="Y42" s="1">
         <f>SUM(Y31:Y41)</f>
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="Z42">
         <v>70510</v>
       </c>
       <c r="AA42" s="21">
         <f>PRODUCT(Y42,Z42)</f>
-        <v>2961420</v>
+        <v>1833260</v>
       </c>
     </row>
     <row r="43" spans="5:27" x14ac:dyDescent="0.25">
@@ -2841,7 +2825,7 @@
       <c r="J43" s="5"/>
       <c r="N43" s="4"/>
       <c r="O43" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="P43" t="s">
         <v>7</v>
@@ -2863,7 +2847,7 @@
         <f>SUM(H39:H43)</f>
         <v>15</v>
       </c>
-      <c r="I44" s="27">
+      <c r="I44">
         <f>37940</f>
         <v>37940</v>
       </c>
@@ -2873,7 +2857,7 @@
       </c>
       <c r="N44" s="4"/>
       <c r="O44" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="P44" t="s">
         <v>58</v>
@@ -2883,10 +2867,10 @@
       </c>
       <c r="S44" s="5"/>
       <c r="V44" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="W44" t="s">
         <v>126</v>
-      </c>
-      <c r="W44" t="s">
-        <v>127</v>
       </c>
       <c r="X44" t="s">
         <v>58</v>
@@ -2904,7 +2888,7 @@
       <c r="J45" s="7"/>
       <c r="N45" s="4"/>
       <c r="O45" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="P45" t="s">
         <v>6</v>
@@ -2915,7 +2899,7 @@
       <c r="S45" s="5"/>
       <c r="V45" s="4"/>
       <c r="W45" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="X45" t="s">
         <v>58</v>
@@ -2938,10 +2922,9 @@
       <c r="H46">
         <v>4</v>
       </c>
-      <c r="I46" s="27"/>
       <c r="N46" s="4"/>
       <c r="O46" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="P46" t="s">
         <v>6</v>
@@ -2952,7 +2935,7 @@
       <c r="S46" s="5"/>
       <c r="V46" s="4"/>
       <c r="W46" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="X46" t="s">
         <v>6</v>
@@ -2986,10 +2969,10 @@
       </c>
       <c r="V47" s="4"/>
       <c r="W47" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="X47" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="Y47">
         <v>8</v>
@@ -3005,7 +2988,7 @@
       <c r="J48" s="7"/>
       <c r="N48" s="6"/>
       <c r="O48" s="16" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="P48" s="16"/>
       <c r="Q48" s="16"/>
@@ -3013,10 +2996,10 @@
       <c r="S48" s="7"/>
       <c r="V48" s="4"/>
       <c r="W48" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="X48" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="Y48">
         <v>8</v>
@@ -3025,7 +3008,7 @@
     </row>
     <row r="49" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E49" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F49" t="s">
         <v>21</v>
@@ -3038,12 +3021,12 @@
       </c>
       <c r="I49" s="10"/>
       <c r="N49" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="O49" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="O49" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="P49" s="35" t="s">
+      <c r="P49" s="10" t="s">
         <v>58</v>
       </c>
       <c r="Q49" s="10">
@@ -3054,7 +3037,7 @@
       <c r="T49" s="1"/>
       <c r="V49" s="4"/>
       <c r="W49" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="X49" t="s">
         <v>67</v>
@@ -3067,7 +3050,7 @@
     <row r="50" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E50" s="4"/>
       <c r="F50" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G50" t="s">
         <v>26</v>
@@ -3077,24 +3060,23 @@
       </c>
       <c r="J50" s="5"/>
       <c r="N50" s="4"/>
-      <c r="O50" s="33" t="s">
-        <v>174</v>
-      </c>
-      <c r="P50" s="33" t="s">
-        <v>175</v>
-      </c>
-      <c r="Q50" s="27">
+      <c r="O50" t="s">
+        <v>164</v>
+      </c>
+      <c r="P50" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q50">
         <f>25+2</f>
         <v>27</v>
       </c>
-      <c r="R50" s="27"/>
       <c r="S50" s="5"/>
       <c r="V50" s="4"/>
       <c r="W50" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="X50" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="Y50">
         <v>8</v>
@@ -3104,7 +3086,7 @@
     <row r="51" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E51" s="4"/>
       <c r="F51" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G51" t="s">
         <v>58</v>
@@ -3116,20 +3098,20 @@
       <c r="N51" s="6"/>
       <c r="O51" s="16"/>
       <c r="P51" s="16"/>
-      <c r="Q51" s="26">
+      <c r="Q51" s="25">
         <f>SUM(Q49:Q50)</f>
         <v>31</v>
       </c>
       <c r="R51">
         <v>44</v>
       </c>
-      <c r="S51" s="36">
+      <c r="S51" s="29">
         <f>PRODUCT(Q51:R51)</f>
         <v>1364</v>
       </c>
       <c r="V51" s="4"/>
       <c r="W51" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X51" t="s">
         <v>58</v>
@@ -3142,7 +3124,7 @@
     <row r="52" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E52" s="4"/>
       <c r="F52" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G52" t="s">
         <v>58</v>
@@ -3152,9 +3134,9 @@
       </c>
       <c r="J52" s="5"/>
       <c r="N52" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="O52" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="O52" s="10" t="s">
         <v>21</v>
       </c>
       <c r="P52" s="10" t="s">
@@ -3167,10 +3149,10 @@
       <c r="S52" s="11"/>
       <c r="V52" s="4"/>
       <c r="W52" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="X52" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="Y52">
         <v>8</v>
@@ -3191,16 +3173,15 @@
         <v>5628</v>
       </c>
       <c r="N53" s="4"/>
-      <c r="O53" s="33" t="s">
+      <c r="O53" t="s">
         <v>17</v>
       </c>
-      <c r="P53" s="27" t="s">
-        <v>177</v>
+      <c r="P53" t="s">
+        <v>167</v>
       </c>
       <c r="Q53">
         <v>6</v>
       </c>
-      <c r="R53" s="27"/>
       <c r="S53" s="5"/>
       <c r="V53" s="4"/>
       <c r="Y53" s="1">
@@ -3225,14 +3206,14 @@
       <c r="N54" s="6"/>
       <c r="O54" s="16"/>
       <c r="P54" s="16"/>
-      <c r="Q54" s="26">
+      <c r="Q54" s="25">
         <f>SUM(Q52:Q53)</f>
         <v>10</v>
       </c>
       <c r="R54">
         <v>2</v>
       </c>
-      <c r="S54" s="36">
+      <c r="S54" s="29">
         <f>PRODUCT(Q54:R54)</f>
         <v>20</v>
       </c>
@@ -3245,12 +3226,12 @@
     </row>
     <row r="55" spans="5:27" x14ac:dyDescent="0.25">
       <c r="N55" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="O55" s="35" t="s">
+        <v>168</v>
+      </c>
+      <c r="O55" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="P55" s="35" t="s">
+      <c r="P55" s="10" t="s">
         <v>6</v>
       </c>
       <c r="Q55" s="10">
@@ -3258,11 +3239,11 @@
       </c>
       <c r="R55" s="10"/>
       <c r="S55" s="11"/>
-      <c r="V55" s="2" t="s">
-        <v>71</v>
+      <c r="V55" s="13" t="s">
+        <v>134</v>
       </c>
       <c r="W55" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="X55" t="s">
         <v>58</v>
@@ -3270,71 +3251,81 @@
       <c r="Y55">
         <v>4</v>
       </c>
-      <c r="Z55" s="27"/>
     </row>
     <row r="56" spans="5:27" x14ac:dyDescent="0.25">
       <c r="N56" s="4"/>
-      <c r="O56" s="33" t="s">
+      <c r="O56" t="s">
         <v>17</v>
       </c>
-      <c r="P56" s="33" t="s">
-        <v>175</v>
-      </c>
-      <c r="Q56" s="27">
+      <c r="P56" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q56">
         <v>25</v>
       </c>
-      <c r="R56" s="27"/>
       <c r="S56" s="5"/>
       <c r="V56" s="4"/>
       <c r="W56" t="s">
         <v>135</v>
       </c>
       <c r="X56" t="s">
-        <v>154</v>
+        <v>11</v>
       </c>
       <c r="Y56">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="AA56" s="5"/>
     </row>
     <row r="57" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E57" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="N57" s="6"/>
       <c r="O57" s="16"/>
       <c r="P57" s="16"/>
-      <c r="Q57" s="26">
+      <c r="Q57" s="25">
         <f>SUM(Q55:Q56)</f>
         <v>27</v>
       </c>
       <c r="R57" s="16">
         <v>5</v>
       </c>
-      <c r="S57" s="36">
+      <c r="S57" s="29">
         <f>PRODUCT(Q57:R57)</f>
         <v>135</v>
       </c>
-      <c r="T57" s="27"/>
       <c r="V57" s="4"/>
-      <c r="Y57" s="1">
-        <f>SUM(Y55:Y56)</f>
-        <v>12</v>
-      </c>
-      <c r="Z57">
-        <v>70510</v>
-      </c>
-      <c r="AA57" s="21">
-        <f>PRODUCT(Y57,Z57)</f>
-        <v>846120</v>
-      </c>
+      <c r="W57" t="s">
+        <v>121</v>
+      </c>
+      <c r="X57" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y57">
+        <v>3</v>
+      </c>
+      <c r="AA57" s="5"/>
     </row>
     <row r="58" spans="5:27" x14ac:dyDescent="0.25">
+      <c r="E58" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="F58" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="G58" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="H58" s="10">
+        <v>8</v>
+      </c>
+      <c r="I58" s="10"/>
+      <c r="J58" s="11"/>
       <c r="N58" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="O58" t="s">
         <v>113</v>
-      </c>
-      <c r="O58" t="s">
-        <v>114</v>
       </c>
       <c r="P58" t="s">
         <v>7</v>
@@ -3342,31 +3333,33 @@
       <c r="Q58">
         <v>1</v>
       </c>
-      <c r="V58" s="6"/>
-      <c r="W58" s="16"/>
-      <c r="X58" s="16"/>
-      <c r="Y58" s="16"/>
-      <c r="Z58" s="16"/>
-      <c r="AA58" s="7"/>
+      <c r="V58" s="4"/>
+      <c r="W58" t="s">
+        <v>136</v>
+      </c>
+      <c r="X58" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y58">
+        <v>4</v>
+      </c>
+      <c r="AA58" s="5"/>
     </row>
     <row r="59" spans="5:27" x14ac:dyDescent="0.25">
-      <c r="E59" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F59" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="G59" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="H59" s="10">
-        <v>4</v>
-      </c>
-      <c r="I59" s="10"/>
-      <c r="J59" s="11"/>
+      <c r="E59" s="4"/>
+      <c r="F59" t="s">
+        <v>173</v>
+      </c>
+      <c r="G59" t="s">
+        <v>175</v>
+      </c>
+      <c r="H59">
+        <v>8</v>
+      </c>
+      <c r="J59" s="5"/>
       <c r="N59" s="4"/>
       <c r="O59" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="P59" t="s">
         <v>58</v>
@@ -3375,31 +3368,27 @@
         <v>4</v>
       </c>
       <c r="S59" s="5"/>
-      <c r="V59" s="13" t="s">
-        <v>136</v>
-      </c>
-      <c r="W59" t="s">
-        <v>128</v>
-      </c>
-      <c r="X59" t="s">
-        <v>58</v>
-      </c>
-      <c r="Y59">
-        <v>4</v>
+      <c r="V59" s="4"/>
+      <c r="Y59" s="1">
+        <f>SUM(Y55:Y58)</f>
+        <v>14</v>
+      </c>
+      <c r="Z59">
+        <v>272</v>
+      </c>
+      <c r="AA59" s="21">
+        <f>PRODUCT(Y59:Z59)</f>
+        <v>3808</v>
       </c>
     </row>
     <row r="60" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E60" s="4"/>
-      <c r="F60" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="G60" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="H60" s="27">
-        <v>0</v>
-      </c>
-      <c r="I60" s="27"/>
+      <c r="F60" t="s">
+        <v>174</v>
+      </c>
+      <c r="H60">
+        <v>8</v>
+      </c>
       <c r="J60" s="5"/>
       <c r="N60" s="4"/>
       <c r="Q60" s="1">
@@ -3413,129 +3402,82 @@
         <f>PRODUCT(Q60,R60)</f>
         <v>2540</v>
       </c>
-      <c r="V60" s="4"/>
-      <c r="W60" t="s">
-        <v>137</v>
-      </c>
-      <c r="X60" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y60">
-        <v>3</v>
-      </c>
-      <c r="AA60" s="5"/>
+      <c r="V60" s="6"/>
+      <c r="W60" s="16"/>
+      <c r="X60" s="16"/>
+      <c r="Y60" s="16"/>
+      <c r="Z60" s="16"/>
+      <c r="AA60" s="7"/>
     </row>
     <row r="61" spans="5:27" x14ac:dyDescent="0.25">
-      <c r="E61" s="6"/>
-      <c r="F61" s="16"/>
-      <c r="G61" s="16"/>
-      <c r="H61" s="26">
-        <f>SUM(H59:H60)</f>
-        <v>4</v>
-      </c>
-      <c r="I61">
-        <v>32</v>
-      </c>
-      <c r="J61" s="37">
-        <f>PRODUCT(H61:I61)</f>
-        <v>128</v>
-      </c>
+      <c r="E61" s="4"/>
+      <c r="F61" t="s">
+        <v>145</v>
+      </c>
+      <c r="G61" t="s">
+        <v>8</v>
+      </c>
+      <c r="H61">
+        <v>8</v>
+      </c>
+      <c r="J61" s="5"/>
       <c r="N61" s="6"/>
       <c r="O61" s="16"/>
       <c r="P61" s="16"/>
       <c r="Q61" s="16"/>
       <c r="R61" s="16"/>
       <c r="S61" s="7"/>
-      <c r="V61" s="4"/>
-      <c r="W61" t="s">
-        <v>122</v>
-      </c>
-      <c r="X61" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y61">
-        <v>3</v>
-      </c>
-      <c r="AA61" s="5"/>
     </row>
     <row r="62" spans="5:27" x14ac:dyDescent="0.25">
-      <c r="E62" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F62" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="G62" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="H62" s="10">
-        <v>4</v>
-      </c>
-      <c r="I62" s="10"/>
-      <c r="J62" s="11"/>
+      <c r="E62" s="4"/>
+      <c r="F62" t="s">
+        <v>146</v>
+      </c>
+      <c r="G62" t="s">
+        <v>10</v>
+      </c>
+      <c r="H62">
+        <v>1</v>
+      </c>
+      <c r="J62" s="5"/>
       <c r="N62" s="10"/>
       <c r="O62" s="10"/>
       <c r="P62" s="10"/>
       <c r="Q62" s="10"/>
       <c r="R62" s="10"/>
       <c r="S62" s="10"/>
-      <c r="V62" s="4"/>
-      <c r="W62" t="s">
-        <v>138</v>
-      </c>
-      <c r="X62" t="s">
-        <v>58</v>
-      </c>
-      <c r="Y62">
-        <v>4</v>
-      </c>
-      <c r="AA62" s="5"/>
     </row>
     <row r="63" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E63" s="4"/>
-      <c r="F63" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="G63" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="H63" s="27"/>
-      <c r="I63" s="27"/>
+      <c r="F63" t="s">
+        <v>147</v>
+      </c>
+      <c r="G63" t="s">
+        <v>10</v>
+      </c>
+      <c r="H63">
+        <v>1</v>
+      </c>
       <c r="J63" s="5"/>
       <c r="O63" s="16"/>
       <c r="P63" s="16"/>
       <c r="Q63" s="16"/>
-      <c r="V63" s="4"/>
-      <c r="Y63" s="1">
-        <f>SUM(Y59:Y62)</f>
-        <v>14</v>
-      </c>
-      <c r="Z63">
-        <v>272</v>
-      </c>
-      <c r="AA63" s="21">
-        <f>PRODUCT(Y63:Z63)</f>
-        <v>3808</v>
-      </c>
     </row>
     <row r="64" spans="5:27" x14ac:dyDescent="0.25">
-      <c r="E64" s="4"/>
-      <c r="F64" s="27" t="s">
-        <v>165</v>
-      </c>
-      <c r="G64" s="27" t="s">
-        <v>58</v>
-      </c>
-      <c r="H64" s="27">
-        <v>4</v>
-      </c>
-      <c r="I64" s="27"/>
-      <c r="J64" s="5"/>
+      <c r="F64" t="s">
+        <v>66</v>
+      </c>
+      <c r="G64" t="s">
+        <v>12</v>
+      </c>
+      <c r="H64">
+        <v>8</v>
+      </c>
       <c r="N64" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="O64" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="P64" t="s">
         <v>58</v>
@@ -3545,52 +3487,46 @@
       </c>
       <c r="R64" s="10"/>
       <c r="S64" s="11"/>
-      <c r="V64" s="6"/>
-      <c r="W64" s="16"/>
-      <c r="X64" s="16"/>
-      <c r="Y64" s="16"/>
-      <c r="Z64" s="16"/>
-      <c r="AA64" s="7"/>
     </row>
     <row r="65" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E65" s="6"/>
+      <c r="E65" s="17"/>
       <c r="F65" s="16"/>
       <c r="G65" s="16"/>
-      <c r="H65" s="26">
-        <f>SUM(H62:H64)</f>
-        <v>8</v>
+      <c r="H65" s="25">
+        <f>SUM(H58:H64)</f>
+        <v>42</v>
       </c>
       <c r="I65">
         <v>114</v>
       </c>
-      <c r="J65" s="37">
-        <f>PRODUCT(H65:I65)</f>
-        <v>912</v>
+      <c r="J65" s="30">
+        <f>PRODUCT(H65,I65)</f>
+        <v>4788</v>
       </c>
       <c r="N65" s="4"/>
       <c r="O65" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="P65" t="s">
         <v>26</v>
       </c>
       <c r="Q65" s="19" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="S65" s="5"/>
     </row>
     <row r="66" spans="5:19" x14ac:dyDescent="0.25">
       <c r="E66" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="F66" s="35" t="s">
-        <v>167</v>
-      </c>
-      <c r="G66" s="35" t="s">
-        <v>58</v>
-      </c>
-      <c r="H66" s="10">
-        <v>4</v>
+        <v>160</v>
+      </c>
+      <c r="F66" t="s">
+        <v>173</v>
+      </c>
+      <c r="G66" t="s">
+        <v>26</v>
+      </c>
+      <c r="H66">
+        <v>8</v>
       </c>
       <c r="I66" s="10"/>
       <c r="J66" s="11"/>
@@ -3607,16 +3543,15 @@
     </row>
     <row r="67" spans="5:19" x14ac:dyDescent="0.25">
       <c r="E67" s="4"/>
-      <c r="F67" s="33" t="s">
-        <v>168</v>
-      </c>
-      <c r="G67" s="33" t="s">
-        <v>58</v>
-      </c>
-      <c r="H67" s="27">
-        <v>4</v>
-      </c>
-      <c r="I67" s="27"/>
+      <c r="F67" t="s">
+        <v>148</v>
+      </c>
+      <c r="G67" t="s">
+        <v>8</v>
+      </c>
+      <c r="H67">
+        <v>8</v>
+      </c>
       <c r="J67" s="5"/>
       <c r="N67" s="6"/>
       <c r="O67" s="16"/>
@@ -3627,22 +3562,21 @@
     </row>
     <row r="68" spans="5:19" x14ac:dyDescent="0.25">
       <c r="E68" s="4"/>
-      <c r="F68" s="27" t="s">
-        <v>147</v>
-      </c>
-      <c r="G68" s="27" t="s">
+      <c r="F68" t="s">
+        <v>149</v>
+      </c>
+      <c r="G68" t="s">
         <v>8</v>
       </c>
-      <c r="H68" s="27">
+      <c r="H68">
         <v>8</v>
       </c>
-      <c r="I68" s="27"/>
       <c r="J68" s="5"/>
       <c r="N68" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="O68" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="P68" t="s">
         <v>58</v>
@@ -3655,20 +3589,19 @@
     </row>
     <row r="69" spans="5:19" x14ac:dyDescent="0.25">
       <c r="E69" s="4"/>
-      <c r="F69" s="27" t="s">
-        <v>148</v>
-      </c>
-      <c r="G69" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="H69" s="27">
-        <v>1</v>
-      </c>
-      <c r="I69" s="27"/>
+      <c r="F69" t="s">
+        <v>66</v>
+      </c>
+      <c r="G69" t="s">
+        <v>12</v>
+      </c>
+      <c r="H69">
+        <v>8</v>
+      </c>
       <c r="J69" s="5"/>
       <c r="N69" s="4"/>
       <c r="O69" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="P69" t="s">
         <v>58</v>
@@ -3679,21 +3612,23 @@
       <c r="S69" s="5"/>
     </row>
     <row r="70" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E70" s="4"/>
-      <c r="F70" s="27" t="s">
-        <v>149</v>
-      </c>
-      <c r="G70" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="H70" s="27">
-        <v>1</v>
-      </c>
-      <c r="I70" s="27"/>
-      <c r="J70" s="5"/>
+      <c r="E70" s="6"/>
+      <c r="F70" s="16"/>
+      <c r="G70" s="16"/>
+      <c r="H70" s="16">
+        <f>SUM(H66:H69)</f>
+        <v>32</v>
+      </c>
+      <c r="I70" s="16">
+        <v>32</v>
+      </c>
+      <c r="J70" s="30">
+        <f>PRODUCT(H70:I70)</f>
+        <v>1024</v>
+      </c>
       <c r="N70" s="4"/>
       <c r="O70" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="P70" t="s">
         <v>26</v>
@@ -3702,21 +3637,9 @@
       <c r="S70" s="5"/>
     </row>
     <row r="71" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E71" s="4"/>
-      <c r="F71" s="27" t="s">
-        <v>66</v>
-      </c>
-      <c r="G71" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="H71" s="27">
-        <v>8</v>
-      </c>
-      <c r="I71" s="27"/>
-      <c r="J71" s="5"/>
       <c r="N71" s="4"/>
       <c r="O71" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="P71" t="s">
         <v>12</v>
@@ -3727,20 +3650,6 @@
       <c r="S71" s="5"/>
     </row>
     <row r="72" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E72" s="17"/>
-      <c r="F72" s="16"/>
-      <c r="G72" s="16"/>
-      <c r="H72" s="26">
-        <f>SUM(H66:H71)</f>
-        <v>26</v>
-      </c>
-      <c r="I72">
-        <v>114</v>
-      </c>
-      <c r="J72" s="37">
-        <f>PRODUCT(H72,I72)</f>
-        <v>2964</v>
-      </c>
       <c r="N72" s="4"/>
       <c r="Q72" s="1">
         <f>SUM(Q68:Q71)</f>
@@ -3753,20 +3662,6 @@
       </c>
     </row>
     <row r="73" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E73" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="F73" t="s">
-        <v>170</v>
-      </c>
-      <c r="G73" t="s">
-        <v>58</v>
-      </c>
-      <c r="H73">
-        <v>4</v>
-      </c>
-      <c r="I73" s="10"/>
-      <c r="J73" s="11"/>
       <c r="N73" s="6"/>
       <c r="O73" s="16"/>
       <c r="P73" s="16"/>
@@ -3774,90 +3669,8 @@
       <c r="R73" s="16"/>
       <c r="S73" s="7"/>
     </row>
-    <row r="74" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E74" s="4"/>
-      <c r="F74" t="s">
-        <v>150</v>
-      </c>
-      <c r="G74" t="s">
-        <v>8</v>
-      </c>
-      <c r="H74">
-        <v>8</v>
-      </c>
-      <c r="J74" s="5"/>
-    </row>
-    <row r="75" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E75" s="4"/>
-      <c r="F75" t="s">
-        <v>151</v>
-      </c>
-      <c r="G75" t="s">
-        <v>8</v>
-      </c>
-      <c r="H75">
-        <v>8</v>
-      </c>
-      <c r="J75" s="5"/>
-    </row>
-    <row r="76" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E76" s="4"/>
-      <c r="F76" t="s">
-        <v>66</v>
-      </c>
-      <c r="G76" t="s">
-        <v>12</v>
-      </c>
-      <c r="H76">
-        <v>8</v>
-      </c>
-      <c r="J76" s="5"/>
-    </row>
-    <row r="77" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E77" s="6"/>
-      <c r="F77" s="16"/>
-      <c r="G77" s="16"/>
-      <c r="H77" s="16">
-        <f>SUM(H73:H76)</f>
-        <v>28</v>
-      </c>
-      <c r="I77" s="16">
-        <v>32</v>
-      </c>
-      <c r="J77" s="37">
-        <f>PRODUCT(H77:I77)</f>
-        <v>896</v>
-      </c>
-    </row>
-    <row r="78" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E78" s="10"/>
-      <c r="F78" s="10"/>
-      <c r="G78" s="10"/>
-      <c r="H78" s="10"/>
-      <c r="I78" s="10"/>
-      <c r="J78" s="10"/>
-    </row>
-    <row r="79" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E79" s="27"/>
-      <c r="F79" s="27"/>
-      <c r="G79" s="27"/>
-      <c r="H79" s="27"/>
-      <c r="I79" s="27"/>
-      <c r="J79" s="27"/>
-    </row>
     <row r="80" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E80" s="27"/>
-      <c r="F80" s="27"/>
-      <c r="G80" s="27"/>
-      <c r="H80" s="34"/>
-    </row>
-    <row r="81" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E81" s="27"/>
-      <c r="F81" s="27"/>
-      <c r="G81" s="27"/>
-      <c r="H81" s="27"/>
-      <c r="I81" s="27"/>
-      <c r="J81" s="27"/>
+      <c r="H80" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
fix: products queries + tables size
</commit_message>
<xml_diff>
--- a/filegroup_support/Filegroups_support.xlsx
+++ b/filegroup_support/Filegroups_support.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\wwi\filegroup_support\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE4327CD-18EE-4D1C-ABE2-1F40193B387C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DE6A7EC-E005-4DD3-AFB4-B1925DF8080F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{060E0144-75C7-4C12-B4D9-C7F9369402C2}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="179">
   <si>
     <t>Data types</t>
   </si>
@@ -579,6 +579,9 @@
   </si>
   <si>
     <t>Para Transport</t>
+  </si>
+  <si>
+    <t>FK (TaxRate)</t>
   </si>
 </sst>
 </file>
@@ -824,7 +827,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
@@ -840,6 +842,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1159,8 +1162,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61C2F128-56C4-4A17-AFB6-7B93C606ECA2}">
   <dimension ref="A1:AA80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J34" workbookViewId="0">
-      <selection activeCell="U63" sqref="U63"/>
+    <sheetView tabSelected="1" topLeftCell="C55" workbookViewId="0">
+      <selection activeCell="Q35" sqref="Q35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1200,13 +1203,13 @@
       <c r="E1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="23" t="s">
+      <c r="G1" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="22" t="s">
         <v>89</v>
       </c>
       <c r="I1" s="12" t="s">
@@ -1219,16 +1222,16 @@
       <c r="N1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="O1" s="23" t="s">
+      <c r="O1" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="P1" s="23" t="s">
+      <c r="P1" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="Q1" s="23" t="s">
+      <c r="Q1" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="R1" s="23" t="s">
+      <c r="R1" s="22" t="s">
         <v>37</v>
       </c>
       <c r="S1" s="9" t="s">
@@ -1238,13 +1241,13 @@
       <c r="V1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="W1" s="23" t="s">
+      <c r="W1" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="X1" s="23" t="s">
+      <c r="X1" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="Y1" s="23" t="s">
+      <c r="Y1" s="22" t="s">
         <v>89</v>
       </c>
       <c r="Z1" s="12" t="s">
@@ -1372,7 +1375,7 @@
       <c r="R4">
         <v>5</v>
       </c>
-      <c r="S4" s="21">
+      <c r="S4" s="20">
         <f>PRODUCT(Q4,R4)</f>
         <v>70</v>
       </c>
@@ -1451,7 +1454,7 @@
       <c r="R6">
         <v>2</v>
       </c>
-      <c r="S6" s="21">
+      <c r="S6" s="20">
         <f>SUM(S7:S8)</f>
         <v>36</v>
       </c>
@@ -1463,7 +1466,7 @@
       <c r="Z6" s="19">
         <v>0</v>
       </c>
-      <c r="AA6" s="26">
+      <c r="AA6" s="25">
         <f>PRODUCT(Y6:Z6)</f>
         <v>0</v>
       </c>
@@ -1478,14 +1481,14 @@
       <c r="E7" s="4"/>
       <c r="F7" s="16"/>
       <c r="G7" s="16"/>
-      <c r="H7" s="25">
+      <c r="H7" s="24">
         <f>SUM(H2:H6)</f>
         <v>22</v>
       </c>
       <c r="I7">
         <v>19</v>
       </c>
-      <c r="J7" s="21">
+      <c r="J7" s="20">
         <f>PRODUCT(H7,I7)</f>
         <v>418</v>
       </c>
@@ -1638,7 +1641,7 @@
       <c r="I11">
         <v>10</v>
       </c>
-      <c r="J11" s="21">
+      <c r="J11" s="20">
         <f>PRODUCT(H11,I11)</f>
         <v>130</v>
       </c>
@@ -1646,7 +1649,7 @@
       <c r="O11" t="s">
         <v>17</v>
       </c>
-      <c r="P11" s="22" t="s">
+      <c r="P11" s="21" t="s">
         <v>153</v>
       </c>
       <c r="Q11">
@@ -1687,7 +1690,7 @@
       <c r="R12">
         <v>3</v>
       </c>
-      <c r="S12" s="24">
+      <c r="S12" s="23">
         <f>PRODUCT(R12,Q12)</f>
         <v>18</v>
       </c>
@@ -1799,7 +1802,7 @@
       <c r="I15">
         <v>9</v>
       </c>
-      <c r="J15" s="21">
+      <c r="J15" s="20">
         <f>PRODUCT(H15,I15)</f>
         <v>135</v>
       </c>
@@ -1822,7 +1825,7 @@
       <c r="Z15">
         <v>402</v>
       </c>
-      <c r="AA15" s="21">
+      <c r="AA15" s="20">
         <f>PRODUCT(Y15:Z15)</f>
         <v>6834</v>
       </c>
@@ -1847,7 +1850,7 @@
       <c r="R16">
         <v>2</v>
       </c>
-      <c r="S16" s="21">
+      <c r="S16" s="20">
         <f>PRODUCT(Q16,R16)</f>
         <v>16</v>
       </c>
@@ -1878,7 +1881,7 @@
       <c r="Q17" s="16"/>
       <c r="R17" s="16"/>
       <c r="S17" s="7"/>
-      <c r="V17" s="28" t="s">
+      <c r="V17" s="27" t="s">
         <v>161</v>
       </c>
       <c r="W17" s="10" t="s">
@@ -1946,7 +1949,7 @@
       <c r="I19">
         <v>23272</v>
       </c>
-      <c r="J19" s="21">
+      <c r="J19" s="20">
         <f>PRODUCT(H19,I19)</f>
         <v>349080</v>
       </c>
@@ -2000,14 +2003,14 @@
       <c r="V20" s="6"/>
       <c r="W20" s="16"/>
       <c r="X20" s="16"/>
-      <c r="Y20" s="25">
+      <c r="Y20" s="24">
         <f>SUM(Y17:Y19)</f>
         <v>20</v>
       </c>
       <c r="Z20" s="16">
         <v>402</v>
       </c>
-      <c r="AA20" s="30">
+      <c r="AA20" s="29">
         <f>PRODUCT(Y20:Z20)</f>
         <v>8040</v>
       </c>
@@ -2083,7 +2086,7 @@
       <c r="R22">
         <v>2</v>
       </c>
-      <c r="S22" s="21">
+      <c r="S22" s="20">
         <f>PRODUCT(Q22*R22)</f>
         <v>38</v>
       </c>
@@ -2114,7 +2117,7 @@
       <c r="I23">
         <v>1</v>
       </c>
-      <c r="J23" s="21">
+      <c r="J23" s="20">
         <f>PRODUCT(H23,I23,)</f>
         <v>16</v>
       </c>
@@ -2168,7 +2171,7 @@
       <c r="Z24">
         <v>402</v>
       </c>
-      <c r="AA24" s="21">
+      <c r="AA24" s="20">
         <f>PRODUCT(Y24,Z24)</f>
         <v>17286</v>
       </c>
@@ -2230,7 +2233,7 @@
       <c r="R26">
         <v>11</v>
       </c>
-      <c r="S26" s="21">
+      <c r="S26" s="20">
         <f>PRODUCT(Q26,R26)</f>
         <v>99</v>
       </c>
@@ -2250,11 +2253,11 @@
       <c r="AA26" s="3"/>
     </row>
     <row r="27" spans="1:27" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="30" t="s">
         <v>90</v>
       </c>
-      <c r="B27" s="31"/>
-      <c r="C27" s="31"/>
+      <c r="B27" s="30"/>
+      <c r="C27" s="30"/>
       <c r="E27" s="4"/>
       <c r="F27" t="s">
         <v>44</v>
@@ -2297,7 +2300,7 @@
       <c r="I28">
         <v>1</v>
       </c>
-      <c r="J28" s="21">
+      <c r="J28" s="20">
         <f>PRODUCT(H28,I28)</f>
         <v>17</v>
       </c>
@@ -2327,9 +2330,9 @@
       <c r="AA28" s="5"/>
     </row>
     <row r="29" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A29" s="27"/>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
+      <c r="A29" s="26"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
       <c r="E29" s="6"/>
       <c r="F29" s="16"/>
       <c r="G29" s="16"/>
@@ -2342,7 +2345,10 @@
       <c r="P29" t="s">
         <v>26</v>
       </c>
-      <c r="Q29" s="19"/>
+      <c r="Q29">
+        <f>21+2</f>
+        <v>23</v>
+      </c>
       <c r="S29" s="5"/>
       <c r="V29" s="4" t="s">
         <v>109</v>
@@ -2354,7 +2360,7 @@
       <c r="Z29" s="19">
         <v>0</v>
       </c>
-      <c r="AA29" s="26">
+      <c r="AA29" s="25">
         <f>PRODUCT(Y29:Z29)</f>
         <v>0</v>
       </c>
@@ -2374,10 +2380,17 @@
       </c>
       <c r="I30" s="10"/>
       <c r="N30" s="4"/>
-      <c r="Q30" s="19"/>
-      <c r="R30" s="20"/>
-      <c r="S30" s="5">
-        <v>0</v>
+      <c r="Q30">
+        <f>SUM(Q28:Q29)</f>
+        <v>27</v>
+      </c>
+      <c r="R30" s="31">
+        <f>65+4</f>
+        <v>69</v>
+      </c>
+      <c r="S30" s="20">
+        <f>PRODUCT(Q30,R30)</f>
+        <v>1863</v>
       </c>
       <c r="V30" s="17"/>
       <c r="W30" s="16"/>
@@ -2467,7 +2480,7 @@
       <c r="I33">
         <v>53</v>
       </c>
-      <c r="J33" s="21">
+      <c r="J33" s="20">
         <f>PRODUCT(H33,I33)</f>
         <v>848</v>
       </c>
@@ -2508,7 +2521,10 @@
       <c r="P34" t="s">
         <v>26</v>
       </c>
-      <c r="Q34" s="19"/>
+      <c r="Q34">
+        <f>22+2</f>
+        <v>24</v>
+      </c>
       <c r="S34" s="5"/>
       <c r="V34" s="4"/>
       <c r="W34" t="s">
@@ -2582,16 +2598,16 @@
         <v>4</v>
       </c>
       <c r="S36" s="5"/>
-      <c r="V36" s="22" t="s">
+      <c r="V36" s="21" t="s">
         <v>177</v>
       </c>
-      <c r="W36" s="22" t="s">
+      <c r="W36" s="21" t="s">
         <v>121</v>
       </c>
-      <c r="X36" s="22" t="s">
+      <c r="X36" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="Y36" s="22">
+      <c r="Y36" s="21">
         <v>0</v>
       </c>
       <c r="AA36" s="5"/>
@@ -2605,7 +2621,7 @@
       <c r="I37">
         <v>53</v>
       </c>
-      <c r="J37" s="21">
+      <c r="J37" s="20">
         <f>PRODUCT(H37,I37)</f>
         <v>159</v>
       </c>
@@ -2687,16 +2703,16 @@
         <v>8</v>
       </c>
       <c r="S39" s="5"/>
-      <c r="V39" s="22" t="s">
+      <c r="V39" s="21" t="s">
         <v>176</v>
       </c>
-      <c r="W39" s="22" t="s">
+      <c r="W39" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="X39" s="22" t="s">
+      <c r="X39" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="Y39" s="22">
+      <c r="Y39" s="21">
         <v>0</v>
       </c>
       <c r="AA39" s="5"/>
@@ -2724,16 +2740,16 @@
         <v>5</v>
       </c>
       <c r="S40" s="5"/>
-      <c r="V40" s="22" t="s">
+      <c r="V40" s="21" t="s">
         <v>176</v>
       </c>
-      <c r="W40" s="22" t="s">
+      <c r="W40" s="21" t="s">
         <v>123</v>
       </c>
-      <c r="X40" s="22" t="s">
+      <c r="X40" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="Y40" s="22">
+      <c r="Y40" s="21">
         <v>0</v>
       </c>
       <c r="AA40" s="5"/>
@@ -2761,16 +2777,16 @@
         <v>5</v>
       </c>
       <c r="S41" s="5"/>
-      <c r="V41" s="22" t="s">
+      <c r="V41" s="21" t="s">
         <v>176</v>
       </c>
-      <c r="W41" s="22" t="s">
+      <c r="W41" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="X41" s="22" t="s">
+      <c r="X41" s="21" t="s">
         <v>150</v>
       </c>
-      <c r="Y41" s="22">
+      <c r="Y41" s="21">
         <v>0</v>
       </c>
       <c r="AA41" s="5"/>
@@ -2806,7 +2822,7 @@
       <c r="Z42">
         <v>70510</v>
       </c>
-      <c r="AA42" s="21">
+      <c r="AA42" s="20">
         <f>PRODUCT(Y42,Z42)</f>
         <v>1833260</v>
       </c>
@@ -2851,7 +2867,7 @@
         <f>37940</f>
         <v>37940</v>
       </c>
-      <c r="J44" s="21">
+      <c r="J44" s="20">
         <f>PRODUCT(H44,I44)</f>
         <v>569100</v>
       </c>
@@ -2953,19 +2969,22 @@
       <c r="I47">
         <v>317</v>
       </c>
-      <c r="J47" s="21">
+      <c r="J47" s="20">
         <f>PRODUCT(H47,I47)</f>
         <v>1268</v>
       </c>
       <c r="N47" s="4"/>
       <c r="Q47">
         <f>SUM(Q32:Q46)</f>
-        <v>56</v>
-      </c>
-      <c r="R47" s="20"/>
-      <c r="S47" s="15">
+        <v>80</v>
+      </c>
+      <c r="R47">
+        <f>33+65</f>
+        <v>98</v>
+      </c>
+      <c r="S47" s="20">
         <f>PRODUCT(Q47,R47)</f>
-        <v>56</v>
+        <v>7840</v>
       </c>
       <c r="V47" s="4"/>
       <c r="W47" t="s">
@@ -3037,7 +3056,7 @@
       <c r="T49" s="1"/>
       <c r="V49" s="4"/>
       <c r="W49" t="s">
-        <v>79</v>
+        <v>178</v>
       </c>
       <c r="X49" t="s">
         <v>67</v>
@@ -3098,14 +3117,14 @@
       <c r="N51" s="6"/>
       <c r="O51" s="16"/>
       <c r="P51" s="16"/>
-      <c r="Q51" s="25">
+      <c r="Q51" s="24">
         <f>SUM(Q49:Q50)</f>
         <v>31</v>
       </c>
       <c r="R51">
         <v>44</v>
       </c>
-      <c r="S51" s="29">
+      <c r="S51" s="28">
         <f>PRODUCT(Q51:R51)</f>
         <v>1364</v>
       </c>
@@ -3168,7 +3187,7 @@
       <c r="I53">
         <v>402</v>
       </c>
-      <c r="J53" s="21">
+      <c r="J53" s="20">
         <f>PRODUCT(H53,I53)</f>
         <v>5628</v>
       </c>
@@ -3191,7 +3210,7 @@
       <c r="Z53">
         <v>228265</v>
       </c>
-      <c r="AA53" s="21">
+      <c r="AA53" s="20">
         <f>PRODUCT(Y53,Z53)</f>
         <v>11641515</v>
       </c>
@@ -3206,14 +3225,14 @@
       <c r="N54" s="6"/>
       <c r="O54" s="16"/>
       <c r="P54" s="16"/>
-      <c r="Q54" s="25">
+      <c r="Q54" s="24">
         <f>SUM(Q52:Q53)</f>
         <v>10</v>
       </c>
       <c r="R54">
         <v>2</v>
       </c>
-      <c r="S54" s="29">
+      <c r="S54" s="28">
         <f>PRODUCT(Q54:R54)</f>
         <v>20</v>
       </c>
@@ -3283,14 +3302,14 @@
       <c r="N57" s="6"/>
       <c r="O57" s="16"/>
       <c r="P57" s="16"/>
-      <c r="Q57" s="25">
+      <c r="Q57" s="24">
         <f>SUM(Q55:Q56)</f>
         <v>27</v>
       </c>
       <c r="R57" s="16">
         <v>5</v>
       </c>
-      <c r="S57" s="29">
+      <c r="S57" s="28">
         <f>PRODUCT(Q57:R57)</f>
         <v>135</v>
       </c>
@@ -3376,7 +3395,7 @@
       <c r="Z59">
         <v>272</v>
       </c>
-      <c r="AA59" s="21">
+      <c r="AA59" s="20">
         <f>PRODUCT(Y59:Z59)</f>
         <v>3808</v>
       </c>
@@ -3398,7 +3417,7 @@
       <c r="R60">
         <v>508</v>
       </c>
-      <c r="S60" s="21">
+      <c r="S60" s="20">
         <f>PRODUCT(Q60,R60)</f>
         <v>2540</v>
       </c>
@@ -3427,6 +3446,9 @@
       <c r="Q61" s="16"/>
       <c r="R61" s="16"/>
       <c r="S61" s="7"/>
+      <c r="V61" s="1" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="62" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E62" s="4"/>
@@ -3492,14 +3514,14 @@
       <c r="E65" s="17"/>
       <c r="F65" s="16"/>
       <c r="G65" s="16"/>
-      <c r="H65" s="25">
+      <c r="H65" s="24">
         <f>SUM(H58:H64)</f>
         <v>42</v>
       </c>
       <c r="I65">
         <v>114</v>
       </c>
-      <c r="J65" s="30">
+      <c r="J65" s="29">
         <f>PRODUCT(H65,I65)</f>
         <v>4788</v>
       </c>
@@ -3622,7 +3644,7 @@
       <c r="I70" s="16">
         <v>32</v>
       </c>
-      <c r="J70" s="30">
+      <c r="J70" s="29">
         <f>PRODUCT(H70:I70)</f>
         <v>1024</v>
       </c>

</xml_diff>

<commit_message>
fix: filegroup size counts
</commit_message>
<xml_diff>
--- a/filegroup_support/Filegroups_support.xlsx
+++ b/filegroup_support/Filegroups_support.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\wwi\filegroup_support\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DE6A7EC-E005-4DD3-AFB4-B1925DF8080F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A00873C4-6EAC-4499-BF2C-8A68A4415F55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{060E0144-75C7-4C12-B4D9-C7F9369402C2}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{060E0144-75C7-4C12-B4D9-C7F9369402C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="184">
   <si>
     <t>Data types</t>
   </si>
@@ -512,9 +512,6 @@
     <t>Total Init(Bytes)</t>
   </si>
   <si>
-    <t>DEFINE THE ERROR MSGs</t>
-  </si>
-  <si>
     <t xml:space="preserve">uniqueidentifier </t>
   </si>
   <si>
@@ -582,6 +579,24 @@
   </si>
   <si>
     <t>FK (TaxRate)</t>
+  </si>
+  <si>
+    <t>TOTAL SIZE (B)</t>
+  </si>
+  <si>
+    <t>MB</t>
+  </si>
+  <si>
+    <t>Filegroup</t>
+  </si>
+  <si>
+    <t>fg1</t>
+  </si>
+  <si>
+    <t>fg2</t>
+  </si>
+  <si>
+    <t>fg3</t>
   </si>
 </sst>
 </file>
@@ -634,7 +649,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -654,6 +669,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
       </patternFill>
     </fill>
   </fills>
@@ -798,13 +831,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -836,15 +872,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="6" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="6" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="7">
+    <cellStyle name="60% - Accent1" xfId="4" builtinId="32"/>
+    <cellStyle name="60% - Accent2" xfId="5" builtinId="36"/>
+    <cellStyle name="60% - Accent6" xfId="6" builtinId="52"/>
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1162,8 +1215,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61C2F128-56C4-4A17-AFB6-7B93C606ECA2}">
   <dimension ref="A1:AA80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C55" workbookViewId="0">
-      <selection activeCell="Q35" sqref="Q35"/>
+    <sheetView tabSelected="1" topLeftCell="J16" workbookViewId="0">
+      <selection activeCell="Z42" sqref="Z42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1264,7 +1317,7 @@
       <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="35" t="s">
         <v>91</v>
       </c>
       <c r="F2" t="s">
@@ -1278,7 +1331,7 @@
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="11"/>
-      <c r="N2" s="2" t="s">
+      <c r="N2" s="32" t="s">
         <v>54</v>
       </c>
       <c r="O2" t="s">
@@ -1290,7 +1343,7 @@
       <c r="Q2">
         <v>4</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="V2" s="35" t="s">
         <v>71</v>
       </c>
       <c r="W2" t="s">
@@ -1445,7 +1498,7 @@
         <v>2</v>
       </c>
       <c r="J6" s="5"/>
-      <c r="N6" s="2" t="s">
+      <c r="N6" s="35" t="s">
         <v>53</v>
       </c>
       <c r="O6" s="10"/>
@@ -1519,7 +1572,7 @@
       <c r="B8" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="36" t="s">
         <v>19</v>
       </c>
       <c r="F8" t="s">
@@ -1552,7 +1605,7 @@
         <f>PRODUCT(R8,Q8)</f>
         <v>28</v>
       </c>
-      <c r="V8" s="2" t="s">
+      <c r="V8" s="36" t="s">
         <v>99</v>
       </c>
       <c r="W8" t="s">
@@ -1611,7 +1664,7 @@
         <v>8</v>
       </c>
       <c r="J10" s="5"/>
-      <c r="N10" s="13" t="s">
+      <c r="N10" s="33" t="s">
         <v>55</v>
       </c>
       <c r="O10" t="s">
@@ -1713,7 +1766,7 @@
       <c r="B13" s="5">
         <v>5</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="31" t="s">
         <v>36</v>
       </c>
       <c r="F13" t="s">
@@ -1751,7 +1804,6 @@
       <c r="B14" s="5">
         <v>4</v>
       </c>
-      <c r="E14" s="4"/>
       <c r="F14" t="s">
         <v>38</v>
       </c>
@@ -1763,7 +1815,7 @@
         <v>11</v>
       </c>
       <c r="J14" s="5"/>
-      <c r="N14" s="2" t="s">
+      <c r="N14" s="32" t="s">
         <v>60</v>
       </c>
       <c r="O14" t="s">
@@ -1832,7 +1884,7 @@
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B16" s="7">
         <v>16</v>
@@ -1862,7 +1914,7 @@
       <c r="AA16" s="7"/>
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="E17" s="2" t="s">
+      <c r="E17" s="32" t="s">
         <v>40</v>
       </c>
       <c r="F17" t="s">
@@ -1881,8 +1933,8 @@
       <c r="Q17" s="16"/>
       <c r="R17" s="16"/>
       <c r="S17" s="7"/>
-      <c r="V17" s="27" t="s">
-        <v>161</v>
+      <c r="V17" s="35" t="s">
+        <v>160</v>
       </c>
       <c r="W17" s="10" t="s">
         <v>17</v>
@@ -1913,7 +1965,7 @@
         <v>11</v>
       </c>
       <c r="J18" s="5"/>
-      <c r="N18" s="13" t="s">
+      <c r="N18" s="34" t="s">
         <v>62</v>
       </c>
       <c r="O18" t="s">
@@ -1927,7 +1979,7 @@
       </c>
       <c r="V18" s="4"/>
       <c r="W18" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="X18" t="s">
         <v>10</v>
@@ -1966,7 +2018,7 @@
       <c r="S19" s="5"/>
       <c r="V19" s="4"/>
       <c r="W19" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="X19" t="s">
         <v>58</v>
@@ -2010,7 +2062,7 @@
       <c r="Z20" s="16">
         <v>402</v>
       </c>
-      <c r="AA20" s="29">
+      <c r="AA20" s="27">
         <f>PRODUCT(Y20:Z20)</f>
         <v>8040</v>
       </c>
@@ -2022,7 +2074,7 @@
       <c r="B21" s="5">
         <v>5</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="E21" s="32" t="s">
         <v>41</v>
       </c>
       <c r="F21" t="s">
@@ -2045,7 +2097,7 @@
         <v>8</v>
       </c>
       <c r="S21" s="5"/>
-      <c r="V21" s="13" t="s">
+      <c r="V21" s="30" t="s">
         <v>104</v>
       </c>
       <c r="W21" t="s">
@@ -2151,7 +2203,7 @@
       <c r="G24" s="16"/>
       <c r="H24" s="16"/>
       <c r="J24" s="7"/>
-      <c r="N24" s="1" t="s">
+      <c r="N24" s="31" t="s">
         <v>56</v>
       </c>
       <c r="O24" t="s">
@@ -2177,7 +2229,7 @@
       </c>
     </row>
     <row r="25" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E25" s="2" t="s">
+      <c r="E25" s="32" t="s">
         <v>42</v>
       </c>
       <c r="F25" t="s">
@@ -2237,14 +2289,14 @@
         <f>PRODUCT(Q26,R26)</f>
         <v>99</v>
       </c>
-      <c r="V26" s="2" t="s">
+      <c r="V26" s="32" t="s">
         <v>108</v>
       </c>
       <c r="W26" t="s">
         <v>21</v>
       </c>
       <c r="X26" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="Y26">
         <v>16</v>
@@ -2253,11 +2305,11 @@
       <c r="AA26" s="3"/>
     </row>
     <row r="27" spans="1:27" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="30" t="s">
+      <c r="A27" s="28" t="s">
         <v>90</v>
       </c>
-      <c r="B27" s="30"/>
-      <c r="C27" s="30"/>
+      <c r="B27" s="28"/>
+      <c r="C27" s="28"/>
       <c r="E27" s="4"/>
       <c r="F27" t="s">
         <v>44</v>
@@ -2304,7 +2356,7 @@
         <f>PRODUCT(H28,I28)</f>
         <v>17</v>
       </c>
-      <c r="N28" s="13" t="s">
+      <c r="N28" s="34" t="s">
         <v>59</v>
       </c>
       <c r="O28" t="s">
@@ -2366,7 +2418,7 @@
       </c>
     </row>
     <row r="30" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="E30" s="13" t="s">
+      <c r="E30" s="33" t="s">
         <v>39</v>
       </c>
       <c r="F30" t="s">
@@ -2384,7 +2436,7 @@
         <f>SUM(Q28:Q29)</f>
         <v>27</v>
       </c>
-      <c r="R30" s="31">
+      <c r="R30">
         <f>65+4</f>
         <v>69</v>
       </c>
@@ -2419,7 +2471,7 @@
       <c r="R31" s="16"/>
       <c r="S31" s="18"/>
       <c r="T31" s="1"/>
-      <c r="V31" s="13" t="s">
+      <c r="V31" s="30" t="s">
         <v>115</v>
       </c>
       <c r="W31" t="s">
@@ -2433,6 +2485,15 @@
       </c>
     </row>
     <row r="32" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A32" s="37" t="s">
+        <v>180</v>
+      </c>
+      <c r="B32" s="38" t="s">
+        <v>178</v>
+      </c>
+      <c r="C32" s="39" t="s">
+        <v>179</v>
+      </c>
       <c r="E32" s="4"/>
       <c r="F32" t="s">
         <v>43</v>
@@ -2445,7 +2506,7 @@
         <v>4</v>
       </c>
       <c r="J32" s="5"/>
-      <c r="N32" s="2" t="s">
+      <c r="N32" s="35" t="s">
         <v>72</v>
       </c>
       <c r="O32" t="s">
@@ -2471,7 +2532,17 @@
       </c>
       <c r="AA32" s="5"/>
     </row>
-    <row r="33" spans="5:27" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A33" s="33" t="s">
+        <v>181</v>
+      </c>
+      <c r="B33" s="29">
+        <f>SUM(J15,J19,J23,J28,J33,J37,S4,S12,S16,S26,S57,S66,AA63,J44,AA29)</f>
+        <v>919988</v>
+      </c>
+      <c r="C33" s="5">
+        <v>0.92</v>
+      </c>
       <c r="E33" s="4"/>
       <c r="H33" s="1">
         <f>SUM(H30:H32)</f>
@@ -2507,7 +2578,17 @@
       </c>
       <c r="AA33" s="5"/>
     </row>
-    <row r="34" spans="5:27" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A34" s="30" t="s">
+        <v>182</v>
+      </c>
+      <c r="B34" s="29">
+        <f>SUM(J7,J65,J70,S51,S47,S6,AA20,AA24,AA42,S72,AA6)</f>
+        <v>1874072</v>
+      </c>
+      <c r="C34" s="5">
+        <v>1.88</v>
+      </c>
       <c r="E34" s="6"/>
       <c r="F34" s="16"/>
       <c r="G34" s="16"/>
@@ -2538,8 +2619,18 @@
       </c>
       <c r="AA34" s="5"/>
     </row>
-    <row r="35" spans="5:27" x14ac:dyDescent="0.25">
-      <c r="E35" s="2" t="s">
+    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A35" s="34" t="s">
+        <v>183</v>
+      </c>
+      <c r="B35" s="29">
+        <f>SUM(J11,J47,J53,S22,S30,S54,S60,AA59,AA53,AA15)</f>
+        <v>11663644</v>
+      </c>
+      <c r="C35" s="5">
+        <v>11.67</v>
+      </c>
+      <c r="E35" s="32" t="s">
         <v>93</v>
       </c>
       <c r="F35" t="s">
@@ -2554,7 +2645,7 @@
       <c r="I35" s="10"/>
       <c r="N35" s="4"/>
       <c r="O35" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="P35" t="s">
         <v>58</v>
@@ -2575,7 +2666,15 @@
       </c>
       <c r="AA35" s="5"/>
     </row>
-    <row r="36" spans="5:27" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A36" s="6"/>
+      <c r="B36" s="16">
+        <f>SUM(J70,J65,J53,J47,J44,J37,J33,J28,J23,J19,J15,J11,J7,S4,S6,S12,S16,S22,S26,S30,S47,S51,S54,S57,S60,S66,S72,AA59,AA53,AA42,AA24,AA20,AA15,AA6,AA29,AA63)</f>
+        <v>14457704</v>
+      </c>
+      <c r="C36" s="7">
+        <v>14.5</v>
+      </c>
       <c r="E36" s="4"/>
       <c r="F36" t="s">
         <v>95</v>
@@ -2589,7 +2688,7 @@
       <c r="J36" s="5"/>
       <c r="N36" s="13"/>
       <c r="O36" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="P36" t="s">
         <v>58</v>
@@ -2599,7 +2698,7 @@
       </c>
       <c r="S36" s="5"/>
       <c r="V36" s="21" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="W36" s="21" t="s">
         <v>121</v>
@@ -2612,7 +2711,11 @@
       </c>
       <c r="AA36" s="5"/>
     </row>
-    <row r="37" spans="5:27" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <f>SUM(B33:B35)</f>
+        <v>14457704</v>
+      </c>
       <c r="E37" s="4"/>
       <c r="H37" s="1">
         <f>SUM(H35:H36)</f>
@@ -2648,7 +2751,7 @@
       </c>
       <c r="AA37" s="5"/>
     </row>
-    <row r="38" spans="5:27" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
       <c r="E38" s="6"/>
       <c r="F38" s="16"/>
       <c r="G38" s="16"/>
@@ -2678,8 +2781,8 @@
       </c>
       <c r="AA38" s="5"/>
     </row>
-    <row r="39" spans="5:27" x14ac:dyDescent="0.25">
-      <c r="E39" s="13" t="s">
+    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="E39" s="33" t="s">
         <v>47</v>
       </c>
       <c r="F39" t="s">
@@ -2704,7 +2807,7 @@
       </c>
       <c r="S39" s="5"/>
       <c r="V39" s="21" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="W39" s="21" t="s">
         <v>81</v>
@@ -2717,7 +2820,7 @@
       </c>
       <c r="AA39" s="5"/>
     </row>
-    <row r="40" spans="5:27" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
       <c r="E40" s="4"/>
       <c r="F40" t="s">
         <v>48</v>
@@ -2741,7 +2844,7 @@
       </c>
       <c r="S40" s="5"/>
       <c r="V40" s="21" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="W40" s="21" t="s">
         <v>123</v>
@@ -2754,7 +2857,7 @@
       </c>
       <c r="AA40" s="5"/>
     </row>
-    <row r="41" spans="5:27" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
       <c r="E41" s="4"/>
       <c r="F41" t="s">
         <v>49</v>
@@ -2778,7 +2881,7 @@
       </c>
       <c r="S41" s="5"/>
       <c r="V41" s="21" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="W41" s="21" t="s">
         <v>124</v>
@@ -2791,7 +2894,7 @@
       </c>
       <c r="AA41" s="5"/>
     </row>
-    <row r="42" spans="5:27" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
       <c r="E42" s="4"/>
       <c r="F42" t="s">
         <v>50</v>
@@ -2827,7 +2930,7 @@
         <v>1833260</v>
       </c>
     </row>
-    <row r="43" spans="5:27" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
       <c r="E43" s="4"/>
       <c r="F43" t="s">
         <v>51</v>
@@ -2857,7 +2960,7 @@
       <c r="Z43" s="16"/>
       <c r="AA43" s="7"/>
     </row>
-    <row r="44" spans="5:27" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:27" x14ac:dyDescent="0.25">
       <c r="E44" s="4"/>
       <c r="H44" s="1">
         <f>SUM(H39:H43)</f>
@@ -2882,7 +2985,7 @@
         <v>4</v>
       </c>
       <c r="S44" s="5"/>
-      <c r="V44" s="2" t="s">
+      <c r="V44" s="36" t="s">
         <v>125</v>
       </c>
       <c r="W44" t="s">
@@ -2895,7 +2998,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="5:27" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:27" x14ac:dyDescent="0.25">
       <c r="E45" s="6"/>
       <c r="F45" s="16"/>
       <c r="G45" s="16"/>
@@ -2904,7 +3007,7 @@
       <c r="J45" s="7"/>
       <c r="N45" s="4"/>
       <c r="O45" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="P45" t="s">
         <v>6</v>
@@ -2925,8 +3028,8 @@
       </c>
       <c r="AA45" s="5"/>
     </row>
-    <row r="46" spans="5:27" x14ac:dyDescent="0.25">
-      <c r="E46" s="13" t="s">
+    <row r="46" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="E46" s="34" t="s">
         <v>52</v>
       </c>
       <c r="F46" t="s">
@@ -2940,7 +3043,7 @@
       </c>
       <c r="N46" s="4"/>
       <c r="O46" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="P46" t="s">
         <v>6</v>
@@ -2961,7 +3064,7 @@
       </c>
       <c r="AA46" s="5"/>
     </row>
-    <row r="47" spans="5:27" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:27" x14ac:dyDescent="0.25">
       <c r="E47" s="4"/>
       <c r="H47">
         <v>4</v>
@@ -2998,7 +3101,7 @@
       </c>
       <c r="AA47" s="5"/>
     </row>
-    <row r="48" spans="5:27" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:27" x14ac:dyDescent="0.25">
       <c r="E48" s="6"/>
       <c r="F48" s="16"/>
       <c r="G48" s="16"/>
@@ -3026,7 +3129,7 @@
       <c r="AA48" s="5"/>
     </row>
     <row r="49" spans="5:27" x14ac:dyDescent="0.25">
-      <c r="E49" s="2" t="s">
+      <c r="E49" s="36" t="s">
         <v>96</v>
       </c>
       <c r="F49" t="s">
@@ -3039,7 +3142,7 @@
         <v>4</v>
       </c>
       <c r="I49" s="10"/>
-      <c r="N49" s="2" t="s">
+      <c r="N49" s="35" t="s">
         <v>75</v>
       </c>
       <c r="O49" s="10" t="s">
@@ -3056,7 +3159,7 @@
       <c r="T49" s="1"/>
       <c r="V49" s="4"/>
       <c r="W49" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="X49" t="s">
         <v>67</v>
@@ -3080,10 +3183,10 @@
       <c r="J50" s="5"/>
       <c r="N50" s="4"/>
       <c r="O50" t="s">
+        <v>163</v>
+      </c>
+      <c r="P50" t="s">
         <v>164</v>
-      </c>
-      <c r="P50" t="s">
-        <v>165</v>
       </c>
       <c r="Q50">
         <f>25+2</f>
@@ -3124,7 +3227,7 @@
       <c r="R51">
         <v>44</v>
       </c>
-      <c r="S51" s="28">
+      <c r="S51" s="27">
         <f>PRODUCT(Q51:R51)</f>
         <v>1364</v>
       </c>
@@ -3152,7 +3255,7 @@
         <v>4</v>
       </c>
       <c r="J52" s="5"/>
-      <c r="N52" s="2" t="s">
+      <c r="N52" s="36" t="s">
         <v>74</v>
       </c>
       <c r="O52" s="10" t="s">
@@ -3196,7 +3299,7 @@
         <v>17</v>
       </c>
       <c r="P53" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="Q53">
         <v>6</v>
@@ -3232,7 +3335,7 @@
       <c r="R54">
         <v>2</v>
       </c>
-      <c r="S54" s="28">
+      <c r="S54" s="27">
         <f>PRODUCT(Q54:R54)</f>
         <v>20</v>
       </c>
@@ -3244,8 +3347,8 @@
       <c r="AA54" s="7"/>
     </row>
     <row r="55" spans="5:27" x14ac:dyDescent="0.25">
-      <c r="N55" s="2" t="s">
-        <v>168</v>
+      <c r="N55" s="32" t="s">
+        <v>167</v>
       </c>
       <c r="O55" s="10" t="s">
         <v>21</v>
@@ -3258,7 +3361,7 @@
       </c>
       <c r="R55" s="10"/>
       <c r="S55" s="11"/>
-      <c r="V55" s="13" t="s">
+      <c r="V55" s="34" t="s">
         <v>134</v>
       </c>
       <c r="W55" t="s">
@@ -3277,7 +3380,7 @@
         <v>17</v>
       </c>
       <c r="P56" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="Q56">
         <v>25</v>
@@ -3297,7 +3400,7 @@
     </row>
     <row r="57" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E57" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="N57" s="6"/>
       <c r="O57" s="16"/>
@@ -3309,7 +3412,7 @@
       <c r="R57" s="16">
         <v>5</v>
       </c>
-      <c r="S57" s="28">
+      <c r="S57" s="27">
         <f>PRODUCT(Q57:R57)</f>
         <v>135</v>
       </c>
@@ -3326,11 +3429,11 @@
       <c r="AA57" s="5"/>
     </row>
     <row r="58" spans="5:27" x14ac:dyDescent="0.25">
-      <c r="E58" s="2" t="s">
-        <v>159</v>
+      <c r="E58" s="35" t="s">
+        <v>158</v>
       </c>
       <c r="F58" s="10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G58" s="10" t="s">
         <v>26</v>
@@ -3340,7 +3443,7 @@
       </c>
       <c r="I58" s="10"/>
       <c r="J58" s="11"/>
-      <c r="N58" s="2" t="s">
+      <c r="N58" s="36" t="s">
         <v>112</v>
       </c>
       <c r="O58" t="s">
@@ -3367,10 +3470,10 @@
     <row r="59" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E59" s="4"/>
       <c r="F59" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G59" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H59">
         <v>8</v>
@@ -3403,7 +3506,7 @@
     <row r="60" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E60" s="4"/>
       <c r="F60" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H60">
         <v>8</v>
@@ -3446,9 +3549,14 @@
       <c r="Q61" s="16"/>
       <c r="R61" s="16"/>
       <c r="S61" s="7"/>
-      <c r="V61" s="1" t="s">
+      <c r="V61" s="32" t="s">
         <v>79</v>
       </c>
+      <c r="W61" s="10"/>
+      <c r="X61" s="10"/>
+      <c r="Y61" s="10"/>
+      <c r="Z61" s="10"/>
+      <c r="AA61" s="11"/>
     </row>
     <row r="62" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E62" s="4"/>
@@ -3468,6 +3576,18 @@
       <c r="Q62" s="10"/>
       <c r="R62" s="10"/>
       <c r="S62" s="10"/>
+      <c r="V62" s="4"/>
+      <c r="W62" s="29" t="s">
+        <v>177</v>
+      </c>
+      <c r="X62" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y62" s="29">
+        <v>5</v>
+      </c>
+      <c r="Z62" s="29"/>
+      <c r="AA62" s="5"/>
     </row>
     <row r="63" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E63" s="4"/>
@@ -3484,6 +3604,19 @@
       <c r="O63" s="16"/>
       <c r="P63" s="16"/>
       <c r="Q63" s="16"/>
+      <c r="V63" s="6"/>
+      <c r="W63" s="16"/>
+      <c r="X63" s="16"/>
+      <c r="Y63" s="16">
+        <v>5</v>
+      </c>
+      <c r="Z63" s="16">
+        <v>2</v>
+      </c>
+      <c r="AA63" s="27">
+        <f>PRODUCT(Y63,Z63)</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="64" spans="5:27" x14ac:dyDescent="0.25">
       <c r="F64" t="s">
@@ -3495,7 +3628,7 @@
       <c r="H64">
         <v>8</v>
       </c>
-      <c r="N64" s="2" t="s">
+      <c r="N64" s="32" t="s">
         <v>137</v>
       </c>
       <c r="O64" t="s">
@@ -3521,7 +3654,7 @@
       <c r="I65">
         <v>114</v>
       </c>
-      <c r="J65" s="29">
+      <c r="J65" s="27">
         <f>PRODUCT(H65,I65)</f>
         <v>4788</v>
       </c>
@@ -3532,17 +3665,17 @@
       <c r="P65" t="s">
         <v>26</v>
       </c>
-      <c r="Q65" s="19" t="s">
-        <v>155</v>
+      <c r="Q65" s="19">
+        <v>15</v>
       </c>
       <c r="S65" s="5"/>
     </row>
     <row r="66" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E66" s="2" t="s">
-        <v>160</v>
+      <c r="E66" s="35" t="s">
+        <v>159</v>
       </c>
       <c r="F66" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G66" t="s">
         <v>26</v>
@@ -3555,12 +3688,14 @@
       <c r="N66" s="4"/>
       <c r="Q66" s="19">
         <f>SUM(Q64:Q65)</f>
-        <v>4</v>
-      </c>
-      <c r="R66" s="19"/>
+        <v>19</v>
+      </c>
+      <c r="R66" s="19">
+        <v>15</v>
+      </c>
       <c r="S66" s="5">
         <f>PRODUCT(Q66:R66)</f>
-        <v>4</v>
+        <v>285</v>
       </c>
     </row>
     <row r="67" spans="5:19" x14ac:dyDescent="0.25">
@@ -3594,7 +3729,7 @@
         <v>8</v>
       </c>
       <c r="J68" s="5"/>
-      <c r="N68" s="2" t="s">
+      <c r="N68" s="35" t="s">
         <v>140</v>
       </c>
       <c r="O68" t="s">
@@ -3644,7 +3779,7 @@
       <c r="I70" s="16">
         <v>32</v>
       </c>
-      <c r="J70" s="29">
+      <c r="J70" s="27">
         <f>PRODUCT(H70:I70)</f>
         <v>1024</v>
       </c>

</xml_diff>

<commit_message>
fix: transport to fg2
</commit_message>
<xml_diff>
--- a/filegroup_support/Filegroups_support.xlsx
+++ b/filegroup_support/Filegroups_support.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\wwi\filegroup_support\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D3D4A60-C8F9-4577-B269-FD50BB484589}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F15CFB1C-5455-4364-BE53-0585E9FAB017}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{060E0144-75C7-4C12-B4D9-C7F9369402C2}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="183">
   <si>
     <t>Data types</t>
   </si>
@@ -82,9 +82,6 @@
   </si>
   <si>
     <t>Photo</t>
-  </si>
-  <si>
-    <t>Salesman</t>
   </si>
   <si>
     <t>PK, FK</t>
@@ -518,12 +515,6 @@
     <t>uniqueidentifier</t>
   </si>
   <si>
-    <t>SystemControl Schema</t>
-  </si>
-  <si>
-    <t>ColumnInfo</t>
-  </si>
-  <si>
     <t>Estimation</t>
   </si>
   <si>
@@ -597,6 +588,12 @@
   </si>
   <si>
     <t>fg3</t>
+  </si>
+  <si>
+    <t>SystemControl</t>
+  </si>
+  <si>
+    <t>Salesperson</t>
   </si>
 </sst>
 </file>
@@ -840,7 +837,7 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -873,10 +870,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="4" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="5" applyBorder="1"/>
@@ -892,6 +885,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -1215,8 +1211,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61C2F128-56C4-4A17-AFB6-7B93C606ECA2}">
   <dimension ref="A1:AA80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J16" workbookViewId="0">
-      <selection activeCell="Z42" sqref="Z42"/>
+    <sheetView tabSelected="1" topLeftCell="B28" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1251,7 +1247,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>15</v>
@@ -1260,16 +1256,16 @@
         <v>16</v>
       </c>
       <c r="G1" s="22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H1" s="22" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I1" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K1" s="1"/>
       <c r="N1" s="2" t="s">
@@ -1279,16 +1275,16 @@
         <v>16</v>
       </c>
       <c r="P1" s="22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q1" s="22" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="R1" s="22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="S1" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="T1" s="1"/>
       <c r="V1" s="2" t="s">
@@ -1298,16 +1294,16 @@
         <v>16</v>
       </c>
       <c r="X1" s="22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Y1" s="22" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="Z1" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AA1" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
@@ -1317,25 +1313,25 @@
       <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="35" t="s">
-        <v>91</v>
+      <c r="E2" s="33" t="s">
+        <v>90</v>
       </c>
       <c r="F2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H2">
         <v>4</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="11"/>
-      <c r="N2" s="32" t="s">
-        <v>54</v>
+      <c r="N2" s="30" t="s">
+        <v>53</v>
       </c>
       <c r="O2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P2" t="s">
         <v>5</v>
@@ -1343,14 +1339,14 @@
       <c r="Q2">
         <v>4</v>
       </c>
-      <c r="V2" s="35" t="s">
-        <v>71</v>
+      <c r="V2" s="33" t="s">
+        <v>70</v>
       </c>
       <c r="W2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="X2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Y2">
         <v>4</v>
@@ -1367,10 +1363,10 @@
       </c>
       <c r="E3" s="4"/>
       <c r="F3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H3">
         <f>5+2</f>
@@ -1383,7 +1379,7 @@
         <v>17</v>
       </c>
       <c r="P3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Q3">
         <f>(12+16+9+8+5)/5</f>
@@ -1391,7 +1387,7 @@
       </c>
       <c r="V3" s="4"/>
       <c r="W3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="X3" t="s">
         <v>11</v>
@@ -1410,10 +1406,10 @@
       </c>
       <c r="E4" s="4"/>
       <c r="F4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H4">
         <f>6+2</f>
@@ -1434,7 +1430,7 @@
       </c>
       <c r="V4" s="4"/>
       <c r="W4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="X4" t="s">
         <v>11</v>
@@ -1453,7 +1449,7 @@
       </c>
       <c r="E5" s="4"/>
       <c r="F5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G5" t="s">
         <v>10</v>
@@ -1470,10 +1466,10 @@
       <c r="S5" s="7"/>
       <c r="V5" s="4"/>
       <c r="W5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="X5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Y5">
         <v>4</v>
@@ -1492,14 +1488,14 @@
         <v>18</v>
       </c>
       <c r="G6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H6">
         <v>2</v>
       </c>
       <c r="J6" s="5"/>
-      <c r="N6" s="35" t="s">
-        <v>53</v>
+      <c r="N6" s="33" t="s">
+        <v>52</v>
       </c>
       <c r="O6" s="10"/>
       <c r="P6" s="10"/>
@@ -1547,10 +1543,10 @@
       </c>
       <c r="N7" s="4"/>
       <c r="O7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q7">
         <v>4</v>
@@ -1570,13 +1566,13 @@
         <v>9</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="34" t="s">
+        <v>182</v>
+      </c>
+      <c r="F8" t="s">
         <v>19</v>
-      </c>
-      <c r="F8" t="s">
-        <v>20</v>
       </c>
       <c r="G8" t="s">
         <v>5</v>
@@ -1592,7 +1588,7 @@
         <v>17</v>
       </c>
       <c r="P8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Q8">
         <f>12+2</f>
@@ -1605,14 +1601,14 @@
         <f>PRODUCT(R8,Q8)</f>
         <v>28</v>
       </c>
-      <c r="V8" s="36" t="s">
-        <v>99</v>
+      <c r="V8" s="34" t="s">
+        <v>98</v>
       </c>
       <c r="W8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="X8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Y8">
         <v>4</v>
@@ -1628,7 +1624,7 @@
       </c>
       <c r="E9" s="4"/>
       <c r="F9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G9" t="s">
         <v>7</v>
@@ -1655,20 +1651,20 @@
       </c>
       <c r="E10" s="4"/>
       <c r="F10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H10">
         <v>8</v>
       </c>
       <c r="J10" s="5"/>
-      <c r="N10" s="33" t="s">
-        <v>55</v>
+      <c r="N10" s="31" t="s">
+        <v>54</v>
       </c>
       <c r="O10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P10" t="s">
         <v>7</v>
@@ -1703,7 +1699,7 @@
         <v>17</v>
       </c>
       <c r="P11" s="21" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="Q11">
         <f>3+2</f>
@@ -1712,7 +1708,7 @@
       <c r="S11" s="5"/>
       <c r="V11" s="4"/>
       <c r="W11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="X11" t="s">
         <v>10</v>
@@ -1749,10 +1745,10 @@
       </c>
       <c r="V12" s="4"/>
       <c r="W12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="X12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Y12">
         <v>4</v>
@@ -1766,11 +1762,11 @@
       <c r="B13" s="5">
         <v>5</v>
       </c>
-      <c r="E13" s="31" t="s">
-        <v>36</v>
+      <c r="E13" s="29" t="s">
+        <v>35</v>
       </c>
       <c r="F13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G13" t="s">
         <v>5</v>
@@ -1787,10 +1783,10 @@
       <c r="T13" s="1"/>
       <c r="V13" s="4"/>
       <c r="W13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="X13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Y13">
         <v>4</v>
@@ -1799,40 +1795,40 @@
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B14" s="5">
         <v>4</v>
       </c>
       <c r="F14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H14">
         <f xml:space="preserve"> 9+2</f>
         <v>11</v>
       </c>
       <c r="J14" s="5"/>
-      <c r="N14" s="32" t="s">
+      <c r="N14" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="O14" t="s">
+        <v>20</v>
+      </c>
+      <c r="P14" t="s">
         <v>60</v>
-      </c>
-      <c r="O14" t="s">
-        <v>21</v>
-      </c>
-      <c r="P14" t="s">
-        <v>61</v>
       </c>
       <c r="Q14">
         <v>3</v>
       </c>
       <c r="V14" s="4"/>
       <c r="W14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="X14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Y14">
         <v>4</v>
@@ -1841,7 +1837,7 @@
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B15" s="5">
         <v>8</v>
@@ -1863,7 +1859,7 @@
         <v>17</v>
       </c>
       <c r="P15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Q15">
         <v>5</v>
@@ -1884,7 +1880,7 @@
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B16" s="7">
         <v>16</v>
@@ -1914,11 +1910,11 @@
       <c r="AA16" s="7"/>
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="E17" s="32" t="s">
-        <v>40</v>
+      <c r="E17" s="30" t="s">
+        <v>39</v>
       </c>
       <c r="F17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G17" t="s">
         <v>5</v>
@@ -1933,14 +1929,14 @@
       <c r="Q17" s="16"/>
       <c r="R17" s="16"/>
       <c r="S17" s="7"/>
-      <c r="V17" s="35" t="s">
-        <v>160</v>
+      <c r="V17" s="33" t="s">
+        <v>157</v>
       </c>
       <c r="W17" s="10" t="s">
         <v>17</v>
       </c>
       <c r="X17" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Y17" s="10">
         <f>13+2</f>
@@ -1951,35 +1947,35 @@
     </row>
     <row r="18" spans="1:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E18" s="4"/>
       <c r="F18" t="s">
         <v>17</v>
       </c>
       <c r="G18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H18">
         <f>9+2</f>
         <v>11</v>
       </c>
       <c r="J18" s="5"/>
-      <c r="N18" s="34" t="s">
+      <c r="N18" s="32" t="s">
+        <v>61</v>
+      </c>
+      <c r="O18" t="s">
         <v>62</v>
       </c>
-      <c r="O18" t="s">
-        <v>63</v>
-      </c>
       <c r="P18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q18">
         <v>3</v>
       </c>
       <c r="V18" s="4"/>
       <c r="W18" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="X18" t="s">
         <v>10</v>
@@ -1991,7 +1987,7 @@
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E19" s="4"/>
       <c r="H19" s="1">
@@ -2007,10 +2003,10 @@
       </c>
       <c r="N19" s="4"/>
       <c r="O19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q19">
         <v>3</v>
@@ -2018,10 +2014,10 @@
       <c r="S19" s="5"/>
       <c r="V19" s="4"/>
       <c r="W19" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="X19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Y19">
         <v>4</v>
@@ -2030,10 +2026,10 @@
     </row>
     <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="16"/>
@@ -2043,10 +2039,10 @@
       <c r="J20" s="7"/>
       <c r="N20" s="4"/>
       <c r="O20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="P20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="Q20">
         <v>5</v>
@@ -2069,16 +2065,16 @@
     </row>
     <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B21" s="5">
         <v>5</v>
       </c>
-      <c r="E21" s="32" t="s">
-        <v>41</v>
+      <c r="E21" s="30" t="s">
+        <v>40</v>
       </c>
       <c r="F21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G21" t="s">
         <v>7</v>
@@ -2088,7 +2084,7 @@
       </c>
       <c r="N21" s="4"/>
       <c r="O21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="P21" t="s">
         <v>12</v>
@@ -2097,14 +2093,14 @@
         <v>8</v>
       </c>
       <c r="S21" s="5"/>
-      <c r="V21" s="30" t="s">
+      <c r="V21" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="W21" t="s">
         <v>104</v>
       </c>
-      <c r="W21" t="s">
-        <v>105</v>
-      </c>
       <c r="X21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Y21">
         <v>4</v>
@@ -2113,7 +2109,7 @@
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B22" s="5">
         <v>9</v>
@@ -2123,7 +2119,7 @@
         <v>17</v>
       </c>
       <c r="G22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H22">
         <f>13+2</f>
@@ -2144,10 +2140,10 @@
       </c>
       <c r="V22" s="4"/>
       <c r="W22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="X22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Y22">
         <v>22</v>
@@ -2156,7 +2152,7 @@
     </row>
     <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B23" s="5">
         <v>13</v>
@@ -2181,10 +2177,10 @@
       <c r="S23" s="7"/>
       <c r="V23" s="4"/>
       <c r="W23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="X23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Y23">
         <v>17</v>
@@ -2193,7 +2189,7 @@
     </row>
     <row r="24" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B24" s="7">
         <v>17</v>
@@ -2203,11 +2199,11 @@
       <c r="G24" s="16"/>
       <c r="H24" s="16"/>
       <c r="J24" s="7"/>
-      <c r="N24" s="31" t="s">
-        <v>56</v>
+      <c r="N24" s="29" t="s">
+        <v>55</v>
       </c>
       <c r="O24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P24" t="s">
         <v>7</v>
@@ -2229,11 +2225,11 @@
       </c>
     </row>
     <row r="25" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E25" s="32" t="s">
-        <v>42</v>
+      <c r="E25" s="30" t="s">
+        <v>41</v>
       </c>
       <c r="F25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G25" t="s">
         <v>7</v>
@@ -2244,10 +2240,10 @@
       <c r="I25" s="10"/>
       <c r="N25" s="4"/>
       <c r="O25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Q25">
         <f>6+2</f>
@@ -2263,14 +2259,14 @@
     </row>
     <row r="26" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E26" s="4"/>
       <c r="F26" t="s">
         <v>17</v>
       </c>
       <c r="G26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H26">
         <f>13+2</f>
@@ -2289,14 +2285,14 @@
         <f>PRODUCT(Q26,R26)</f>
         <v>99</v>
       </c>
-      <c r="V26" s="32" t="s">
-        <v>108</v>
+      <c r="V26" s="30" t="s">
+        <v>107</v>
       </c>
       <c r="W26" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="X26" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="Y26">
         <v>16</v>
@@ -2305,14 +2301,14 @@
       <c r="AA26" s="3"/>
     </row>
     <row r="27" spans="1:27" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="28" t="s">
-        <v>90</v>
-      </c>
-      <c r="B27" s="28"/>
-      <c r="C27" s="28"/>
+      <c r="A27" s="38" t="s">
+        <v>89</v>
+      </c>
+      <c r="B27" s="38"/>
+      <c r="C27" s="38"/>
       <c r="E27" s="4"/>
       <c r="F27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G27" t="s">
         <v>7</v>
@@ -2330,7 +2326,7 @@
       <c r="T27" s="1"/>
       <c r="V27" s="4"/>
       <c r="W27" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="X27" t="s">
         <v>12</v>
@@ -2342,7 +2338,7 @@
     </row>
     <row r="28" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E28" s="4"/>
       <c r="H28" s="1">
@@ -2356,14 +2352,14 @@
         <f>PRODUCT(H28,I28)</f>
         <v>17</v>
       </c>
-      <c r="N28" s="34" t="s">
-        <v>59</v>
+      <c r="N28" s="32" t="s">
+        <v>58</v>
       </c>
       <c r="O28" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P28" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q28">
         <v>4</v>
@@ -2371,10 +2367,10 @@
       <c r="S28" s="5"/>
       <c r="V28" s="4"/>
       <c r="W28" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="X28" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Y28">
         <v>4</v>
@@ -2395,7 +2391,7 @@
         <v>17</v>
       </c>
       <c r="P29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Q29">
         <f>21+2</f>
@@ -2403,7 +2399,7 @@
       </c>
       <c r="S29" s="5"/>
       <c r="V29" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="Y29" s="1">
         <f>SUM(Y26:Y28)</f>
@@ -2418,14 +2414,14 @@
       </c>
     </row>
     <row r="30" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="E30" s="33" t="s">
-        <v>39</v>
+      <c r="E30" s="31" t="s">
+        <v>38</v>
       </c>
       <c r="F30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G30" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H30">
         <v>2</v>
@@ -2457,7 +2453,7 @@
         <v>17</v>
       </c>
       <c r="G31" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H31">
         <f>8+2</f>
@@ -2471,49 +2467,49 @@
       <c r="R31" s="16"/>
       <c r="S31" s="18"/>
       <c r="T31" s="1"/>
-      <c r="V31" s="30" t="s">
+      <c r="V31" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="W31" t="s">
         <v>115</v>
       </c>
-      <c r="W31" t="s">
-        <v>116</v>
-      </c>
       <c r="X31" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Y31">
         <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A32" s="37" t="s">
-        <v>180</v>
-      </c>
-      <c r="B32" s="38" t="s">
-        <v>178</v>
-      </c>
-      <c r="C32" s="39" t="s">
-        <v>179</v>
+      <c r="A32" s="35" t="s">
+        <v>177</v>
+      </c>
+      <c r="B32" s="36" t="s">
+        <v>175</v>
+      </c>
+      <c r="C32" s="37" t="s">
+        <v>176</v>
       </c>
       <c r="E32" s="4"/>
       <c r="F32" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G32" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H32">
         <f>H13</f>
         <v>4</v>
       </c>
       <c r="J32" s="5"/>
-      <c r="N32" s="35" t="s">
-        <v>72</v>
+      <c r="N32" s="33" t="s">
+        <v>71</v>
       </c>
       <c r="O32" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P32" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q32">
         <v>4</v>
@@ -2522,10 +2518,10 @@
       <c r="T32" s="1"/>
       <c r="V32" s="4"/>
       <c r="W32" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="X32" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Y32">
         <v>4</v>
@@ -2533,10 +2529,10 @@
       <c r="AA32" s="5"/>
     </row>
     <row r="33" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A33" s="33" t="s">
-        <v>181</v>
-      </c>
-      <c r="B33" s="29">
+      <c r="A33" s="31" t="s">
+        <v>178</v>
+      </c>
+      <c r="B33">
         <f>SUM(J15,J19,J23,J28,J33,J37,S4,S12,S16,S26,S57,S66,AA63,J44,AA29)</f>
         <v>919988</v>
       </c>
@@ -2557,10 +2553,10 @@
       </c>
       <c r="N33" s="4"/>
       <c r="O33" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="P33" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q33">
         <v>4</v>
@@ -2568,10 +2564,10 @@
       <c r="S33" s="5"/>
       <c r="V33" s="4"/>
       <c r="W33" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="X33" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Y33">
         <v>4</v>
@@ -2579,12 +2575,12 @@
       <c r="AA33" s="5"/>
     </row>
     <row r="34" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A34" s="30" t="s">
-        <v>182</v>
-      </c>
-      <c r="B34" s="29">
-        <f>SUM(J7,J65,J70,S51,S47,S6,AA20,AA24,AA42,S72,AA6)</f>
-        <v>1874072</v>
+      <c r="A34" s="28" t="s">
+        <v>179</v>
+      </c>
+      <c r="B34">
+        <f>SUM(J7,J65,J70,S51,S47,S6,AA20,AA24,AA42,S72,AA6,AA59)</f>
+        <v>1877880</v>
       </c>
       <c r="C34" s="5">
         <v>1.88</v>
@@ -2597,10 +2593,10 @@
       <c r="J34" s="7"/>
       <c r="N34" s="4"/>
       <c r="O34" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="P34" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Q34">
         <f>22+2</f>
@@ -2609,10 +2605,10 @@
       <c r="S34" s="5"/>
       <c r="V34" s="4"/>
       <c r="W34" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="X34" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Y34">
         <v>4</v>
@@ -2620,24 +2616,24 @@
       <c r="AA34" s="5"/>
     </row>
     <row r="35" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A35" s="34" t="s">
-        <v>183</v>
-      </c>
-      <c r="B35" s="29">
-        <f>SUM(J11,J47,J53,S22,S30,S54,S60,AA59,AA53,AA15)</f>
-        <v>11663644</v>
+      <c r="A35" s="32" t="s">
+        <v>180</v>
+      </c>
+      <c r="B35">
+        <f>SUM(J11,J47,J53,S22,S30,S54,S60,AA53,AA15)</f>
+        <v>11659836</v>
       </c>
       <c r="C35" s="5">
-        <v>11.67</v>
-      </c>
-      <c r="E35" s="32" t="s">
+        <v>11.66</v>
+      </c>
+      <c r="E35" s="30" t="s">
+        <v>92</v>
+      </c>
+      <c r="F35" t="s">
         <v>93</v>
       </c>
-      <c r="F35" t="s">
-        <v>94</v>
-      </c>
       <c r="G35" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H35">
         <v>2</v>
@@ -2645,10 +2641,10 @@
       <c r="I35" s="10"/>
       <c r="N35" s="4"/>
       <c r="O35" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="P35" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q35">
         <v>4</v>
@@ -2656,7 +2652,7 @@
       <c r="S35" s="5"/>
       <c r="V35" s="13"/>
       <c r="W35" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="X35" t="s">
         <v>11</v>
@@ -2668,16 +2664,17 @@
     </row>
     <row r="36" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
-      <c r="B36" s="16">
-        <f>SUM(J70,J65,J53,J47,J44,J37,J33,J28,J23,J19,J15,J11,J7,S4,S6,S12,S16,S22,S26,S30,S47,S51,S54,S57,S60,S66,S72,AA59,AA53,AA42,AA24,AA20,AA15,AA6,AA29,AA63)</f>
+      <c r="B36">
+        <f>SUM(B33:B35)</f>
         <v>14457704</v>
       </c>
       <c r="C36" s="7">
-        <v>14.5</v>
+        <f>SUM(C33:C35)</f>
+        <v>14.46</v>
       </c>
       <c r="E36" s="4"/>
       <c r="F36" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G36" t="s">
         <v>7</v>
@@ -2688,20 +2685,20 @@
       <c r="J36" s="5"/>
       <c r="N36" s="13"/>
       <c r="O36" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="P36" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q36">
         <v>4</v>
       </c>
       <c r="S36" s="5"/>
       <c r="V36" s="21" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="W36" s="21" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="X36" s="21" t="s">
         <v>11</v>
@@ -2712,8 +2709,8 @@
       <c r="AA36" s="5"/>
     </row>
     <row r="37" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B37">
-        <f>SUM(B33:B35)</f>
+      <c r="B37" s="10">
+        <f>SUM(J70,J65,J53,J47,J44,J37,J33,J28,J23,J19,J15,J11,J7,S4,S6,S12,S16,S22,S26,S30,S47,S51,S54,S57,S60,S66,S72,AA59,AA53,AA42,AA24,AA20,AA15,AA6,AA29,AA63)</f>
         <v>14457704</v>
       </c>
       <c r="E37" s="4"/>
@@ -2730,10 +2727,10 @@
       </c>
       <c r="N37" s="4"/>
       <c r="O37" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="P37" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q37">
         <v>4</v>
@@ -2741,10 +2738,10 @@
       <c r="S37" s="5"/>
       <c r="V37" s="4"/>
       <c r="W37" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="X37" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Y37">
         <v>4</v>
@@ -2760,10 +2757,10 @@
       <c r="J38" s="7"/>
       <c r="N38" s="4"/>
       <c r="O38" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="P38" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="Q38">
         <v>8</v>
@@ -2771,10 +2768,10 @@
       <c r="S38" s="5"/>
       <c r="V38" s="4"/>
       <c r="W38" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="X38" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Y38">
         <v>3</v>
@@ -2782,11 +2779,11 @@
       <c r="AA38" s="5"/>
     </row>
     <row r="39" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="E39" s="33" t="s">
-        <v>47</v>
+      <c r="E39" s="31" t="s">
+        <v>46</v>
       </c>
       <c r="F39" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G39" t="s">
         <v>5</v>
@@ -2797,20 +2794,20 @@
       <c r="I39" s="10"/>
       <c r="N39" s="4"/>
       <c r="O39" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="P39" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="Q39">
         <v>8</v>
       </c>
       <c r="S39" s="5"/>
       <c r="V39" s="21" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="W39" s="21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="X39" s="21" t="s">
         <v>10</v>
@@ -2823,7 +2820,7 @@
     <row r="40" spans="1:27" x14ac:dyDescent="0.25">
       <c r="E40" s="4"/>
       <c r="F40" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G40" t="s">
         <v>5</v>
@@ -2834,23 +2831,23 @@
       <c r="J40" s="5"/>
       <c r="N40" s="4"/>
       <c r="O40" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="P40" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="Q40">
         <v>5</v>
       </c>
       <c r="S40" s="5"/>
       <c r="V40" s="21" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="W40" s="21" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="X40" s="21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Y40" s="21">
         <v>0</v>
@@ -2860,7 +2857,7 @@
     <row r="41" spans="1:27" x14ac:dyDescent="0.25">
       <c r="E41" s="4"/>
       <c r="F41" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G41" t="s">
         <v>5</v>
@@ -2871,23 +2868,23 @@
       <c r="J41" s="5"/>
       <c r="N41" s="4"/>
       <c r="O41" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="P41" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="Q41">
         <v>5</v>
       </c>
       <c r="S41" s="5"/>
       <c r="V41" s="21" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="W41" s="21" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="X41" s="21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="Y41" s="21">
         <v>0</v>
@@ -2897,10 +2894,10 @@
     <row r="42" spans="1:27" x14ac:dyDescent="0.25">
       <c r="E42" s="4"/>
       <c r="F42" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G42" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H42">
         <v>2</v>
@@ -2908,7 +2905,7 @@
       <c r="J42" s="5"/>
       <c r="N42" s="4"/>
       <c r="O42" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="P42" t="s">
         <v>10</v>
@@ -2933,7 +2930,7 @@
     <row r="43" spans="1:27" x14ac:dyDescent="0.25">
       <c r="E43" s="4"/>
       <c r="F43" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G43" t="s">
         <v>7</v>
@@ -2944,7 +2941,7 @@
       <c r="J43" s="5"/>
       <c r="N43" s="4"/>
       <c r="O43" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="P43" t="s">
         <v>7</v>
@@ -2976,23 +2973,23 @@
       </c>
       <c r="N44" s="4"/>
       <c r="O44" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="P44" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q44">
         <v>4</v>
       </c>
       <c r="S44" s="5"/>
-      <c r="V44" s="36" t="s">
+      <c r="V44" s="34" t="s">
+        <v>124</v>
+      </c>
+      <c r="W44" t="s">
         <v>125</v>
       </c>
-      <c r="W44" t="s">
-        <v>126</v>
-      </c>
       <c r="X44" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Y44">
         <v>4</v>
@@ -3007,7 +3004,7 @@
       <c r="J45" s="7"/>
       <c r="N45" s="4"/>
       <c r="O45" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="P45" t="s">
         <v>6</v>
@@ -3018,10 +3015,10 @@
       <c r="S45" s="5"/>
       <c r="V45" s="4"/>
       <c r="W45" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="X45" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Y45">
         <v>4</v>
@@ -3029,11 +3026,11 @@
       <c r="AA45" s="5"/>
     </row>
     <row r="46" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="E46" s="34" t="s">
-        <v>52</v>
+      <c r="E46" s="32" t="s">
+        <v>51</v>
       </c>
       <c r="F46" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G46" t="s">
         <v>5</v>
@@ -3043,7 +3040,7 @@
       </c>
       <c r="N46" s="4"/>
       <c r="O46" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="P46" t="s">
         <v>6</v>
@@ -3054,7 +3051,7 @@
       <c r="S46" s="5"/>
       <c r="V46" s="4"/>
       <c r="W46" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="X46" t="s">
         <v>6</v>
@@ -3091,10 +3088,10 @@
       </c>
       <c r="V47" s="4"/>
       <c r="W47" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="X47" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="Y47">
         <v>8</v>
@@ -3110,7 +3107,7 @@
       <c r="J48" s="7"/>
       <c r="N48" s="6"/>
       <c r="O48" s="16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="P48" s="16"/>
       <c r="Q48" s="16"/>
@@ -3118,10 +3115,10 @@
       <c r="S48" s="7"/>
       <c r="V48" s="4"/>
       <c r="W48" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="X48" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="Y48">
         <v>8</v>
@@ -3129,27 +3126,27 @@
       <c r="AA48" s="5"/>
     </row>
     <row r="49" spans="5:27" x14ac:dyDescent="0.25">
-      <c r="E49" s="36" t="s">
-        <v>96</v>
+      <c r="E49" s="34" t="s">
+        <v>95</v>
       </c>
       <c r="F49" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G49" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H49">
         <v>4</v>
       </c>
       <c r="I49" s="10"/>
-      <c r="N49" s="35" t="s">
-        <v>75</v>
+      <c r="N49" s="33" t="s">
+        <v>74</v>
       </c>
       <c r="O49" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P49" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q49" s="10">
         <v>4</v>
@@ -3159,10 +3156,10 @@
       <c r="T49" s="1"/>
       <c r="V49" s="4"/>
       <c r="W49" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="X49" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="Y49">
         <v>5</v>
@@ -3172,10 +3169,10 @@
     <row r="50" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E50" s="4"/>
       <c r="F50" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G50" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H50">
         <v>2</v>
@@ -3183,10 +3180,10 @@
       <c r="J50" s="5"/>
       <c r="N50" s="4"/>
       <c r="O50" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="P50" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="Q50">
         <f>25+2</f>
@@ -3195,10 +3192,10 @@
       <c r="S50" s="5"/>
       <c r="V50" s="4"/>
       <c r="W50" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="X50" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="Y50">
         <v>8</v>
@@ -3208,10 +3205,10 @@
     <row r="51" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E51" s="4"/>
       <c r="F51" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G51" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H51">
         <v>4</v>
@@ -3233,10 +3230,10 @@
       </c>
       <c r="V51" s="4"/>
       <c r="W51" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="X51" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Y51">
         <v>4</v>
@@ -3246,23 +3243,23 @@
     <row r="52" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E52" s="4"/>
       <c r="F52" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G52" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H52">
         <v>4</v>
       </c>
       <c r="J52" s="5"/>
-      <c r="N52" s="36" t="s">
-        <v>74</v>
+      <c r="N52" s="34" t="s">
+        <v>73</v>
       </c>
       <c r="O52" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P52" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q52" s="10">
         <v>4</v>
@@ -3271,10 +3268,10 @@
       <c r="S52" s="11"/>
       <c r="V52" s="4"/>
       <c r="W52" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X52" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="Y52">
         <v>8</v>
@@ -3299,7 +3296,7 @@
         <v>17</v>
       </c>
       <c r="P53" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="Q53">
         <v>6</v>
@@ -3347,11 +3344,11 @@
       <c r="AA54" s="7"/>
     </row>
     <row r="55" spans="5:27" x14ac:dyDescent="0.25">
-      <c r="N55" s="32" t="s">
-        <v>167</v>
+      <c r="N55" s="30" t="s">
+        <v>164</v>
       </c>
       <c r="O55" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P55" s="10" t="s">
         <v>6</v>
@@ -3361,14 +3358,14 @@
       </c>
       <c r="R55" s="10"/>
       <c r="S55" s="11"/>
-      <c r="V55" s="34" t="s">
-        <v>134</v>
+      <c r="V55" s="28" t="s">
+        <v>133</v>
       </c>
       <c r="W55" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="X55" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Y55">
         <v>4</v>
@@ -3380,7 +3377,7 @@
         <v>17</v>
       </c>
       <c r="P56" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="Q56">
         <v>25</v>
@@ -3388,7 +3385,7 @@
       <c r="S56" s="5"/>
       <c r="V56" s="4"/>
       <c r="W56" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="X56" t="s">
         <v>11</v>
@@ -3399,9 +3396,6 @@
       <c r="AA56" s="5"/>
     </row>
     <row r="57" spans="5:27" x14ac:dyDescent="0.25">
-      <c r="E57" t="s">
-        <v>157</v>
-      </c>
       <c r="N57" s="6"/>
       <c r="O57" s="16"/>
       <c r="P57" s="16"/>
@@ -3418,7 +3412,7 @@
       </c>
       <c r="V57" s="4"/>
       <c r="W57" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="X57" t="s">
         <v>11</v>
@@ -3429,25 +3423,25 @@
       <c r="AA57" s="5"/>
     </row>
     <row r="58" spans="5:27" x14ac:dyDescent="0.25">
-      <c r="E58" s="35" t="s">
-        <v>158</v>
+      <c r="E58" s="33" t="s">
+        <v>181</v>
       </c>
       <c r="F58" s="10" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="G58" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H58" s="10">
         <v>8</v>
       </c>
       <c r="I58" s="10"/>
       <c r="J58" s="11"/>
-      <c r="N58" s="36" t="s">
+      <c r="N58" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="O58" t="s">
         <v>112</v>
-      </c>
-      <c r="O58" t="s">
-        <v>113</v>
       </c>
       <c r="P58" t="s">
         <v>7</v>
@@ -3457,10 +3451,10 @@
       </c>
       <c r="V58" s="4"/>
       <c r="W58" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="X58" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Y58">
         <v>4</v>
@@ -3470,10 +3464,10 @@
     <row r="59" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E59" s="4"/>
       <c r="F59" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="G59" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="H59">
         <v>8</v>
@@ -3481,10 +3475,10 @@
       <c r="J59" s="5"/>
       <c r="N59" s="4"/>
       <c r="O59" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="P59" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q59">
         <v>4</v>
@@ -3506,7 +3500,7 @@
     <row r="60" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E60" s="4"/>
       <c r="F60" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="H60">
         <v>8</v>
@@ -3534,7 +3528,7 @@
     <row r="61" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E61" s="4"/>
       <c r="F61" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G61" t="s">
         <v>8</v>
@@ -3549,8 +3543,8 @@
       <c r="Q61" s="16"/>
       <c r="R61" s="16"/>
       <c r="S61" s="7"/>
-      <c r="V61" s="32" t="s">
-        <v>79</v>
+      <c r="V61" s="30" t="s">
+        <v>78</v>
       </c>
       <c r="W61" s="10"/>
       <c r="X61" s="10"/>
@@ -3561,7 +3555,7 @@
     <row r="62" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E62" s="4"/>
       <c r="F62" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G62" t="s">
         <v>10</v>
@@ -3577,22 +3571,21 @@
       <c r="R62" s="10"/>
       <c r="S62" s="10"/>
       <c r="V62" s="4"/>
-      <c r="W62" s="29" t="s">
-        <v>177</v>
-      </c>
-      <c r="X62" s="29" t="s">
-        <v>67</v>
-      </c>
-      <c r="Y62" s="29">
+      <c r="W62" t="s">
+        <v>174</v>
+      </c>
+      <c r="X62" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y62">
         <v>5</v>
       </c>
-      <c r="Z62" s="29"/>
       <c r="AA62" s="5"/>
     </row>
     <row r="63" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E63" s="4"/>
       <c r="F63" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G63" t="s">
         <v>10</v>
@@ -3620,7 +3613,7 @@
     </row>
     <row r="64" spans="5:27" x14ac:dyDescent="0.25">
       <c r="F64" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G64" t="s">
         <v>12</v>
@@ -3628,14 +3621,14 @@
       <c r="H64">
         <v>8</v>
       </c>
-      <c r="N64" s="32" t="s">
+      <c r="N64" s="30" t="s">
+        <v>136</v>
+      </c>
+      <c r="O64" t="s">
         <v>137</v>
       </c>
-      <c r="O64" t="s">
-        <v>138</v>
-      </c>
       <c r="P64" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q64">
         <v>4</v>
@@ -3660,10 +3653,10 @@
       </c>
       <c r="N65" s="4"/>
       <c r="O65" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="P65" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Q65" s="19">
         <v>15</v>
@@ -3671,14 +3664,14 @@
       <c r="S65" s="5"/>
     </row>
     <row r="66" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E66" s="35" t="s">
-        <v>159</v>
+      <c r="E66" s="33" t="s">
+        <v>156</v>
       </c>
       <c r="F66" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="G66" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H66">
         <v>8</v>
@@ -3701,7 +3694,7 @@
     <row r="67" spans="5:19" x14ac:dyDescent="0.25">
       <c r="E67" s="4"/>
       <c r="F67" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G67" t="s">
         <v>8</v>
@@ -3720,7 +3713,7 @@
     <row r="68" spans="5:19" x14ac:dyDescent="0.25">
       <c r="E68" s="4"/>
       <c r="F68" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G68" t="s">
         <v>8</v>
@@ -3729,14 +3722,14 @@
         <v>8</v>
       </c>
       <c r="J68" s="5"/>
-      <c r="N68" s="35" t="s">
+      <c r="N68" s="33" t="s">
+        <v>139</v>
+      </c>
+      <c r="O68" t="s">
         <v>140</v>
       </c>
-      <c r="O68" t="s">
-        <v>141</v>
-      </c>
       <c r="P68" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q68">
         <v>4</v>
@@ -3747,7 +3740,7 @@
     <row r="69" spans="5:19" x14ac:dyDescent="0.25">
       <c r="E69" s="4"/>
       <c r="F69" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G69" t="s">
         <v>12</v>
@@ -3758,10 +3751,10 @@
       <c r="J69" s="5"/>
       <c r="N69" s="4"/>
       <c r="O69" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="P69" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q69">
         <v>4</v>
@@ -3785,10 +3778,10 @@
       </c>
       <c r="N70" s="4"/>
       <c r="O70" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="P70" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Q70" s="19"/>
       <c r="S70" s="5"/>
@@ -3796,7 +3789,7 @@
     <row r="71" spans="5:19" x14ac:dyDescent="0.25">
       <c r="N71" s="4"/>
       <c r="O71" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="P71" t="s">
         <v>12</v>

</xml_diff>